<commit_message>
updated related files for kabu STATION ver 5.12.5
</commit_message>
<xml_diff>
--- a/sample/ExcelMacro/kabuSTATION_API_function_sample.xlsx
+++ b/sample/ExcelMacro/kabuSTATION_API_function_sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\fsv1\Develop\Vendor\JOL\プロジェクト\202012_kabuS12月リリース\70.リリース\GitHubリリース\function_sample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lu\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,11 +18,12 @@
     <sheet name="注文約定照会" sheetId="5" r:id="rId4"/>
     <sheet name="銘柄情報" sheetId="4" r:id="rId5"/>
     <sheet name="残高照会" sheetId="6" r:id="rId6"/>
-    <sheet name="銘柄登録" sheetId="7" r:id="rId7"/>
-    <sheet name="銘柄登録解除" sheetId="8" r:id="rId8"/>
-    <sheet name="銘柄登録全解除" sheetId="9" r:id="rId9"/>
-    <sheet name="先物銘柄コード取得" sheetId="10" r:id="rId10"/>
-    <sheet name="オプション銘柄コード取得" sheetId="11" r:id="rId11"/>
+    <sheet name="詳細ランキング" sheetId="12" r:id="rId7"/>
+    <sheet name="銘柄登録" sheetId="7" r:id="rId8"/>
+    <sheet name="銘柄登録解除" sheetId="8" r:id="rId9"/>
+    <sheet name="銘柄登録全解除" sheetId="9" r:id="rId10"/>
+    <sheet name="先物銘柄コード取得" sheetId="10" r:id="rId11"/>
+    <sheet name="オプション銘柄コード取得" sheetId="11" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">注文約定照会!$B$5:$J$8</definedName>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1502" uniqueCount="390">
   <si>
     <t>概要</t>
     <rPh sb="0" eb="2">
@@ -1638,6 +1639,602 @@
   </si>
   <si>
     <t>※いずれのパラメータの指定が必要です。</t>
+  </si>
+  <si>
+    <t>種別</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>市場</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>種別</t>
+    <rPh sb="0" eb="2">
+      <t>シュベツ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>市場</t>
+    <rPh sb="0" eb="2">
+      <t>シジョウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>順位</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>トレンド</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>平均順位</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>銘柄コード</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">銘柄名称    </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>現在値</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>前日比</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>騰落率（%）</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>時刻</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>売買高</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>売買代金</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>市場名</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>業種名</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>xxx</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>レスポンスボディ（種別：TICK回数）</t>
+    <rPh sb="9" eb="11">
+      <t>シュベツ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>カイスウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>市場</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>順位</t>
+  </si>
+  <si>
+    <t>TICK回数</t>
+  </si>
+  <si>
+    <t>UP</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>DOWN</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>騰落率（%）</t>
+  </si>
+  <si>
+    <t>業種名</t>
+  </si>
+  <si>
+    <t>レスポンスボディ（種別：売買高急増）</t>
+    <rPh sb="9" eb="11">
+      <t>シュベツ</t>
+    </rPh>
+    <rPh sb="12" eb="15">
+      <t>バイバイダカ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>キュウゾウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>売買高急増（％）</t>
+  </si>
+  <si>
+    <t>レスポンスボディ（種別：売買代金急増）</t>
+    <rPh sb="9" eb="11">
+      <t>シュベツ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>バイバイ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ダイキン</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>キュウゾウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>代金急増（％）</t>
+  </si>
+  <si>
+    <t>レスポンスボディ（種別：信用売残増、信用売残減、信用買残増、信用買残減、信用高倍率、信用低倍率）</t>
+    <rPh sb="9" eb="11">
+      <t>シュベツ</t>
+    </rPh>
+    <rPh sb="12" eb="15">
+      <t>シンヨウウ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>ザン</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>ゾウ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>シンヨウ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>ウ</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>ザン</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>ゲン</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>シンヨウ</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>ザン</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>ゾウ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>シンヨウ</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>ザン</t>
+    </rPh>
+    <rPh sb="34" eb="35">
+      <t>ゲン</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>シンヨウ</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>コウ</t>
+    </rPh>
+    <rPh sb="39" eb="41">
+      <t>バイリツ</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>シンヨウ</t>
+    </rPh>
+    <rPh sb="44" eb="45">
+      <t>テイ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>バイリツ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>売残（千株）</t>
+  </si>
+  <si>
+    <t>売残前週比</t>
+  </si>
+  <si>
+    <t>買残（千株）</t>
+  </si>
+  <si>
+    <t>買残前週比</t>
+  </si>
+  <si>
+    <t>倍率</t>
+  </si>
+  <si>
+    <t>レスポンスボディ（種別：業種別値上がり率、業種別値下がり率）</t>
+    <rPh sb="9" eb="11">
+      <t>シュベツ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ギョウシュ</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>ベツ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ネア</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>リツ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>ネサ</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>リツ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>業種コード</t>
+  </si>
+  <si>
+    <t>時刻</t>
+  </si>
+  <si>
+    <t>定義値</t>
+    <rPh sb="0" eb="3">
+      <t>テイギチ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>値上がり率（デフォルト）</t>
+    <rPh sb="0" eb="2">
+      <t>ネア</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>リツ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>値下がり率</t>
+    <rPh sb="0" eb="2">
+      <t>ネサ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>リツ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>売買高上位</t>
+    <rPh sb="0" eb="3">
+      <t>バイバイダカ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ジョウイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>売買代金</t>
+    <rPh sb="0" eb="2">
+      <t>バイバイ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ダイキン</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>TICK回数</t>
+    <rPh sb="4" eb="6">
+      <t>カイスウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>売買高急増</t>
+    <rPh sb="0" eb="3">
+      <t>バイバイダカ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>キュウゾウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>売買代金急増</t>
+    <rPh sb="0" eb="2">
+      <t>バイバイ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ダイキン</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>キュウゾウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>信用売残増</t>
+    <rPh sb="0" eb="2">
+      <t>シンヨウ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>バイ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ザン</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ゾウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>信用売残減</t>
+    <rPh sb="0" eb="2">
+      <t>シンヨウ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>バイ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ザン</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ゲン</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>信用買残増</t>
+    <rPh sb="0" eb="2">
+      <t>シンヨウ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ザン</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ゾウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>信用買残減</t>
+    <rPh sb="0" eb="2">
+      <t>シンヨウ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ザン</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ゲン</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>信用高倍率</t>
+    <rPh sb="0" eb="2">
+      <t>シンヨウ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>コウ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>バイリツ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>信用低倍率</t>
+    <rPh sb="0" eb="2">
+      <t>シンヨウ</t>
+    </rPh>
+    <rPh sb="2" eb="5">
+      <t>テイバイリツ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>業種別値上がり率</t>
+    <rPh sb="0" eb="2">
+      <t>ギョウシュ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ベツ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ネア</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>リツ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>業種別値下がり率</t>
+    <rPh sb="0" eb="2">
+      <t>ギョウシュ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ベツ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ネサ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>リツ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>全市場（デフォルト）</t>
+    <rPh sb="0" eb="3">
+      <t>ゼンシジョウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>T</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>東証全体</t>
+    <rPh sb="0" eb="2">
+      <t>トウショウ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ゼンタイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>T1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>東証一部</t>
+    <rPh sb="0" eb="2">
+      <t>トウショウ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>イチブ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>T2</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>東証二部</t>
+    <rPh sb="0" eb="2">
+      <t>トウショウ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ニブ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>TM</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>マザーズ</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>JQ</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>JASDAQ</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>名証</t>
+    <rPh sb="0" eb="2">
+      <t>メイショウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>FK</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>S</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>札証</t>
+    <rPh sb="0" eb="2">
+      <t>サッショウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>詳細ランキングを取得する</t>
+  </si>
+  <si>
+    <t>RANKING</t>
+  </si>
+  <si>
+    <t>=RANKING(C9,D9)</t>
+  </si>
+  <si>
+    <t>レスポンスボディ（種別：値上がり率、値下がり率、売買高上位、売買代金）</t>
+    <rPh sb="9" eb="11">
+      <t>シュベツ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ネア</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>リツ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ネサ</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>リツ</t>
+    </rPh>
+    <rPh sb="24" eb="27">
+      <t>バイバイダカ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>ジョウイ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>バイバイ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>ダイキン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>関数入力する際、「"」ダブルクォーテーションで囲む必要があります。</t>
   </si>
 </sst>
 </file>
@@ -1647,7 +2244,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1726,6 +2323,27 @@
       <sz val="11"/>
       <color rgb="FF263238"/>
       <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Meiryo UI"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Meiryo UI"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Meiryo UI"/>
       <family val="3"/>
       <charset val="128"/>
     </font>
@@ -2009,7 +2627,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -2156,16 +2774,37 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2174,17 +2813,23 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2198,38 +2843,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2680,6 +3341,158 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet13"/>
+  <dimension ref="A2:I20"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="B9" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="B10" s="5"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="B11" s="5"/>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="C12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="24"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="6"/>
+      <c r="C13" t="str">
+        <f>"(D"&amp;ROW()&amp;"に関数入力)"</f>
+        <v>(D13に関数入力)</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0</v>
+      </c>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="24"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="6"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="24"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="6"/>
+      <c r="B15" t="s">
+        <v>211</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="24"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="B16" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" t="s">
+        <v>188</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F27"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -2889,7 +3702,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G19"/>
   <sheetViews>
@@ -5359,7 +6172,9 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A2:AK319"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -5508,80 +6323,80 @@
       <c r="C11" s="72" t="s">
         <v>306</v>
       </c>
-      <c r="D11" s="86" t="s">
+      <c r="D11" s="81" t="s">
         <v>300</v>
       </c>
-      <c r="E11" s="87"/>
-      <c r="F11" s="86" t="s">
+      <c r="E11" s="82"/>
+      <c r="F11" s="81" t="s">
         <v>301</v>
       </c>
-      <c r="G11" s="87"/>
+      <c r="G11" s="82"/>
     </row>
     <row r="12" spans="2:12">
-      <c r="B12" s="102" t="s">
+      <c r="B12" s="80" t="s">
         <v>280</v>
       </c>
       <c r="C12" s="48">
         <v>0</v>
       </c>
-      <c r="D12" s="98" t="s">
+      <c r="D12" s="83" t="s">
         <v>204</v>
       </c>
-      <c r="E12" s="99"/>
-      <c r="F12" s="88" t="s">
+      <c r="E12" s="84"/>
+      <c r="F12" s="97" t="s">
         <v>302</v>
       </c>
-      <c r="G12" s="89"/>
+      <c r="G12" s="98"/>
     </row>
     <row r="13" spans="2:12">
-      <c r="B13" s="102"/>
+      <c r="B13" s="80"/>
       <c r="C13" s="48">
         <v>1</v>
       </c>
-      <c r="D13" s="98" t="s">
+      <c r="D13" s="83" t="s">
         <v>203</v>
       </c>
-      <c r="E13" s="99"/>
-      <c r="F13" s="90" t="s">
+      <c r="E13" s="84"/>
+      <c r="F13" s="99" t="s">
         <v>309</v>
       </c>
-      <c r="G13" s="91"/>
+      <c r="G13" s="100"/>
     </row>
     <row r="14" spans="2:12">
-      <c r="B14" s="102"/>
+      <c r="B14" s="80"/>
       <c r="C14" s="48">
         <v>2</v>
       </c>
-      <c r="D14" s="98" t="s">
+      <c r="D14" s="83" t="s">
         <v>202</v>
       </c>
-      <c r="E14" s="99"/>
-      <c r="F14" s="90"/>
-      <c r="G14" s="91"/>
+      <c r="E14" s="84"/>
+      <c r="F14" s="99"/>
+      <c r="G14" s="100"/>
     </row>
     <row r="15" spans="2:12">
-      <c r="B15" s="102"/>
+      <c r="B15" s="80"/>
       <c r="C15" s="49">
         <v>3</v>
       </c>
-      <c r="D15" s="98" t="s">
+      <c r="D15" s="83" t="s">
         <v>267</v>
       </c>
-      <c r="E15" s="99"/>
-      <c r="F15" s="90"/>
-      <c r="G15" s="91"/>
+      <c r="E15" s="84"/>
+      <c r="F15" s="99"/>
+      <c r="G15" s="100"/>
     </row>
     <row r="16" spans="2:12">
-      <c r="B16" s="102"/>
+      <c r="B16" s="80"/>
       <c r="C16" s="49">
         <v>4</v>
       </c>
-      <c r="D16" s="98" t="s">
+      <c r="D16" s="83" t="s">
         <v>268</v>
       </c>
-      <c r="E16" s="99"/>
-      <c r="F16" s="92"/>
-      <c r="G16" s="93"/>
+      <c r="E16" s="84"/>
+      <c r="F16" s="93"/>
+      <c r="G16" s="94"/>
     </row>
     <row r="17" spans="2:7">
       <c r="B17" s="65" t="s">
@@ -5636,30 +6451,30 @@
       <c r="G20" s="69"/>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="100" t="s">
+      <c r="B21" s="78" t="s">
         <v>289</v>
       </c>
       <c r="C21" s="48" t="b">
         <v>1</v>
       </c>
-      <c r="D21" s="98" t="s">
+      <c r="D21" s="83" t="s">
         <v>307</v>
       </c>
-      <c r="E21" s="99"/>
+      <c r="E21" s="84"/>
       <c r="F21" s="73" t="s">
         <v>302</v>
       </c>
       <c r="G21" s="74"/>
     </row>
     <row r="22" spans="2:7">
-      <c r="B22" s="100"/>
+      <c r="B22" s="78"/>
       <c r="C22" s="48" t="b">
         <v>0</v>
       </c>
-      <c r="D22" s="98" t="s">
+      <c r="D22" s="83" t="s">
         <v>308</v>
       </c>
-      <c r="E22" s="99"/>
+      <c r="E22" s="84"/>
       <c r="F22" s="75" t="s">
         <v>310</v>
       </c>
@@ -5682,130 +6497,130 @@
       <c r="G23" s="71"/>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="100" t="s">
+      <c r="B24" s="78" t="s">
         <v>292</v>
       </c>
       <c r="C24" s="47">
         <v>1</v>
       </c>
-      <c r="D24" s="96" t="s">
+      <c r="D24" s="85" t="s">
         <v>290</v>
       </c>
-      <c r="E24" s="97"/>
-      <c r="F24" s="94" t="s">
+      <c r="E24" s="86"/>
+      <c r="F24" s="91" t="s">
         <v>302</v>
       </c>
-      <c r="G24" s="95"/>
+      <c r="G24" s="92"/>
     </row>
     <row r="25" spans="2:7">
-      <c r="B25" s="100"/>
+      <c r="B25" s="78"/>
       <c r="C25" s="47">
         <v>2</v>
       </c>
-      <c r="D25" s="84" t="s">
+      <c r="D25" s="87" t="s">
         <v>281</v>
       </c>
-      <c r="E25" s="85"/>
-      <c r="F25" s="78" t="s">
+      <c r="E25" s="88"/>
+      <c r="F25" s="95" t="s">
         <v>309</v>
       </c>
-      <c r="G25" s="79"/>
+      <c r="G25" s="96"/>
     </row>
     <row r="26" spans="2:7">
-      <c r="B26" s="100"/>
+      <c r="B26" s="78"/>
       <c r="C26" s="47">
         <v>3</v>
       </c>
-      <c r="D26" s="84" t="s">
+      <c r="D26" s="87" t="s">
         <v>282</v>
       </c>
-      <c r="E26" s="85"/>
-      <c r="F26" s="78"/>
-      <c r="G26" s="79"/>
+      <c r="E26" s="88"/>
+      <c r="F26" s="95"/>
+      <c r="G26" s="96"/>
     </row>
     <row r="27" spans="2:7">
-      <c r="B27" s="100"/>
+      <c r="B27" s="78"/>
       <c r="C27" s="47">
         <v>4</v>
       </c>
-      <c r="D27" s="84" t="s">
+      <c r="D27" s="87" t="s">
         <v>283</v>
       </c>
-      <c r="E27" s="85"/>
-      <c r="F27" s="78"/>
-      <c r="G27" s="79"/>
+      <c r="E27" s="88"/>
+      <c r="F27" s="95"/>
+      <c r="G27" s="96"/>
     </row>
     <row r="28" spans="2:7">
-      <c r="B28" s="100"/>
+      <c r="B28" s="78"/>
       <c r="C28" s="47">
         <v>5</v>
       </c>
-      <c r="D28" s="84" t="s">
+      <c r="D28" s="87" t="s">
         <v>284</v>
       </c>
-      <c r="E28" s="85"/>
-      <c r="F28" s="82"/>
-      <c r="G28" s="83"/>
+      <c r="E28" s="88"/>
+      <c r="F28" s="89"/>
+      <c r="G28" s="90"/>
     </row>
     <row r="29" spans="2:7">
-      <c r="B29" s="100" t="s">
+      <c r="B29" s="78" t="s">
         <v>293</v>
       </c>
       <c r="C29" s="47">
         <v>1</v>
       </c>
-      <c r="D29" s="96" t="s">
+      <c r="D29" s="85" t="s">
         <v>291</v>
       </c>
-      <c r="E29" s="97"/>
-      <c r="F29" s="94" t="s">
+      <c r="E29" s="86"/>
+      <c r="F29" s="91" t="s">
         <v>302</v>
       </c>
-      <c r="G29" s="95"/>
+      <c r="G29" s="92"/>
     </row>
     <row r="30" spans="2:7">
-      <c r="B30" s="100"/>
+      <c r="B30" s="78"/>
       <c r="C30" s="47">
         <v>2</v>
       </c>
-      <c r="D30" s="84" t="s">
+      <c r="D30" s="87" t="s">
         <v>285</v>
       </c>
-      <c r="E30" s="85"/>
-      <c r="F30" s="78" t="s">
+      <c r="E30" s="88"/>
+      <c r="F30" s="95" t="s">
         <v>309</v>
       </c>
-      <c r="G30" s="79"/>
+      <c r="G30" s="96"/>
     </row>
     <row r="31" spans="2:7">
-      <c r="B31" s="101" t="s">
+      <c r="B31" s="79" t="s">
         <v>294</v>
       </c>
       <c r="C31" s="47">
         <v>2</v>
       </c>
-      <c r="D31" s="84" t="s">
+      <c r="D31" s="87" t="s">
         <v>286</v>
       </c>
-      <c r="E31" s="85"/>
-      <c r="F31" s="80" t="s">
+      <c r="E31" s="88"/>
+      <c r="F31" s="101" t="s">
         <v>302</v>
       </c>
-      <c r="G31" s="81"/>
+      <c r="G31" s="102"/>
     </row>
     <row r="32" spans="2:7">
-      <c r="B32" s="101"/>
+      <c r="B32" s="79"/>
       <c r="C32" s="47">
         <v>3</v>
       </c>
-      <c r="D32" s="84" t="s">
+      <c r="D32" s="87" t="s">
         <v>287</v>
       </c>
-      <c r="E32" s="85"/>
-      <c r="F32" s="82" t="s">
+      <c r="E32" s="88"/>
+      <c r="F32" s="89" t="s">
         <v>309</v>
       </c>
-      <c r="G32" s="83"/>
+      <c r="G32" s="90"/>
     </row>
     <row r="33" spans="1:36">
       <c r="B33" s="6"/>
@@ -16405,43 +17220,43 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B24:B28"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F27:G27"/>
     <mergeCell ref="F28:G28"/>
     <mergeCell ref="F29:G29"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="B21:B22"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="5">
@@ -17326,6 +18141,1512 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:T64"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="7.85546875" style="107" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="107" customWidth="1"/>
+    <col min="3" max="3" width="17" style="107" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="107" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="107" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" style="107" customWidth="1"/>
+    <col min="7" max="7" width="12" style="107" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" style="107" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" style="107" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" style="107" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" style="107" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" style="107" customWidth="1"/>
+    <col min="13" max="13" width="20.5703125" style="107" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" style="107" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" style="107" customWidth="1"/>
+    <col min="16" max="16" width="13.85546875" style="107" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" style="107" customWidth="1"/>
+    <col min="18" max="18" width="12.5703125" style="107" bestFit="1" customWidth="1"/>
+    <col min="19" max="24" width="10.42578125" style="107" customWidth="1"/>
+    <col min="25" max="16384" width="9" style="107"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:13">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="104" t="s">
+        <v>385</v>
+      </c>
+      <c r="D2" s="105"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="106"/>
+    </row>
+    <row r="3" spans="2:13">
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="104" t="s">
+        <v>386</v>
+      </c>
+      <c r="D3" s="105"/>
+      <c r="E3" s="105"/>
+      <c r="F3" s="106"/>
+    </row>
+    <row r="5" spans="2:13">
+      <c r="B5" s="108" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13">
+      <c r="B6" s="109"/>
+      <c r="C6" s="109" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13">
+      <c r="B7" s="109"/>
+      <c r="C7" s="42" t="s">
+        <v>313</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13">
+      <c r="B8" s="109"/>
+      <c r="C8" s="123">
+        <v>1</v>
+      </c>
+      <c r="D8" s="123" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13">
+      <c r="C10" s="72" t="s">
+        <v>353</v>
+      </c>
+      <c r="D10" s="124" t="s">
+        <v>269</v>
+      </c>
+      <c r="E10" s="125"/>
+      <c r="H10" s="72" t="s">
+        <v>353</v>
+      </c>
+      <c r="I10" s="124" t="s">
+        <v>269</v>
+      </c>
+      <c r="J10" s="125"/>
+      <c r="K10" s="127" t="s">
+        <v>301</v>
+      </c>
+      <c r="L10" s="127"/>
+      <c r="M10" s="127"/>
+    </row>
+    <row r="11" spans="2:13" ht="15.75">
+      <c r="B11" s="115" t="s">
+        <v>316</v>
+      </c>
+      <c r="C11" s="116">
+        <v>1</v>
+      </c>
+      <c r="D11" s="117" t="s">
+        <v>354</v>
+      </c>
+      <c r="E11" s="106"/>
+      <c r="G11" s="121" t="s">
+        <v>317</v>
+      </c>
+      <c r="H11" s="122" t="s">
+        <v>315</v>
+      </c>
+      <c r="I11" s="117" t="s">
+        <v>369</v>
+      </c>
+      <c r="J11" s="106"/>
+      <c r="K11" s="117"/>
+      <c r="L11" s="105"/>
+      <c r="M11" s="106"/>
+    </row>
+    <row r="12" spans="2:13" ht="15.75">
+      <c r="B12" s="118"/>
+      <c r="C12" s="116">
+        <v>2</v>
+      </c>
+      <c r="D12" s="117" t="s">
+        <v>355</v>
+      </c>
+      <c r="E12" s="106"/>
+      <c r="G12" s="119"/>
+      <c r="H12" s="122" t="s">
+        <v>370</v>
+      </c>
+      <c r="I12" s="117" t="s">
+        <v>371</v>
+      </c>
+      <c r="J12" s="106"/>
+      <c r="K12" s="117"/>
+      <c r="L12" s="105"/>
+      <c r="M12" s="106"/>
+    </row>
+    <row r="13" spans="2:13" ht="15.75">
+      <c r="B13" s="118"/>
+      <c r="C13" s="116">
+        <v>3</v>
+      </c>
+      <c r="D13" s="117" t="s">
+        <v>356</v>
+      </c>
+      <c r="E13" s="106"/>
+      <c r="G13" s="119"/>
+      <c r="H13" s="122" t="s">
+        <v>372</v>
+      </c>
+      <c r="I13" s="117" t="s">
+        <v>373</v>
+      </c>
+      <c r="J13" s="106"/>
+      <c r="K13" s="126" t="s">
+        <v>389</v>
+      </c>
+      <c r="L13" s="105"/>
+      <c r="M13" s="106"/>
+    </row>
+    <row r="14" spans="2:13" ht="15.75">
+      <c r="B14" s="118"/>
+      <c r="C14" s="116">
+        <v>4</v>
+      </c>
+      <c r="D14" s="117" t="s">
+        <v>357</v>
+      </c>
+      <c r="E14" s="106"/>
+      <c r="G14" s="119"/>
+      <c r="H14" s="122" t="s">
+        <v>374</v>
+      </c>
+      <c r="I14" s="117" t="s">
+        <v>375</v>
+      </c>
+      <c r="J14" s="106"/>
+      <c r="K14" s="126" t="s">
+        <v>389</v>
+      </c>
+      <c r="L14" s="105"/>
+      <c r="M14" s="106"/>
+    </row>
+    <row r="15" spans="2:13" ht="15.75">
+      <c r="B15" s="118"/>
+      <c r="C15" s="116">
+        <v>5</v>
+      </c>
+      <c r="D15" s="117" t="s">
+        <v>358</v>
+      </c>
+      <c r="E15" s="106"/>
+      <c r="G15" s="119"/>
+      <c r="H15" s="122" t="s">
+        <v>376</v>
+      </c>
+      <c r="I15" s="117" t="s">
+        <v>377</v>
+      </c>
+      <c r="J15" s="106"/>
+      <c r="K15" s="117"/>
+      <c r="L15" s="105"/>
+      <c r="M15" s="106"/>
+    </row>
+    <row r="16" spans="2:13" ht="15.75">
+      <c r="B16" s="118"/>
+      <c r="C16" s="116">
+        <v>6</v>
+      </c>
+      <c r="D16" s="117" t="s">
+        <v>359</v>
+      </c>
+      <c r="E16" s="106"/>
+      <c r="G16" s="119"/>
+      <c r="H16" s="122" t="s">
+        <v>378</v>
+      </c>
+      <c r="I16" s="117" t="s">
+        <v>379</v>
+      </c>
+      <c r="J16" s="106"/>
+      <c r="K16" s="117"/>
+      <c r="L16" s="105"/>
+      <c r="M16" s="106"/>
+    </row>
+    <row r="17" spans="2:18" ht="15.75">
+      <c r="B17" s="118"/>
+      <c r="C17" s="116">
+        <v>7</v>
+      </c>
+      <c r="D17" s="117" t="s">
+        <v>360</v>
+      </c>
+      <c r="E17" s="106"/>
+      <c r="G17" s="119"/>
+      <c r="H17" s="122" t="s">
+        <v>380</v>
+      </c>
+      <c r="I17" s="117" t="s">
+        <v>381</v>
+      </c>
+      <c r="J17" s="106"/>
+      <c r="K17" s="117"/>
+      <c r="L17" s="105"/>
+      <c r="M17" s="106"/>
+    </row>
+    <row r="18" spans="2:18" ht="15.75">
+      <c r="B18" s="118"/>
+      <c r="C18" s="116">
+        <v>8</v>
+      </c>
+      <c r="D18" s="117" t="s">
+        <v>361</v>
+      </c>
+      <c r="E18" s="106"/>
+      <c r="G18" s="119"/>
+      <c r="H18" s="122" t="s">
+        <v>382</v>
+      </c>
+      <c r="I18" s="117" t="s">
+        <v>197</v>
+      </c>
+      <c r="J18" s="106"/>
+      <c r="K18" s="117"/>
+      <c r="L18" s="105"/>
+      <c r="M18" s="106"/>
+    </row>
+    <row r="19" spans="2:18" ht="15.75">
+      <c r="B19" s="119"/>
+      <c r="C19" s="116">
+        <v>9</v>
+      </c>
+      <c r="D19" s="117" t="s">
+        <v>362</v>
+      </c>
+      <c r="E19" s="106"/>
+      <c r="G19" s="120"/>
+      <c r="H19" s="122" t="s">
+        <v>383</v>
+      </c>
+      <c r="I19" s="117" t="s">
+        <v>384</v>
+      </c>
+      <c r="J19" s="106"/>
+      <c r="K19" s="117"/>
+      <c r="L19" s="105"/>
+      <c r="M19" s="106"/>
+    </row>
+    <row r="20" spans="2:18" ht="15.75">
+      <c r="B20" s="119"/>
+      <c r="C20" s="116">
+        <v>10</v>
+      </c>
+      <c r="D20" s="117" t="s">
+        <v>363</v>
+      </c>
+      <c r="E20" s="106"/>
+    </row>
+    <row r="21" spans="2:18" ht="15.75">
+      <c r="B21" s="119"/>
+      <c r="C21" s="116">
+        <v>11</v>
+      </c>
+      <c r="D21" s="117" t="s">
+        <v>364</v>
+      </c>
+      <c r="E21" s="106"/>
+    </row>
+    <row r="22" spans="2:18" ht="15.75">
+      <c r="B22" s="119"/>
+      <c r="C22" s="116">
+        <v>12</v>
+      </c>
+      <c r="D22" s="117" t="s">
+        <v>365</v>
+      </c>
+      <c r="E22" s="106"/>
+    </row>
+    <row r="23" spans="2:18" ht="15.75">
+      <c r="B23" s="119"/>
+      <c r="C23" s="116">
+        <v>13</v>
+      </c>
+      <c r="D23" s="117" t="s">
+        <v>366</v>
+      </c>
+      <c r="E23" s="106"/>
+    </row>
+    <row r="24" spans="2:18" ht="15.75">
+      <c r="B24" s="119"/>
+      <c r="C24" s="116">
+        <v>14</v>
+      </c>
+      <c r="D24" s="117" t="s">
+        <v>367</v>
+      </c>
+      <c r="E24" s="106"/>
+    </row>
+    <row r="25" spans="2:18" ht="15.75">
+      <c r="B25" s="120"/>
+      <c r="C25" s="116">
+        <v>15</v>
+      </c>
+      <c r="D25" s="117" t="s">
+        <v>368</v>
+      </c>
+      <c r="E25" s="106"/>
+    </row>
+    <row r="28" spans="2:18">
+      <c r="B28" s="108" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18">
+      <c r="D29" s="108"/>
+    </row>
+    <row r="30" spans="2:18" ht="15.75">
+      <c r="C30" s="107" t="s">
+        <v>199</v>
+      </c>
+      <c r="D30" s="114" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18">
+      <c r="C31" s="109" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="J31" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="K31" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="L31" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="M31" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="N31" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="O31" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="P31" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="Q31" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="R31" s="8" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" ht="15.75">
+      <c r="C32" s="110" t="str">
+        <f>"(D"&amp;ROW()&amp;"に関数入力)"</f>
+        <v>(D32に関数入力)</v>
+      </c>
+      <c r="D32" s="111" t="s">
+        <v>296</v>
+      </c>
+      <c r="E32" s="112" t="s">
+        <v>331</v>
+      </c>
+      <c r="F32" s="103">
+        <v>1</v>
+      </c>
+      <c r="G32" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="H32" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="I32" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="J32" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="K32" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="L32" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="M32" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="N32" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="O32" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="P32" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="Q32" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="R32" s="103" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="3:20">
+      <c r="F33" s="103">
+        <v>2</v>
+      </c>
+      <c r="G33" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="H33" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="I33" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="J33" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="K33" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="L33" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="M33" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="N33" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="O33" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="P33" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="Q33" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="R33" s="103" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="3:20">
+      <c r="F34" s="103">
+        <v>3</v>
+      </c>
+      <c r="G34" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="H34" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="I34" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="J34" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="K34" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="L34" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="M34" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="N34" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="O34" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="P34" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="Q34" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="R34" s="103" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="3:20" ht="15.75">
+      <c r="J35" s="50"/>
+      <c r="K35" s="113"/>
+    </row>
+    <row r="36" spans="3:20" ht="15.75">
+      <c r="C36" s="107" t="s">
+        <v>199</v>
+      </c>
+      <c r="D36" s="114" t="s">
+        <v>332</v>
+      </c>
+      <c r="F36" s="50"/>
+      <c r="G36" s="113"/>
+    </row>
+    <row r="37" spans="3:20">
+      <c r="C37" s="109" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="J37" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="K37" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="L37" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="M37" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="N37" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="O37" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="P37" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="Q37" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="R37" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="S37" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="T37" s="8" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="38" spans="3:20" ht="15.75">
+      <c r="C38" s="110" t="str">
+        <f>"(D"&amp;ROW()&amp;"に関数入力)"</f>
+        <v>(D38に関数入力)</v>
+      </c>
+      <c r="D38" s="111" t="s">
+        <v>296</v>
+      </c>
+      <c r="E38" s="112" t="s">
+        <v>331</v>
+      </c>
+      <c r="F38" s="103">
+        <v>1</v>
+      </c>
+      <c r="G38" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="H38" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="I38" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="J38" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="K38" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="L38" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="M38" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="N38" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="O38" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="P38" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="Q38" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="R38" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="S38" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="T38" s="103" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="3:20">
+      <c r="F39" s="103">
+        <v>2</v>
+      </c>
+      <c r="G39" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="H39" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="I39" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="J39" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="K39" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="L39" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="M39" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="N39" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="O39" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="P39" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="Q39" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="R39" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="S39" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="T39" s="103" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="3:20">
+      <c r="F40" s="103">
+        <v>3</v>
+      </c>
+      <c r="G40" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="H40" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="I40" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="J40" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="K40" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="L40" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="M40" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="N40" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="O40" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="P40" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="Q40" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="R40" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="S40" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="T40" s="103" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="3:20">
+      <c r="F41" s="50"/>
+      <c r="G41" s="50"/>
+      <c r="H41" s="50"/>
+      <c r="I41" s="50"/>
+      <c r="J41" s="50"/>
+      <c r="K41" s="50"/>
+      <c r="L41" s="50"/>
+      <c r="M41" s="50"/>
+      <c r="N41" s="50"/>
+      <c r="O41" s="50"/>
+      <c r="P41" s="50"/>
+      <c r="Q41" s="50"/>
+      <c r="R41" s="50"/>
+    </row>
+    <row r="42" spans="3:20" ht="15.75">
+      <c r="C42" s="107" t="s">
+        <v>199</v>
+      </c>
+      <c r="D42" s="114" t="s">
+        <v>340</v>
+      </c>
+      <c r="F42" s="50"/>
+      <c r="G42" s="113"/>
+    </row>
+    <row r="43" spans="3:20">
+      <c r="C43" s="109" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="H43" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="I43" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="J43" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="K43" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="L43" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="M43" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="N43" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="O43" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="P43" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="Q43" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="R43" s="8" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="44" spans="3:20" ht="15.75">
+      <c r="C44" s="110" t="str">
+        <f>"(D"&amp;ROW()&amp;"に関数入力)"</f>
+        <v>(D44に関数入力)</v>
+      </c>
+      <c r="D44" s="111" t="s">
+        <v>296</v>
+      </c>
+      <c r="E44" s="112" t="s">
+        <v>331</v>
+      </c>
+      <c r="F44" s="103">
+        <v>1</v>
+      </c>
+      <c r="G44" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="H44" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="I44" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="J44" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="K44" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="L44" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="M44" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="N44" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="O44" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="P44" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="Q44" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="R44" s="103" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="3:20">
+      <c r="F45" s="103">
+        <v>2</v>
+      </c>
+      <c r="G45" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="H45" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="I45" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="J45" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="K45" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="L45" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="M45" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="N45" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="O45" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="P45" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="Q45" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="R45" s="103" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="3:20">
+      <c r="F46" s="103">
+        <v>3</v>
+      </c>
+      <c r="G46" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="H46" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="I46" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="J46" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="K46" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="L46" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="M46" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="N46" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="O46" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="P46" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="Q46" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="R46" s="103" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="3:20" ht="15.75">
+      <c r="C48" s="107" t="s">
+        <v>199</v>
+      </c>
+      <c r="D48" s="114" t="s">
+        <v>342</v>
+      </c>
+      <c r="E48" s="50"/>
+      <c r="F48" s="50"/>
+      <c r="G48" s="113"/>
+    </row>
+    <row r="49" spans="3:18">
+      <c r="C49" s="109" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="H49" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="I49" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="J49" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="K49" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="L49" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="M49" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="N49" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="O49" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="P49" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="Q49" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="R49" s="8" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="50" spans="3:18" ht="15.75">
+      <c r="C50" s="110" t="str">
+        <f>"(D"&amp;ROW()&amp;"に関数入力)"</f>
+        <v>(D50に関数入力)</v>
+      </c>
+      <c r="D50" s="111" t="s">
+        <v>296</v>
+      </c>
+      <c r="E50" s="112" t="s">
+        <v>331</v>
+      </c>
+      <c r="F50" s="103">
+        <v>1</v>
+      </c>
+      <c r="G50" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="H50" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="I50" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="J50" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="K50" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="L50" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="M50" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="N50" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="O50" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="P50" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="Q50" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="R50" s="103" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="3:18">
+      <c r="F51" s="103">
+        <v>2</v>
+      </c>
+      <c r="G51" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="H51" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="I51" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="J51" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="K51" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="L51" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="M51" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="N51" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="O51" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="P51" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="Q51" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="R51" s="103" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="3:18">
+      <c r="F52" s="103">
+        <v>3</v>
+      </c>
+      <c r="G52" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="H52" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="I52" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="J52" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="K52" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="L52" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="M52" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="N52" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="O52" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="P52" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="Q52" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="R52" s="103" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="3:18">
+      <c r="E53" s="50"/>
+    </row>
+    <row r="54" spans="3:18" ht="15.75">
+      <c r="C54" s="107" t="s">
+        <v>199</v>
+      </c>
+      <c r="D54" s="114" t="s">
+        <v>344</v>
+      </c>
+      <c r="E54" s="113"/>
+      <c r="F54" s="50"/>
+      <c r="G54" s="113"/>
+    </row>
+    <row r="55" spans="3:18">
+      <c r="C55" s="109" t="s">
+        <v>12</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="G55" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="H55" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="I55" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="J55" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="K55" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="L55" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="M55" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="N55" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="O55" s="8" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="56" spans="3:18" ht="15.75">
+      <c r="C56" s="110" t="str">
+        <f>"(D"&amp;ROW()&amp;"に関数入力)"</f>
+        <v>(D56に関数入力)</v>
+      </c>
+      <c r="D56" s="111" t="s">
+        <v>296</v>
+      </c>
+      <c r="E56" s="112" t="s">
+        <v>331</v>
+      </c>
+      <c r="F56" s="103">
+        <v>1</v>
+      </c>
+      <c r="G56" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="H56" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="I56" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="J56" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="K56" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="L56" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="M56" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="N56" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="O56" s="103" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="57" spans="3:18">
+      <c r="F57" s="103">
+        <v>2</v>
+      </c>
+      <c r="G57" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="H57" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="I57" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="J57" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="K57" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="L57" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="M57" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="N57" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="O57" s="103" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="58" spans="3:18">
+      <c r="F58" s="103">
+        <v>3</v>
+      </c>
+      <c r="G58" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="H58" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="I58" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="J58" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="K58" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="L58" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="M58" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="N58" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="O58" s="103" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="60" spans="3:18" ht="15.75">
+      <c r="C60" s="107" t="s">
+        <v>199</v>
+      </c>
+      <c r="D60" s="114" t="s">
+        <v>350</v>
+      </c>
+      <c r="E60" s="113"/>
+      <c r="F60" s="50"/>
+      <c r="G60" s="50"/>
+    </row>
+    <row r="61" spans="3:18">
+      <c r="C61" s="109" t="s">
+        <v>12</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="F61" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="G61" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="H61" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="I61" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="J61" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="K61" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="L61" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="M61" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="N61" s="8" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="62" spans="3:18" ht="15.75">
+      <c r="C62" s="110" t="str">
+        <f>"(D"&amp;ROW()&amp;"に関数入力)"</f>
+        <v>(D62に関数入力)</v>
+      </c>
+      <c r="D62" s="111" t="s">
+        <v>296</v>
+      </c>
+      <c r="E62" s="112" t="s">
+        <v>331</v>
+      </c>
+      <c r="F62" s="103">
+        <v>1</v>
+      </c>
+      <c r="G62" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="H62" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="I62" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="J62" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="K62" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="L62" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="M62" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="N62" s="103" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="63" spans="3:18">
+      <c r="F63" s="103">
+        <v>2</v>
+      </c>
+      <c r="G63" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="H63" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="I63" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="J63" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="K63" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="L63" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="M63" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="N63" s="103" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="64" spans="3:18">
+      <c r="F64" s="103">
+        <v>3</v>
+      </c>
+      <c r="G64" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="H64" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="I64" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="J64" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="K64" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="L64" s="103" t="s">
+        <v>296</v>
+      </c>
+      <c r="M64" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="N64" s="103" t="s">
+        <v>296</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K10:M10"/>
+  </mergeCells>
+  <dataValidations disablePrompts="1" count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8">
+      <formula1>$C$11:$C$25</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8">
+      <formula1>$H$11:$H$19</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A2:I40"/>
   <sheetViews>
@@ -17706,7 +20027,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A2:I37"/>
@@ -18039,156 +20360,4 @@
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet13"/>
-  <dimension ref="A2:I20"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
-    <col min="5" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:9">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="B5" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="B6" s="6"/>
-      <c r="C6" s="6" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="B7" s="6"/>
-      <c r="C7" s="6" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="B9" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="B10" s="5"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="B11" s="5"/>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="C12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="24"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="6"/>
-      <c r="C13" t="str">
-        <f>"(D"&amp;ROW()&amp;"に関数入力)"</f>
-        <v>(D13に関数入力)</v>
-      </c>
-      <c r="D13" s="7">
-        <v>0</v>
-      </c>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="24"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="6"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="24"/>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="6"/>
-      <c r="B15" t="s">
-        <v>211</v>
-      </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="24"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="B16" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2">
-      <c r="B18" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2">
-      <c r="B19" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2">
-      <c r="B20" t="s">
-        <v>188</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
uploaded preview for ver5.16.2
</commit_message>
<xml_diff>
--- a/sample/ExcelMacro/kabuSTATION_API_function_sample.xlsx
+++ b/sample/ExcelMacro/kabuSTATION_API_function_sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\fsv1\システム戦略部\900_Work\lu\kabu STATION\2021_デイトレ信用\70.リリース\GitHubリリース\function_sample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OLDPC\kabuSTATION\workspace\resourse\sample\ExcelMacro\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,9 +25,10 @@
     <sheet name="規制情報" sheetId="16" r:id="rId11"/>
     <sheet name="優先市場" sheetId="17" r:id="rId12"/>
     <sheet name="ソフトリミット" sheetId="18" r:id="rId13"/>
-    <sheet name="銘柄登録" sheetId="7" r:id="rId14"/>
-    <sheet name="銘柄登録解除" sheetId="8" r:id="rId15"/>
-    <sheet name="銘柄登録全解除" sheetId="9" r:id="rId16"/>
+    <sheet name="プレミアム料取得" sheetId="19" r:id="rId14"/>
+    <sheet name="銘柄登録" sheetId="7" r:id="rId15"/>
+    <sheet name="銘柄登録解除" sheetId="8" r:id="rId16"/>
+    <sheet name="銘柄登録全解除" sheetId="9" r:id="rId17"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">注文約定照会!$B$5:$J$8</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1779" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1832" uniqueCount="553">
   <si>
     <t>概要</t>
     <rPh sb="0" eb="2">
@@ -2372,12 +2373,6 @@
     <t>制限終了日（※②）</t>
   </si>
   <si>
-    <t>制限開始日（※②）</t>
-  </si>
-  <si>
-    <t>理由（※①）</t>
-  </si>
-  <si>
     <t>規制売買</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -2842,6 +2837,204 @@
   </si>
   <si>
     <t>xxxx</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>MARGINPREMIUM</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>=MARGINPREMIUM(C8)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>プレミアム料入力区分</t>
+  </si>
+  <si>
+    <t>定義値</t>
+  </si>
+  <si>
+    <t>説明</t>
+  </si>
+  <si>
+    <t>理由（※①）</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>確定プレミアム料（※①）</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>制限開始日（※②）</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>上限プレミアム料（※②）</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>下限プレミアム料（※②）</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>指定した銘柄のプレミアム料を取得するAPI</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>xxxx</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>=MARGINPREMIUM()</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>一般信用（長期）</t>
+    <rPh sb="0" eb="4">
+      <t>イッパンシンヨウ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>チョウキ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>一般信用（デイトレ）</t>
+    <rPh sb="0" eb="4">
+      <t>イッパンシンヨウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>※入札銘柄の場合、入札受付中は随時更新します。受付時間外は、確定したプレミアム料を返します。</t>
+    <rPh sb="1" eb="3">
+      <t>ニュウサツ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>メイガラ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="9" eb="14">
+      <t>ニュウサツウケツケチュウ</t>
+    </rPh>
+    <rPh sb="15" eb="19">
+      <t>ズイジコウシン</t>
+    </rPh>
+    <rPh sb="23" eb="28">
+      <t>ウケツケジカンガイ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>カクテイ</t>
+    </rPh>
+    <rPh sb="39" eb="40">
+      <t>リョウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>※非入札銘柄の場合、常に固定値を返します。</t>
+    <rPh sb="1" eb="6">
+      <t>ヒニュウサツメイガラ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>ツネ</t>
+    </rPh>
+    <rPh sb="12" eb="15">
+      <t>コテイチ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>※信用取引不可の場合、nullを返します。</t>
+    <rPh sb="1" eb="5">
+      <t>シンヨウトリヒキ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>フカ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>バアイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>※19:30~翌営業日のプレミアム料になります。</t>
+    <rPh sb="7" eb="11">
+      <t>ヨクエイギョウビ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>リョウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>※①</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>プレミアム料刻値（※③）</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>※プレミアム料がない場合は、nullを返します。</t>
+    <rPh sb="6" eb="7">
+      <t>リョウ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>バアイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>※③</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>※入札可能銘柄以外は、nullを返します。</t>
+    <rPh sb="1" eb="3">
+      <t>ニュウサツ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>カノウ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>メイガラ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>イガイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>※②</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>null</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>一般信用（長期/デイトレ）非対応銘柄</t>
+    <rPh sb="5" eb="7">
+      <t>チョウキ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>プレミアム料がない銘柄</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>プレミアム料が固定の銘柄</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>プレミアム料が入札で決定する銘柄</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -2852,7 +3045,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2974,8 +3167,32 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2997,6 +3214,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFAFAFA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3293,7 +3522,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="197">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -3512,31 +3741,90 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3545,29 +3833,11 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3581,11 +3851,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3595,6 +3892,21 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4180,7 +4492,7 @@
         <v>14</v>
       </c>
       <c r="I14" s="26" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.4">
@@ -4364,7 +4676,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -4375,7 +4687,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="104" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="D3" s="105"/>
       <c r="E3" s="105"/>
@@ -4389,7 +4701,7 @@
     <row r="6" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B6" s="6"/>
       <c r="C6" s="6" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="F6" s="29"/>
     </row>
@@ -4399,7 +4711,7 @@
         <v>320</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="E7" s="27"/>
     </row>
@@ -4416,159 +4728,159 @@
     <row r="10" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C10" s="124"/>
       <c r="D10" s="127" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="E10" s="127" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="G10" s="124"/>
       <c r="H10" s="127" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="I10" s="127" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C11" s="123" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D11" s="116" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="E11" s="118" t="s">
+        <v>472</v>
+      </c>
+      <c r="G11" s="123" t="s">
+        <v>477</v>
+      </c>
+      <c r="H11" s="116" t="s">
         <v>474</v>
       </c>
-      <c r="G11" s="123" t="s">
-        <v>479</v>
-      </c>
-      <c r="H11" s="116" t="s">
+      <c r="I11" s="118" t="s">
         <v>476</v>
-      </c>
-      <c r="I11" s="118" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C12" s="120"/>
       <c r="D12" s="116" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="E12" s="118" t="s">
+        <v>466</v>
+      </c>
+      <c r="G12" s="120" t="s">
+        <v>470</v>
+      </c>
+      <c r="H12" s="116" t="s">
         <v>468</v>
       </c>
-      <c r="G12" s="120" t="s">
-        <v>472</v>
-      </c>
-      <c r="H12" s="116" t="s">
-        <v>470</v>
-      </c>
       <c r="I12" s="118" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C13" s="120"/>
       <c r="D13" s="116" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E13" s="118" t="s">
+        <v>459</v>
+      </c>
+      <c r="G13" s="117" t="s">
+        <v>463</v>
+      </c>
+      <c r="H13" s="116" t="s">
         <v>461</v>
       </c>
-      <c r="G13" s="117" t="s">
-        <v>465</v>
-      </c>
-      <c r="H13" s="116" t="s">
-        <v>463</v>
-      </c>
       <c r="I13" s="118" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C14" s="121"/>
       <c r="D14" s="116" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="E14" s="115" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="17" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C17" s="124"/>
       <c r="D17" s="127" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="E17" s="127" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="G17" s="124"/>
       <c r="H17" s="127" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="I17" s="127" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C18" s="123" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D18" s="116" t="s">
+        <v>474</v>
+      </c>
+      <c r="E18" s="118" t="s">
         <v>476</v>
       </c>
-      <c r="E18" s="118" t="s">
-        <v>478</v>
-      </c>
       <c r="G18" s="123" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="H18" s="116" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="I18" s="118" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C19" s="120"/>
       <c r="D19" s="116" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="E19" s="118" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="G19" s="120"/>
       <c r="H19" s="116" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="I19" s="118" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="20" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C20" s="120"/>
       <c r="D20" s="116" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="E20" s="118" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="G20" s="117"/>
       <c r="H20" s="116" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="I20" s="118" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C21" s="120"/>
       <c r="D21" s="116" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E21" s="118" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="L21" s="113"/>
       <c r="M21" s="114"/>
@@ -4577,10 +4889,10 @@
     <row r="22" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C22" s="120"/>
       <c r="D22" s="116" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="E22" s="115" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="L22" s="113"/>
       <c r="M22" s="114"/>
@@ -4589,10 +4901,10 @@
     <row r="23" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C23" s="120"/>
       <c r="D23" s="116" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E23" s="118" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="L23" s="113"/>
       <c r="M23" s="114"/>
@@ -4601,10 +4913,10 @@
     <row r="24" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C24" s="120"/>
       <c r="D24" s="116" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="E24" s="118" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="L24" s="113"/>
       <c r="M24" s="114"/>
@@ -4613,10 +4925,10 @@
     <row r="25" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C25" s="117"/>
       <c r="D25" s="116" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="E25" s="118" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="L25" s="113"/>
       <c r="M25" s="114"/>
@@ -4635,10 +4947,10 @@
     <row r="28" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C28" s="124"/>
       <c r="D28" s="127" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="E28" s="127" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="L28" s="113"/>
       <c r="M28" s="114"/>
@@ -4646,13 +4958,13 @@
     </row>
     <row r="29" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C29" s="123" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="D29" s="116" t="s">
+        <v>474</v>
+      </c>
+      <c r="E29" s="118" t="s">
         <v>476</v>
-      </c>
-      <c r="E29" s="118" t="s">
-        <v>478</v>
       </c>
       <c r="L29" s="113"/>
       <c r="M29" s="114"/>
@@ -4660,13 +4972,13 @@
     </row>
     <row r="30" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C30" s="122" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D30" s="116" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="E30" s="118" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="L30" s="113"/>
       <c r="M30" s="114"/>
@@ -4674,13 +4986,13 @@
     </row>
     <row r="31" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C31" s="120" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D31" s="116" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="E31" s="118" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="L31" s="113"/>
       <c r="M31" s="114"/>
@@ -4689,10 +5001,10 @@
     <row r="32" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C32" s="120"/>
       <c r="D32" s="116" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="E32" s="118" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="L32" s="113"/>
       <c r="M32" s="114"/>
@@ -4701,10 +5013,10 @@
     <row r="33" spans="2:14" x14ac:dyDescent="0.4">
       <c r="C33" s="120"/>
       <c r="D33" s="116" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E33" s="118" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="L33" s="113"/>
       <c r="M33" s="114"/>
@@ -4713,10 +5025,10 @@
     <row r="34" spans="2:14" x14ac:dyDescent="0.4">
       <c r="C34" s="120"/>
       <c r="D34" s="116" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E34" s="115" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="L34" s="113"/>
       <c r="M34" s="114"/>
@@ -4725,10 +5037,10 @@
     <row r="35" spans="2:14" x14ac:dyDescent="0.4">
       <c r="C35" s="120"/>
       <c r="D35" s="116" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="E35" s="118" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="L35" s="113"/>
       <c r="M35" s="114"/>
@@ -4737,10 +5049,10 @@
     <row r="36" spans="2:14" x14ac:dyDescent="0.4">
       <c r="C36" s="120"/>
       <c r="D36" s="116" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E36" s="118" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="L36" s="113"/>
       <c r="M36" s="114"/>
@@ -4749,10 +5061,10 @@
     <row r="37" spans="2:14" x14ac:dyDescent="0.4">
       <c r="C37" s="119"/>
       <c r="D37" s="116" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E37" s="118" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="L37" s="113"/>
       <c r="M37" s="114"/>
@@ -4761,10 +5073,10 @@
     <row r="38" spans="2:14" x14ac:dyDescent="0.4">
       <c r="C38" s="117"/>
       <c r="D38" s="116" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E38" s="115" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="L38" s="113"/>
       <c r="M38" s="114"/>
@@ -4794,7 +5106,7 @@
         <v>10</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.4">
@@ -4805,19 +5117,19 @@
         <v>320</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>433</v>
+        <v>528</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>432</v>
+        <v>530</v>
       </c>
       <c r="J45" s="8" t="s">
         <v>431</v>
@@ -4965,17 +5277,17 @@
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B56" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B57" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B58" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
   </sheetData>
@@ -5021,7 +5333,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="D2" s="4"/>
     </row>
@@ -5030,7 +5342,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="104" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="D3" s="106"/>
     </row>
@@ -5042,7 +5354,7 @@
     <row r="6" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B6" s="6"/>
       <c r="C6" s="6" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="F6" s="29"/>
     </row>
@@ -5076,7 +5388,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.4">
@@ -5087,7 +5399,7 @@
         <v>320</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.4">
@@ -5120,7 +5432,7 @@
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.4">
       <c r="D19" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.4">
@@ -5136,10 +5448,10 @@
     <row r="21" spans="2:11" x14ac:dyDescent="0.4">
       <c r="C21" s="124"/>
       <c r="D21" s="127" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="E21" s="127" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="F21" s="46"/>
       <c r="G21" s="46"/>
@@ -5150,40 +5462,40 @@
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.4">
       <c r="C22" s="123" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D22" s="116" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="E22" s="118" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.4">
       <c r="C23" s="120"/>
       <c r="D23" s="116" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="E23" s="118" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.4">
       <c r="C24" s="120"/>
       <c r="D24" s="116" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E24" s="118" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.4">
       <c r="C25" s="121"/>
       <c r="D25" s="116" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="E25" s="115" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.4">
@@ -5238,7 +5550,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
@@ -5248,7 +5560,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="104" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D3" s="105"/>
       <c r="E3" s="106"/>
@@ -5261,7 +5573,7 @@
     <row r="6" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B6" s="6"/>
       <c r="C6" s="6" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="F6" s="29"/>
     </row>
@@ -5284,7 +5596,7 @@
         <v>10</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.4">
@@ -5292,22 +5604,22 @@
         <v>12</v>
       </c>
       <c r="D11" s="103" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="E11" s="103" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="F11" s="103" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="G11" s="103" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H11" s="103" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.4">
@@ -5410,6 +5722,354 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:P40"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="2" width="9" style="136"/>
+    <col min="3" max="3" width="19.125" style="136" customWidth="1"/>
+    <col min="4" max="4" width="18" style="136" customWidth="1"/>
+    <col min="5" max="14" width="21" style="136" customWidth="1"/>
+    <col min="15" max="16" width="22.25" style="136" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9" style="136"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B2" s="132" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="132" t="s">
+        <v>533</v>
+      </c>
+      <c r="D2" s="133"/>
+      <c r="E2" s="133"/>
+      <c r="F2" s="134"/>
+      <c r="G2" s="135"/>
+      <c r="H2" s="135"/>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B3" s="137" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="132" t="s">
+        <v>523</v>
+      </c>
+      <c r="D3" s="133"/>
+      <c r="E3" s="133"/>
+      <c r="F3" s="134"/>
+      <c r="G3" s="135"/>
+      <c r="H3" s="135"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="C6" s="138" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="C7" s="139" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="C8" s="140" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="141"/>
+      <c r="D10" s="141"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="C12" s="142" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="143" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="C13" s="135"/>
+      <c r="D13" s="144"/>
+      <c r="E13" s="145"/>
+      <c r="F13" s="146"/>
+      <c r="G13" s="147" t="s">
+        <v>536</v>
+      </c>
+      <c r="H13" s="146"/>
+      <c r="I13" s="148"/>
+      <c r="J13" s="146"/>
+      <c r="K13" s="146"/>
+      <c r="L13" s="146"/>
+      <c r="M13" s="147" t="s">
+        <v>537</v>
+      </c>
+      <c r="N13" s="148"/>
+      <c r="O13" s="160"/>
+      <c r="P13" s="160"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="C14" s="149" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="150" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="159" t="s">
+        <v>525</v>
+      </c>
+      <c r="F14" s="159" t="s">
+        <v>529</v>
+      </c>
+      <c r="G14" s="159" t="s">
+        <v>531</v>
+      </c>
+      <c r="H14" s="159" t="s">
+        <v>532</v>
+      </c>
+      <c r="I14" s="159" t="s">
+        <v>543</v>
+      </c>
+      <c r="J14" s="159" t="s">
+        <v>525</v>
+      </c>
+      <c r="K14" s="159" t="s">
+        <v>529</v>
+      </c>
+      <c r="L14" s="159" t="s">
+        <v>531</v>
+      </c>
+      <c r="M14" s="159" t="s">
+        <v>532</v>
+      </c>
+      <c r="N14" s="159" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="C15" s="135" t="str">
+        <f>"(D"&amp;ROW()&amp;"に関数入力)"</f>
+        <v>(D15に関数入力)</v>
+      </c>
+      <c r="D15" s="151" t="s">
+        <v>534</v>
+      </c>
+      <c r="E15" s="151" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="151" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="151" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="151" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="151" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" s="151" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" s="151" t="s">
+        <v>14</v>
+      </c>
+      <c r="L15" s="151" t="s">
+        <v>14</v>
+      </c>
+      <c r="M15" s="151" t="s">
+        <v>14</v>
+      </c>
+      <c r="N15" s="151" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="D16" s="151"/>
+      <c r="E16" s="151"/>
+      <c r="F16" s="151"/>
+      <c r="G16" s="151"/>
+      <c r="H16" s="151"/>
+      <c r="I16" s="151"/>
+      <c r="J16" s="151"/>
+      <c r="K16" s="151"/>
+      <c r="L16" s="151"/>
+      <c r="M16" s="151"/>
+      <c r="N16" s="151"/>
+    </row>
+    <row r="17" spans="3:14" x14ac:dyDescent="0.4">
+      <c r="D17" s="151"/>
+      <c r="E17" s="151"/>
+      <c r="F17" s="151"/>
+      <c r="G17" s="151"/>
+      <c r="H17" s="151"/>
+      <c r="I17" s="151"/>
+      <c r="J17" s="151"/>
+      <c r="K17" s="151"/>
+      <c r="L17" s="151"/>
+      <c r="M17" s="151"/>
+      <c r="N17" s="151"/>
+    </row>
+    <row r="18" spans="3:14" x14ac:dyDescent="0.4">
+      <c r="D18" s="151"/>
+      <c r="E18" s="151"/>
+      <c r="F18" s="151"/>
+      <c r="G18" s="151"/>
+      <c r="H18" s="151"/>
+      <c r="I18" s="151"/>
+      <c r="J18" s="151"/>
+      <c r="K18" s="151"/>
+      <c r="L18" s="151"/>
+      <c r="M18" s="151"/>
+      <c r="N18" s="151"/>
+    </row>
+    <row r="19" spans="3:14" x14ac:dyDescent="0.4">
+      <c r="D19" s="151"/>
+      <c r="E19" s="151"/>
+      <c r="F19" s="151"/>
+      <c r="G19" s="151"/>
+      <c r="H19" s="151"/>
+      <c r="I19" s="151"/>
+      <c r="J19" s="151"/>
+      <c r="K19" s="151"/>
+      <c r="L19" s="151"/>
+      <c r="M19" s="151"/>
+      <c r="N19" s="151"/>
+    </row>
+    <row r="20" spans="3:14" x14ac:dyDescent="0.4">
+      <c r="D20" s="151"/>
+      <c r="E20" s="151"/>
+      <c r="F20" s="151"/>
+      <c r="G20" s="151"/>
+      <c r="H20" s="151"/>
+      <c r="I20" s="151"/>
+      <c r="J20" s="151"/>
+      <c r="K20" s="151"/>
+      <c r="L20" s="151"/>
+      <c r="M20" s="151"/>
+      <c r="N20" s="151"/>
+    </row>
+    <row r="23" spans="3:14" x14ac:dyDescent="0.4">
+      <c r="C23" s="152" t="s">
+        <v>525</v>
+      </c>
+      <c r="D23" s="153" t="s">
+        <v>526</v>
+      </c>
+      <c r="E23" s="192" t="s">
+        <v>527</v>
+      </c>
+      <c r="F23" s="193"/>
+    </row>
+    <row r="24" spans="3:14" x14ac:dyDescent="0.4">
+      <c r="C24" s="163"/>
+      <c r="D24" s="155" t="s">
+        <v>548</v>
+      </c>
+      <c r="E24" s="194" t="s">
+        <v>549</v>
+      </c>
+      <c r="F24" s="194"/>
+    </row>
+    <row r="25" spans="3:14" x14ac:dyDescent="0.4">
+      <c r="C25" s="154"/>
+      <c r="D25" s="155">
+        <v>0</v>
+      </c>
+      <c r="E25" s="195" t="s">
+        <v>550</v>
+      </c>
+      <c r="F25" s="195"/>
+    </row>
+    <row r="26" spans="3:14" x14ac:dyDescent="0.4">
+      <c r="C26" s="154"/>
+      <c r="D26" s="156">
+        <v>1</v>
+      </c>
+      <c r="E26" s="196" t="s">
+        <v>551</v>
+      </c>
+      <c r="F26" s="196"/>
+    </row>
+    <row r="27" spans="3:14" x14ac:dyDescent="0.4">
+      <c r="C27" s="157"/>
+      <c r="D27" s="155">
+        <v>2</v>
+      </c>
+      <c r="E27" s="195" t="s">
+        <v>552</v>
+      </c>
+      <c r="F27" s="195"/>
+    </row>
+    <row r="29" spans="3:14" x14ac:dyDescent="0.4">
+      <c r="D29" s="161" t="s">
+        <v>542</v>
+      </c>
+      <c r="E29" s="136" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="30" spans="3:14" x14ac:dyDescent="0.4">
+      <c r="D30" s="162"/>
+      <c r="E30" s="136" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="31" spans="3:14" x14ac:dyDescent="0.4">
+      <c r="E31" s="136" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="32" spans="3:14" x14ac:dyDescent="0.4">
+      <c r="E32" s="136" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.4">
+      <c r="D33" s="162" t="s">
+        <v>547</v>
+      </c>
+      <c r="E33" s="136" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.4">
+      <c r="D34" s="162" t="s">
+        <v>545</v>
+      </c>
+      <c r="E34" s="136" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="40" spans="4:5" x14ac:dyDescent="0.4">
+      <c r="D40" s="158"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+  </mergeCells>
+  <phoneticPr fontId="2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A2:I40"/>
@@ -5791,7 +6451,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A2:I40"/>
@@ -6099,12 +6759,12 @@
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B39" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C39" s="16" t="s">
         <v>40</v>
@@ -6127,7 +6787,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A2:I20"/>
@@ -8554,13 +9214,13 @@
     </row>
     <row r="35" spans="1:89" x14ac:dyDescent="0.4">
       <c r="C35" s="35" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D35" s="130">
         <v>0</v>
       </c>
       <c r="E35" s="35" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
@@ -8662,7 +9322,7 @@
         <v>101</v>
       </c>
       <c r="E37" s="35" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="38" spans="1:89" x14ac:dyDescent="0.4">
@@ -8671,7 +9331,7 @@
         <v>103</v>
       </c>
       <c r="E38" s="35" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="39" spans="1:89" x14ac:dyDescent="0.4">
@@ -8680,7 +9340,7 @@
         <v>107</v>
       </c>
       <c r="E39" s="35" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="40" spans="1:89" x14ac:dyDescent="0.4">
@@ -8689,7 +9349,7 @@
         <v>121</v>
       </c>
       <c r="E40" s="35" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="41" spans="1:89" x14ac:dyDescent="0.4">
@@ -8698,7 +9358,7 @@
         <v>144</v>
       </c>
       <c r="E41" s="35" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="42" spans="1:89" x14ac:dyDescent="0.4">
@@ -8707,7 +9367,7 @@
         <v>145</v>
       </c>
       <c r="E42" s="35" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="43" spans="1:89" x14ac:dyDescent="0.4">
@@ -8716,7 +9376,7 @@
         <v>154</v>
       </c>
       <c r="E43" s="35" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="44" spans="1:89" x14ac:dyDescent="0.4">
@@ -8725,7 +9385,7 @@
         <v>155</v>
       </c>
       <c r="E44" s="35" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="45" spans="1:89" x14ac:dyDescent="0.4">
@@ -8734,7 +9394,7 @@
         <v>171</v>
       </c>
       <c r="E45" s="35" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="46" spans="1:89" x14ac:dyDescent="0.4">
@@ -8743,7 +9403,7 @@
         <v>901</v>
       </c>
       <c r="E46" s="35" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="47" spans="1:89" x14ac:dyDescent="0.4">
@@ -8752,7 +9412,7 @@
         <v>907</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
   </sheetData>
@@ -9340,89 +10000,89 @@
       <c r="C11" s="72" t="s">
         <v>305</v>
       </c>
-      <c r="D11" s="135" t="s">
+      <c r="D11" s="172" t="s">
         <v>299</v>
       </c>
-      <c r="E11" s="136"/>
-      <c r="F11" s="135" t="s">
+      <c r="E11" s="173"/>
+      <c r="F11" s="172" t="s">
         <v>300</v>
       </c>
-      <c r="G11" s="136"/>
+      <c r="G11" s="173"/>
       <c r="L11" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B12" s="134" t="s">
+      <c r="B12" s="188" t="s">
         <v>279</v>
       </c>
       <c r="C12" s="48">
         <v>0</v>
       </c>
-      <c r="D12" s="137" t="s">
+      <c r="D12" s="184" t="s">
         <v>203</v>
       </c>
-      <c r="E12" s="138"/>
-      <c r="F12" s="151" t="s">
+      <c r="E12" s="185"/>
+      <c r="F12" s="174" t="s">
         <v>301</v>
       </c>
-      <c r="G12" s="152"/>
+      <c r="G12" s="175"/>
       <c r="L12" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B13" s="134"/>
+      <c r="B13" s="188"/>
       <c r="C13" s="48">
         <v>1</v>
       </c>
-      <c r="D13" s="137" t="s">
+      <c r="D13" s="184" t="s">
         <v>202</v>
       </c>
-      <c r="E13" s="138"/>
-      <c r="F13" s="153" t="s">
+      <c r="E13" s="185"/>
+      <c r="F13" s="176" t="s">
         <v>308</v>
       </c>
-      <c r="G13" s="154"/>
+      <c r="G13" s="177"/>
       <c r="L13" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B14" s="134"/>
+      <c r="B14" s="188"/>
       <c r="C14" s="48">
         <v>2</v>
       </c>
-      <c r="D14" s="137" t="s">
+      <c r="D14" s="184" t="s">
         <v>201</v>
       </c>
-      <c r="E14" s="138"/>
-      <c r="F14" s="153"/>
-      <c r="G14" s="154"/>
+      <c r="E14" s="185"/>
+      <c r="F14" s="176"/>
+      <c r="G14" s="177"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B15" s="134"/>
+      <c r="B15" s="188"/>
       <c r="C15" s="49">
         <v>3</v>
       </c>
-      <c r="D15" s="137" t="s">
+      <c r="D15" s="184" t="s">
         <v>266</v>
       </c>
-      <c r="E15" s="138"/>
-      <c r="F15" s="153"/>
-      <c r="G15" s="154"/>
+      <c r="E15" s="185"/>
+      <c r="F15" s="176"/>
+      <c r="G15" s="177"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B16" s="134"/>
+      <c r="B16" s="188"/>
       <c r="C16" s="49">
         <v>4</v>
       </c>
-      <c r="D16" s="137" t="s">
+      <c r="D16" s="184" t="s">
         <v>267</v>
       </c>
-      <c r="E16" s="138"/>
-      <c r="F16" s="147"/>
-      <c r="G16" s="148"/>
+      <c r="E16" s="185"/>
+      <c r="F16" s="178"/>
+      <c r="G16" s="179"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B17" s="65" t="s">
@@ -9477,30 +10137,30 @@
       <c r="G20" s="69"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B21" s="132" t="s">
+      <c r="B21" s="186" t="s">
         <v>288</v>
       </c>
       <c r="C21" s="48" t="b">
         <v>1</v>
       </c>
-      <c r="D21" s="137" t="s">
+      <c r="D21" s="184" t="s">
         <v>306</v>
       </c>
-      <c r="E21" s="138"/>
+      <c r="E21" s="185"/>
       <c r="F21" s="73" t="s">
         <v>301</v>
       </c>
       <c r="G21" s="74"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B22" s="132"/>
+      <c r="B22" s="186"/>
       <c r="C22" s="48" t="b">
         <v>0</v>
       </c>
-      <c r="D22" s="137" t="s">
+      <c r="D22" s="184" t="s">
         <v>307</v>
       </c>
-      <c r="E22" s="138"/>
+      <c r="E22" s="185"/>
       <c r="F22" s="75" t="s">
         <v>309</v>
       </c>
@@ -9523,130 +10183,130 @@
       <c r="G23" s="71"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B24" s="132" t="s">
+      <c r="B24" s="186" t="s">
         <v>291</v>
       </c>
       <c r="C24" s="47">
         <v>1</v>
       </c>
-      <c r="D24" s="139" t="s">
+      <c r="D24" s="182" t="s">
         <v>289</v>
       </c>
-      <c r="E24" s="140"/>
-      <c r="F24" s="145" t="s">
+      <c r="E24" s="183"/>
+      <c r="F24" s="180" t="s">
         <v>301</v>
       </c>
-      <c r="G24" s="146"/>
+      <c r="G24" s="181"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B25" s="132"/>
+      <c r="B25" s="186"/>
       <c r="C25" s="47">
         <v>2</v>
       </c>
-      <c r="D25" s="141" t="s">
+      <c r="D25" s="170" t="s">
         <v>280</v>
       </c>
-      <c r="E25" s="142"/>
-      <c r="F25" s="149" t="s">
+      <c r="E25" s="171"/>
+      <c r="F25" s="164" t="s">
         <v>308</v>
       </c>
-      <c r="G25" s="150"/>
+      <c r="G25" s="165"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B26" s="132"/>
+      <c r="B26" s="186"/>
       <c r="C26" s="47">
         <v>3</v>
       </c>
-      <c r="D26" s="141" t="s">
+      <c r="D26" s="170" t="s">
         <v>281</v>
       </c>
-      <c r="E26" s="142"/>
-      <c r="F26" s="149"/>
-      <c r="G26" s="150"/>
+      <c r="E26" s="171"/>
+      <c r="F26" s="164"/>
+      <c r="G26" s="165"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B27" s="132"/>
+      <c r="B27" s="186"/>
       <c r="C27" s="47">
         <v>4</v>
       </c>
-      <c r="D27" s="141" t="s">
+      <c r="D27" s="170" t="s">
         <v>282</v>
       </c>
-      <c r="E27" s="142"/>
-      <c r="F27" s="149"/>
-      <c r="G27" s="150"/>
+      <c r="E27" s="171"/>
+      <c r="F27" s="164"/>
+      <c r="G27" s="165"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B28" s="132"/>
+      <c r="B28" s="186"/>
       <c r="C28" s="47">
         <v>5</v>
       </c>
-      <c r="D28" s="141" t="s">
+      <c r="D28" s="170" t="s">
         <v>283</v>
       </c>
-      <c r="E28" s="142"/>
-      <c r="F28" s="143"/>
-      <c r="G28" s="144"/>
+      <c r="E28" s="171"/>
+      <c r="F28" s="168"/>
+      <c r="G28" s="169"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B29" s="132" t="s">
+      <c r="B29" s="186" t="s">
         <v>292</v>
       </c>
       <c r="C29" s="47">
         <v>1</v>
       </c>
-      <c r="D29" s="139" t="s">
+      <c r="D29" s="182" t="s">
         <v>290</v>
       </c>
-      <c r="E29" s="140"/>
-      <c r="F29" s="145" t="s">
+      <c r="E29" s="183"/>
+      <c r="F29" s="180" t="s">
         <v>301</v>
       </c>
-      <c r="G29" s="146"/>
+      <c r="G29" s="181"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B30" s="132"/>
+      <c r="B30" s="186"/>
       <c r="C30" s="47">
         <v>2</v>
       </c>
-      <c r="D30" s="141" t="s">
+      <c r="D30" s="170" t="s">
         <v>284</v>
       </c>
-      <c r="E30" s="142"/>
-      <c r="F30" s="149" t="s">
+      <c r="E30" s="171"/>
+      <c r="F30" s="164" t="s">
         <v>308</v>
       </c>
-      <c r="G30" s="150"/>
+      <c r="G30" s="165"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B31" s="133" t="s">
+      <c r="B31" s="187" t="s">
         <v>293</v>
       </c>
       <c r="C31" s="47">
         <v>2</v>
       </c>
-      <c r="D31" s="141" t="s">
+      <c r="D31" s="170" t="s">
         <v>285</v>
       </c>
-      <c r="E31" s="142"/>
-      <c r="F31" s="155" t="s">
+      <c r="E31" s="171"/>
+      <c r="F31" s="166" t="s">
         <v>301</v>
       </c>
-      <c r="G31" s="156"/>
+      <c r="G31" s="167"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B32" s="133"/>
+      <c r="B32" s="187"/>
       <c r="C32" s="47">
         <v>3</v>
       </c>
-      <c r="D32" s="141" t="s">
+      <c r="D32" s="170" t="s">
         <v>286</v>
       </c>
-      <c r="E32" s="142"/>
-      <c r="F32" s="143" t="s">
+      <c r="E32" s="171"/>
+      <c r="F32" s="168" t="s">
         <v>308</v>
       </c>
-      <c r="G32" s="144"/>
+      <c r="G32" s="169"/>
     </row>
     <row r="33" spans="1:37" x14ac:dyDescent="0.4">
       <c r="B33" s="6"/>
@@ -9751,7 +10411,7 @@
         <v>129</v>
       </c>
       <c r="W39" s="8" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="X39" s="8" t="s">
         <v>130</v>
@@ -9860,7 +10520,7 @@
         <v>85</v>
       </c>
       <c r="W40" s="7" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="X40" s="7" t="s">
         <v>85</v>
@@ -10160,7 +10820,7 @@
         <v>85</v>
       </c>
       <c r="W44" s="7" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="X44" s="7" t="s">
         <v>85</v>
@@ -20514,43 +21174,43 @@
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
     <mergeCell ref="F30:G30"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="F32:G32"/>
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B24:B28"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="B21:B22"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="5">
@@ -21555,22 +22215,22 @@
       <c r="C10" s="72" t="s">
         <v>352</v>
       </c>
-      <c r="D10" s="157" t="s">
+      <c r="D10" s="189" t="s">
         <v>268</v>
       </c>
-      <c r="E10" s="158"/>
+      <c r="E10" s="190"/>
       <c r="H10" s="72" t="s">
         <v>352</v>
       </c>
-      <c r="I10" s="157" t="s">
+      <c r="I10" s="189" t="s">
         <v>268</v>
       </c>
-      <c r="J10" s="158"/>
-      <c r="K10" s="159" t="s">
+      <c r="J10" s="190"/>
+      <c r="K10" s="191" t="s">
         <v>300</v>
       </c>
-      <c r="L10" s="159"/>
-      <c r="M10" s="159"/>
+      <c r="L10" s="191"/>
+      <c r="M10" s="191"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B11" s="90" t="s">

</xml_diff>

<commit_message>
updated files for ver5.17.0.0
</commit_message>
<xml_diff>
--- a/sample/ExcelMacro/kabuSTATION_API_function_sample.xlsx
+++ b/sample/ExcelMacro/kabuSTATION_API_function_sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OLDPC\kabuSTATION\workspace\resourse\sample\ExcelMacro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\fsv1\システム戦略部\900_Work\Vorthanak\KabuSAPI\東証再編\kabusapi\sample\ExcelMacro\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1832" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1829" uniqueCount="551">
   <si>
     <t>概要</t>
     <rPh sb="0" eb="2">
@@ -2122,50 +2122,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>T1</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>東証一部</t>
-    <rPh sb="0" eb="2">
-      <t>トウショウ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>イチブ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>T2</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>東証二部</t>
-    <rPh sb="0" eb="2">
-      <t>トウショウ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ニブ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>TM</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>マザーズ</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>JQ</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>JASDAQ</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>M</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -2232,9 +2188,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>関数入力する際、「"」ダブルクォーテーションで囲む必要があります。</t>
-  </si>
-  <si>
     <t>追加情報（※）出力フラグ</t>
   </si>
   <si>
@@ -3035,6 +2988,40 @@
   </si>
   <si>
     <t>プレミアム料が入札で決定する銘柄</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>TP</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>TS</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>TG</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>東証プライム</t>
+    <rPh sb="0" eb="2">
+      <t>トウショウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>東証スタンダード</t>
+    <rPh sb="0" eb="2">
+      <t>トウショウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>東証グロース</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>関数入力する際、「"」ダブルクォーテーションで囲む必要があります。</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -3045,7 +3032,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3191,6 +3178,13 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Meiryo UI"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -3230,7 +3224,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -3518,11 +3512,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="197">
+  <cellXfs count="208">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -3694,14 +3697,8 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
@@ -3809,6 +3806,18 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3892,6 +3901,33 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -4381,11 +4417,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="101" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -4395,12 +4431,12 @@
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="104" t="s">
-        <v>400</v>
-      </c>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="106"/>
+      <c r="C3" s="102" t="s">
+        <v>391</v>
+      </c>
+      <c r="D3" s="103"/>
+      <c r="E3" s="103"/>
+      <c r="F3" s="104"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B5" s="5" t="s">
@@ -4410,21 +4446,21 @@
     <row r="6" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B6" s="6"/>
       <c r="C6" s="6" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="F6" s="29"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B7" s="6"/>
       <c r="C7" s="1" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="E7" s="27"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B8" s="6"/>
       <c r="C8" s="7" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
       <c r="E8" s="28"/>
     </row>
@@ -4445,7 +4481,7 @@
         <v>198</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.4">
@@ -4453,16 +4489,16 @@
         <v>12</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>405</v>
+        <v>396</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>323</v>
@@ -4476,10 +4512,10 @@
         <f>"(D"&amp;ROW()&amp;"に関数入力)"</f>
         <v>(D14に関数入力)</v>
       </c>
-      <c r="D14" s="107" t="s">
-        <v>407</v>
-      </c>
-      <c r="E14" s="108" t="s">
+      <c r="D14" s="105" t="s">
+        <v>398</v>
+      </c>
+      <c r="E14" s="106" t="s">
         <v>14</v>
       </c>
       <c r="F14" s="26" t="s">
@@ -4492,12 +4528,12 @@
         <v>14</v>
       </c>
       <c r="I14" s="26" t="s">
-        <v>501</v>
+        <v>492</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D15" s="26"/>
-      <c r="E15" s="108"/>
+      <c r="E15" s="106"/>
       <c r="F15" s="26"/>
       <c r="G15" s="26"/>
       <c r="H15" s="26"/>
@@ -4520,100 +4556,100 @@
       <c r="I17" s="26"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B20" s="109"/>
-      <c r="C20" s="110" t="s">
-        <v>390</v>
+      <c r="B20" s="107"/>
+      <c r="C20" s="108" t="s">
+        <v>381</v>
       </c>
       <c r="D20" s="34" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="C21" s="109" t="s">
+        <v>394</v>
+      </c>
+      <c r="D21" s="109" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="C22" s="109" t="s">
+        <v>400</v>
+      </c>
+      <c r="D22" s="109" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="C23" s="109" t="s">
+        <v>402</v>
+      </c>
+      <c r="D23" s="109" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="C24" s="109" t="s">
+        <v>404</v>
+      </c>
+      <c r="D24" s="109" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="C25" s="109" t="s">
+        <v>406</v>
+      </c>
+      <c r="D25" s="109" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="C26" s="109" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C21" s="111" t="s">
-        <v>403</v>
-      </c>
-      <c r="D21" s="111" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C22" s="111" t="s">
+      <c r="D26" s="109" t="s">
         <v>409</v>
       </c>
-      <c r="D22" s="111" t="s">
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="C27" s="109" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C23" s="111" t="s">
+      <c r="D27" s="109" t="s">
         <v>411</v>
       </c>
-      <c r="D23" s="111" t="s">
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="C28" s="109" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C24" s="111" t="s">
+      <c r="D28" s="109" t="s">
         <v>413</v>
       </c>
-      <c r="D24" s="111" t="s">
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="C29" s="109" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C25" s="111" t="s">
+      <c r="D29" s="109" t="s">
         <v>415</v>
       </c>
-      <c r="D25" s="111" t="s">
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="C30" s="109" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C26" s="111" t="s">
+      <c r="D30" s="109" t="s">
         <v>417</v>
       </c>
-      <c r="D26" s="111" t="s">
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="C31" s="109" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C27" s="111" t="s">
+      <c r="D31" s="109" t="s">
         <v>419</v>
-      </c>
-      <c r="D27" s="111" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C28" s="111" t="s">
-        <v>421</v>
-      </c>
-      <c r="D28" s="111" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C29" s="111" t="s">
-        <v>423</v>
-      </c>
-      <c r="D29" s="111" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C30" s="111" t="s">
-        <v>425</v>
-      </c>
-      <c r="D30" s="111" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C31" s="111" t="s">
-        <v>427</v>
-      </c>
-      <c r="D31" s="111" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.4">
@@ -4672,11 +4708,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="101" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>486</v>
+        <v>477</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -4686,12 +4722,12 @@
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="104" t="s">
-        <v>485</v>
-      </c>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="106"/>
+      <c r="C3" s="102" t="s">
+        <v>476</v>
+      </c>
+      <c r="D3" s="103"/>
+      <c r="E3" s="103"/>
+      <c r="F3" s="104"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B5" s="5" t="s">
@@ -4701,7 +4737,7 @@
     <row r="6" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B6" s="6"/>
       <c r="C6" s="6" t="s">
-        <v>484</v>
+        <v>475</v>
       </c>
       <c r="F6" s="29"/>
     </row>
@@ -4711,7 +4747,7 @@
         <v>320</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="E7" s="27"/>
     </row>
@@ -4726,371 +4762,371 @@
       <c r="E8" s="28"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C10" s="124"/>
-      <c r="D10" s="127" t="s">
-        <v>482</v>
-      </c>
-      <c r="E10" s="127" t="s">
-        <v>481</v>
-      </c>
-      <c r="G10" s="124"/>
-      <c r="H10" s="127" t="s">
-        <v>482</v>
-      </c>
-      <c r="I10" s="127" t="s">
-        <v>481</v>
+      <c r="C10" s="122"/>
+      <c r="D10" s="125" t="s">
+        <v>473</v>
+      </c>
+      <c r="E10" s="125" t="s">
+        <v>472</v>
+      </c>
+      <c r="G10" s="122"/>
+      <c r="H10" s="125" t="s">
+        <v>473</v>
+      </c>
+      <c r="I10" s="125" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C11" s="123" t="s">
-        <v>480</v>
-      </c>
-      <c r="D11" s="116" t="s">
+      <c r="C11" s="121" t="s">
+        <v>471</v>
+      </c>
+      <c r="D11" s="114" t="s">
+        <v>459</v>
+      </c>
+      <c r="E11" s="116" t="s">
+        <v>463</v>
+      </c>
+      <c r="G11" s="121" t="s">
         <v>468</v>
       </c>
-      <c r="E11" s="118" t="s">
+      <c r="H11" s="114" t="s">
+        <v>465</v>
+      </c>
+      <c r="I11" s="116" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="C12" s="118"/>
+      <c r="D12" s="114" t="s">
+        <v>449</v>
+      </c>
+      <c r="E12" s="116" t="s">
+        <v>457</v>
+      </c>
+      <c r="G12" s="118" t="s">
+        <v>461</v>
+      </c>
+      <c r="H12" s="114" t="s">
+        <v>459</v>
+      </c>
+      <c r="I12" s="116" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="C13" s="118"/>
+      <c r="D13" s="114" t="s">
+        <v>443</v>
+      </c>
+      <c r="E13" s="116" t="s">
+        <v>450</v>
+      </c>
+      <c r="G13" s="115" t="s">
+        <v>454</v>
+      </c>
+      <c r="H13" s="114" t="s">
+        <v>452</v>
+      </c>
+      <c r="I13" s="116" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="C14" s="119"/>
+      <c r="D14" s="114" t="s">
+        <v>439</v>
+      </c>
+      <c r="E14" s="113" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="17" spans="3:14" x14ac:dyDescent="0.4">
+      <c r="C17" s="122"/>
+      <c r="D17" s="125" t="s">
+        <v>473</v>
+      </c>
+      <c r="E17" s="125" t="s">
         <v>472</v>
       </c>
-      <c r="G11" s="123" t="s">
-        <v>477</v>
-      </c>
-      <c r="H11" s="116" t="s">
-        <v>474</v>
-      </c>
-      <c r="I11" s="118" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C12" s="120"/>
-      <c r="D12" s="116" t="s">
+      <c r="G17" s="122"/>
+      <c r="H17" s="125" t="s">
+        <v>473</v>
+      </c>
+      <c r="I17" s="125" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="18" spans="3:14" x14ac:dyDescent="0.4">
+      <c r="C18" s="121" t="s">
+        <v>470</v>
+      </c>
+      <c r="D18" s="114" t="s">
+        <v>465</v>
+      </c>
+      <c r="E18" s="116" t="s">
+        <v>467</v>
+      </c>
+      <c r="G18" s="121" t="s">
+        <v>466</v>
+      </c>
+      <c r="H18" s="114" t="s">
+        <v>465</v>
+      </c>
+      <c r="I18" s="116" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="19" spans="3:14" x14ac:dyDescent="0.4">
+      <c r="C19" s="118"/>
+      <c r="D19" s="114" t="s">
+        <v>459</v>
+      </c>
+      <c r="E19" s="116" t="s">
+        <v>463</v>
+      </c>
+      <c r="G19" s="118"/>
+      <c r="H19" s="114" t="s">
+        <v>459</v>
+      </c>
+      <c r="I19" s="116" t="s">
         <v>458</v>
       </c>
-      <c r="E12" s="118" t="s">
-        <v>466</v>
-      </c>
-      <c r="G12" s="120" t="s">
-        <v>470</v>
-      </c>
-      <c r="H12" s="116" t="s">
-        <v>468</v>
-      </c>
-      <c r="I12" s="118" t="s">
+    </row>
+    <row r="20" spans="3:14" x14ac:dyDescent="0.4">
+      <c r="C20" s="118"/>
+      <c r="D20" s="114" t="s">
+        <v>449</v>
+      </c>
+      <c r="E20" s="116" t="s">
+        <v>457</v>
+      </c>
+      <c r="G20" s="115"/>
+      <c r="H20" s="114" t="s">
+        <v>452</v>
+      </c>
+      <c r="I20" s="116" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="21" spans="3:14" x14ac:dyDescent="0.4">
+      <c r="C21" s="118"/>
+      <c r="D21" s="114" t="s">
+        <v>443</v>
+      </c>
+      <c r="E21" s="116" t="s">
+        <v>450</v>
+      </c>
+      <c r="L21" s="111"/>
+      <c r="M21" s="112"/>
+      <c r="N21" s="111"/>
+    </row>
+    <row r="22" spans="3:14" x14ac:dyDescent="0.4">
+      <c r="C22" s="118"/>
+      <c r="D22" s="114" t="s">
+        <v>439</v>
+      </c>
+      <c r="E22" s="113" t="s">
+        <v>447</v>
+      </c>
+      <c r="L22" s="111"/>
+      <c r="M22" s="112"/>
+      <c r="N22" s="111"/>
+    </row>
+    <row r="23" spans="3:14" x14ac:dyDescent="0.4">
+      <c r="C23" s="118"/>
+      <c r="D23" s="114" t="s">
+        <v>431</v>
+      </c>
+      <c r="E23" s="116" t="s">
+        <v>444</v>
+      </c>
+      <c r="L23" s="111"/>
+      <c r="M23" s="112"/>
+      <c r="N23" s="111"/>
+    </row>
+    <row r="24" spans="3:14" x14ac:dyDescent="0.4">
+      <c r="C24" s="118"/>
+      <c r="D24" s="114" t="s">
+        <v>441</v>
+      </c>
+      <c r="E24" s="116" t="s">
+        <v>440</v>
+      </c>
+      <c r="L24" s="111"/>
+      <c r="M24" s="112"/>
+      <c r="N24" s="111"/>
+    </row>
+    <row r="25" spans="3:14" x14ac:dyDescent="0.4">
+      <c r="C25" s="115"/>
+      <c r="D25" s="114" t="s">
+        <v>437</v>
+      </c>
+      <c r="E25" s="116" t="s">
+        <v>436</v>
+      </c>
+      <c r="L25" s="111"/>
+      <c r="M25" s="112"/>
+      <c r="N25" s="111"/>
+    </row>
+    <row r="26" spans="3:14" x14ac:dyDescent="0.4">
+      <c r="L26" s="111"/>
+      <c r="M26" s="112"/>
+      <c r="N26" s="111"/>
+    </row>
+    <row r="27" spans="3:14" x14ac:dyDescent="0.4">
+      <c r="L27" s="111"/>
+      <c r="M27" s="112"/>
+      <c r="N27" s="111"/>
+    </row>
+    <row r="28" spans="3:14" x14ac:dyDescent="0.4">
+      <c r="C28" s="122"/>
+      <c r="D28" s="125" t="s">
+        <v>473</v>
+      </c>
+      <c r="E28" s="125" t="s">
+        <v>472</v>
+      </c>
+      <c r="L28" s="111"/>
+      <c r="M28" s="112"/>
+      <c r="N28" s="111"/>
+    </row>
+    <row r="29" spans="3:14" x14ac:dyDescent="0.4">
+      <c r="C29" s="121" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C13" s="120"/>
-      <c r="D13" s="116" t="s">
+      <c r="D29" s="114" t="s">
+        <v>465</v>
+      </c>
+      <c r="E29" s="116" t="s">
+        <v>467</v>
+      </c>
+      <c r="L29" s="111"/>
+      <c r="M29" s="112"/>
+      <c r="N29" s="111"/>
+    </row>
+    <row r="30" spans="3:14" x14ac:dyDescent="0.4">
+      <c r="C30" s="120" t="s">
+        <v>461</v>
+      </c>
+      <c r="D30" s="114" t="s">
+        <v>459</v>
+      </c>
+      <c r="E30" s="116" t="s">
+        <v>462</v>
+      </c>
+      <c r="L30" s="111"/>
+      <c r="M30" s="112"/>
+      <c r="N30" s="111"/>
+    </row>
+    <row r="31" spans="3:14" x14ac:dyDescent="0.4">
+      <c r="C31" s="118" t="s">
+        <v>456</v>
+      </c>
+      <c r="D31" s="114" t="s">
         <v>452</v>
       </c>
-      <c r="E13" s="118" t="s">
-        <v>459</v>
-      </c>
-      <c r="G13" s="117" t="s">
-        <v>463</v>
-      </c>
-      <c r="H13" s="116" t="s">
-        <v>461</v>
-      </c>
-      <c r="I13" s="118" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C14" s="121"/>
-      <c r="D14" s="116" t="s">
+      <c r="E31" s="116" t="s">
+        <v>455</v>
+      </c>
+      <c r="L31" s="111"/>
+      <c r="M31" s="112"/>
+      <c r="N31" s="111"/>
+    </row>
+    <row r="32" spans="3:14" x14ac:dyDescent="0.4">
+      <c r="C32" s="118"/>
+      <c r="D32" s="114" t="s">
+        <v>449</v>
+      </c>
+      <c r="E32" s="116" t="s">
         <v>448</v>
       </c>
-      <c r="E14" s="115" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.4">
-      <c r="C17" s="124"/>
-      <c r="D17" s="127" t="s">
-        <v>482</v>
-      </c>
-      <c r="E17" s="127" t="s">
-        <v>481</v>
-      </c>
-      <c r="G17" s="124"/>
-      <c r="H17" s="127" t="s">
-        <v>482</v>
-      </c>
-      <c r="I17" s="127" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.4">
-      <c r="C18" s="123" t="s">
-        <v>479</v>
-      </c>
-      <c r="D18" s="116" t="s">
-        <v>474</v>
-      </c>
-      <c r="E18" s="118" t="s">
-        <v>476</v>
-      </c>
-      <c r="G18" s="123" t="s">
-        <v>475</v>
-      </c>
-      <c r="H18" s="116" t="s">
-        <v>474</v>
-      </c>
-      <c r="I18" s="118" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.4">
-      <c r="C19" s="120"/>
-      <c r="D19" s="116" t="s">
-        <v>468</v>
-      </c>
-      <c r="E19" s="118" t="s">
-        <v>472</v>
-      </c>
-      <c r="G19" s="120"/>
-      <c r="H19" s="116" t="s">
-        <v>468</v>
-      </c>
-      <c r="I19" s="118" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.4">
-      <c r="C20" s="120"/>
-      <c r="D20" s="116" t="s">
-        <v>458</v>
-      </c>
-      <c r="E20" s="118" t="s">
-        <v>466</v>
-      </c>
-      <c r="G20" s="117"/>
-      <c r="H20" s="116" t="s">
-        <v>461</v>
-      </c>
-      <c r="I20" s="118" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="21" spans="3:14" x14ac:dyDescent="0.4">
-      <c r="C21" s="120"/>
-      <c r="D21" s="116" t="s">
-        <v>452</v>
-      </c>
-      <c r="E21" s="118" t="s">
-        <v>459</v>
-      </c>
-      <c r="L21" s="113"/>
-      <c r="M21" s="114"/>
-      <c r="N21" s="113"/>
-    </row>
-    <row r="22" spans="3:14" x14ac:dyDescent="0.4">
-      <c r="C22" s="120"/>
-      <c r="D22" s="116" t="s">
-        <v>448</v>
-      </c>
-      <c r="E22" s="115" t="s">
-        <v>456</v>
-      </c>
-      <c r="L22" s="113"/>
-      <c r="M22" s="114"/>
-      <c r="N22" s="113"/>
-    </row>
-    <row r="23" spans="3:14" x14ac:dyDescent="0.4">
-      <c r="C23" s="120"/>
-      <c r="D23" s="116" t="s">
-        <v>440</v>
-      </c>
-      <c r="E23" s="118" t="s">
-        <v>453</v>
-      </c>
-      <c r="L23" s="113"/>
-      <c r="M23" s="114"/>
-      <c r="N23" s="113"/>
-    </row>
-    <row r="24" spans="3:14" x14ac:dyDescent="0.4">
-      <c r="C24" s="120"/>
-      <c r="D24" s="116" t="s">
-        <v>450</v>
-      </c>
-      <c r="E24" s="118" t="s">
-        <v>449</v>
-      </c>
-      <c r="L24" s="113"/>
-      <c r="M24" s="114"/>
-      <c r="N24" s="113"/>
-    </row>
-    <row r="25" spans="3:14" x14ac:dyDescent="0.4">
-      <c r="C25" s="117"/>
-      <c r="D25" s="116" t="s">
+      <c r="L32" s="111"/>
+      <c r="M32" s="112"/>
+      <c r="N32" s="111"/>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.4">
+      <c r="C33" s="118"/>
+      <c r="D33" s="114" t="s">
         <v>446</v>
       </c>
-      <c r="E25" s="118" t="s">
+      <c r="E33" s="116" t="s">
         <v>445</v>
       </c>
-      <c r="L25" s="113"/>
-      <c r="M25" s="114"/>
-      <c r="N25" s="113"/>
-    </row>
-    <row r="26" spans="3:14" x14ac:dyDescent="0.4">
-      <c r="L26" s="113"/>
-      <c r="M26" s="114"/>
-      <c r="N26" s="113"/>
-    </row>
-    <row r="27" spans="3:14" x14ac:dyDescent="0.4">
-      <c r="L27" s="113"/>
-      <c r="M27" s="114"/>
-      <c r="N27" s="113"/>
-    </row>
-    <row r="28" spans="3:14" x14ac:dyDescent="0.4">
-      <c r="C28" s="124"/>
-      <c r="D28" s="127" t="s">
-        <v>482</v>
-      </c>
-      <c r="E28" s="127" t="s">
-        <v>481</v>
-      </c>
-      <c r="L28" s="113"/>
-      <c r="M28" s="114"/>
-      <c r="N28" s="113"/>
-    </row>
-    <row r="29" spans="3:14" x14ac:dyDescent="0.4">
-      <c r="C29" s="123" t="s">
-        <v>478</v>
-      </c>
-      <c r="D29" s="116" t="s">
-        <v>474</v>
-      </c>
-      <c r="E29" s="118" t="s">
-        <v>476</v>
-      </c>
-      <c r="L29" s="113"/>
-      <c r="M29" s="114"/>
-      <c r="N29" s="113"/>
-    </row>
-    <row r="30" spans="3:14" x14ac:dyDescent="0.4">
-      <c r="C30" s="122" t="s">
-        <v>470</v>
-      </c>
-      <c r="D30" s="116" t="s">
-        <v>468</v>
-      </c>
-      <c r="E30" s="118" t="s">
-        <v>471</v>
-      </c>
-      <c r="L30" s="113"/>
-      <c r="M30" s="114"/>
-      <c r="N30" s="113"/>
-    </row>
-    <row r="31" spans="3:14" x14ac:dyDescent="0.4">
-      <c r="C31" s="120" t="s">
-        <v>465</v>
-      </c>
-      <c r="D31" s="116" t="s">
-        <v>461</v>
-      </c>
-      <c r="E31" s="118" t="s">
-        <v>464</v>
-      </c>
-      <c r="L31" s="113"/>
-      <c r="M31" s="114"/>
-      <c r="N31" s="113"/>
-    </row>
-    <row r="32" spans="3:14" x14ac:dyDescent="0.4">
-      <c r="C32" s="120"/>
-      <c r="D32" s="116" t="s">
-        <v>458</v>
-      </c>
-      <c r="E32" s="118" t="s">
-        <v>457</v>
-      </c>
-      <c r="L32" s="113"/>
-      <c r="M32" s="114"/>
-      <c r="N32" s="113"/>
-    </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="C33" s="120"/>
-      <c r="D33" s="116" t="s">
-        <v>455</v>
-      </c>
-      <c r="E33" s="118" t="s">
-        <v>454</v>
-      </c>
-      <c r="L33" s="113"/>
-      <c r="M33" s="114"/>
-      <c r="N33" s="113"/>
+      <c r="L33" s="111"/>
+      <c r="M33" s="112"/>
+      <c r="N33" s="111"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="C34" s="120"/>
-      <c r="D34" s="116" t="s">
-        <v>452</v>
-      </c>
-      <c r="E34" s="115" t="s">
-        <v>451</v>
-      </c>
-      <c r="L34" s="113"/>
-      <c r="M34" s="114"/>
-      <c r="N34" s="113"/>
+      <c r="C34" s="118"/>
+      <c r="D34" s="114" t="s">
+        <v>443</v>
+      </c>
+      <c r="E34" s="113" t="s">
+        <v>442</v>
+      </c>
+      <c r="L34" s="111"/>
+      <c r="M34" s="112"/>
+      <c r="N34" s="111"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="C35" s="120"/>
-      <c r="D35" s="116" t="s">
-        <v>448</v>
-      </c>
-      <c r="E35" s="118" t="s">
-        <v>447</v>
-      </c>
-      <c r="L35" s="113"/>
-      <c r="M35" s="114"/>
-      <c r="N35" s="113"/>
+      <c r="C35" s="118"/>
+      <c r="D35" s="114" t="s">
+        <v>439</v>
+      </c>
+      <c r="E35" s="116" t="s">
+        <v>438</v>
+      </c>
+      <c r="L35" s="111"/>
+      <c r="M35" s="112"/>
+      <c r="N35" s="111"/>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="C36" s="120"/>
-      <c r="D36" s="116" t="s">
-        <v>444</v>
-      </c>
-      <c r="E36" s="118" t="s">
-        <v>443</v>
-      </c>
-      <c r="L36" s="113"/>
-      <c r="M36" s="114"/>
-      <c r="N36" s="113"/>
+      <c r="C36" s="118"/>
+      <c r="D36" s="114" t="s">
+        <v>435</v>
+      </c>
+      <c r="E36" s="116" t="s">
+        <v>434</v>
+      </c>
+      <c r="L36" s="111"/>
+      <c r="M36" s="112"/>
+      <c r="N36" s="111"/>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="C37" s="119"/>
-      <c r="D37" s="116" t="s">
-        <v>442</v>
-      </c>
-      <c r="E37" s="118" t="s">
-        <v>441</v>
-      </c>
-      <c r="L37" s="113"/>
-      <c r="M37" s="114"/>
-      <c r="N37" s="113"/>
+      <c r="C37" s="117"/>
+      <c r="D37" s="114" t="s">
+        <v>433</v>
+      </c>
+      <c r="E37" s="116" t="s">
+        <v>432</v>
+      </c>
+      <c r="L37" s="111"/>
+      <c r="M37" s="112"/>
+      <c r="N37" s="111"/>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="C38" s="117"/>
-      <c r="D38" s="116" t="s">
-        <v>440</v>
-      </c>
-      <c r="E38" s="115" t="s">
-        <v>439</v>
-      </c>
-      <c r="L38" s="113"/>
-      <c r="M38" s="114"/>
-      <c r="N38" s="113"/>
+      <c r="C38" s="115"/>
+      <c r="D38" s="114" t="s">
+        <v>431</v>
+      </c>
+      <c r="E38" s="113" t="s">
+        <v>430</v>
+      </c>
+      <c r="L38" s="111"/>
+      <c r="M38" s="112"/>
+      <c r="N38" s="111"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="L39" s="113"/>
-      <c r="M39" s="114"/>
-      <c r="N39" s="113"/>
+      <c r="L39" s="111"/>
+      <c r="M39" s="112"/>
+      <c r="N39" s="111"/>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="L40" s="113"/>
-      <c r="M40" s="114"/>
-      <c r="N40" s="113"/>
+      <c r="L40" s="111"/>
+      <c r="M40" s="112"/>
+      <c r="N40" s="111"/>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B42" s="5" t="s">
@@ -5106,7 +5142,7 @@
         <v>10</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.4">
@@ -5117,25 +5153,25 @@
         <v>320</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>528</v>
+        <v>519</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>530</v>
+        <v>521</v>
       </c>
       <c r="J45" s="8" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="K45" s="8" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.4">
@@ -5143,10 +5179,10 @@
         <f>"(D"&amp;ROW()&amp;"に関数入力)"</f>
         <v>(D46に関数入力)</v>
       </c>
-      <c r="D46" s="108" t="s">
+      <c r="D46" s="106" t="s">
         <v>295</v>
       </c>
-      <c r="E46" s="108" t="s">
+      <c r="E46" s="106" t="s">
         <v>14</v>
       </c>
       <c r="F46" s="26" t="s">
@@ -5159,20 +5195,20 @@
         <v>14</v>
       </c>
       <c r="I46" s="26" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="J46" s="26" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="K46" s="26" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="D47" s="108" t="s">
+      <c r="D47" s="106" t="s">
         <v>295</v>
       </c>
-      <c r="E47" s="108" t="s">
+      <c r="E47" s="106" t="s">
         <v>14</v>
       </c>
       <c r="F47" s="26" t="s">
@@ -5185,20 +5221,20 @@
         <v>14</v>
       </c>
       <c r="I47" s="26" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="J47" s="26" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="K47" s="26" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="D48" s="108" t="s">
+      <c r="D48" s="106" t="s">
         <v>295</v>
       </c>
-      <c r="E48" s="108" t="s">
+      <c r="E48" s="106" t="s">
         <v>14</v>
       </c>
       <c r="F48" s="26" t="s">
@@ -5211,10 +5247,10 @@
         <v>14</v>
       </c>
       <c r="I48" s="26" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="J48" s="26" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="K48" s="26" t="s">
         <v>14</v>
@@ -5222,7 +5258,7 @@
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.4">
       <c r="D49" s="26"/>
-      <c r="E49" s="108"/>
+      <c r="E49" s="106"/>
       <c r="F49" s="26"/>
       <c r="G49" s="26"/>
       <c r="H49" s="26"/>
@@ -5232,7 +5268,7 @@
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.4">
       <c r="D50" s="26"/>
-      <c r="E50" s="108"/>
+      <c r="E50" s="106"/>
       <c r="F50" s="26"/>
       <c r="G50" s="26"/>
       <c r="H50" s="26"/>
@@ -5277,17 +5313,17 @@
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B56" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B57" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B58" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>
@@ -5329,11 +5365,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="101" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="D2" s="4"/>
     </row>
@@ -5341,10 +5377,10 @@
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="104" t="s">
-        <v>490</v>
-      </c>
-      <c r="D3" s="106"/>
+      <c r="C3" s="102" t="s">
+        <v>481</v>
+      </c>
+      <c r="D3" s="104"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B5" s="5" t="s">
@@ -5354,7 +5390,7 @@
     <row r="6" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B6" s="6"/>
       <c r="C6" s="6" t="s">
-        <v>488</v>
+        <v>479</v>
       </c>
       <c r="F6" s="29"/>
     </row>
@@ -5363,7 +5399,7 @@
       <c r="C7" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="D7" s="126"/>
+      <c r="D7" s="124"/>
       <c r="E7" s="27"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.4">
@@ -5371,7 +5407,7 @@
       <c r="C8" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="125"/>
+      <c r="D8" s="123"/>
       <c r="E8" s="28"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.4">
@@ -5388,7 +5424,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>488</v>
+        <v>479</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.4">
@@ -5399,7 +5435,7 @@
         <v>320</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>487</v>
+        <v>478</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.4">
@@ -5407,32 +5443,32 @@
         <f>"(D"&amp;ROW()&amp;"に関数入力)"</f>
         <v>(D14に関数入力)</v>
       </c>
-      <c r="D14" s="108" t="s">
+      <c r="D14" s="106" t="s">
         <v>295</v>
       </c>
-      <c r="E14" s="108" t="s">
+      <c r="E14" s="106" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.4">
       <c r="D15" s="26"/>
-      <c r="E15" s="108"/>
+      <c r="E15" s="106"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.4">
       <c r="D16" s="26"/>
-      <c r="E16" s="108"/>
+      <c r="E16" s="106"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.4">
       <c r="D17" s="26"/>
-      <c r="E17" s="108"/>
+      <c r="E17" s="106"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.4">
       <c r="D18" s="26"/>
-      <c r="E18" s="108"/>
+      <c r="E18" s="106"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.4">
       <c r="D19" t="s">
-        <v>489</v>
+        <v>480</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.4">
@@ -5446,12 +5482,12 @@
       <c r="K20" s="46"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="C21" s="124"/>
-      <c r="D21" s="127" t="s">
-        <v>482</v>
-      </c>
-      <c r="E21" s="127" t="s">
-        <v>481</v>
+      <c r="C21" s="122"/>
+      <c r="D21" s="125" t="s">
+        <v>473</v>
+      </c>
+      <c r="E21" s="125" t="s">
+        <v>472</v>
       </c>
       <c r="F21" s="46"/>
       <c r="G21" s="46"/>
@@ -5461,41 +5497,41 @@
       <c r="K21" s="46"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="C22" s="123" t="s">
-        <v>502</v>
-      </c>
-      <c r="D22" s="116" t="s">
-        <v>468</v>
-      </c>
-      <c r="E22" s="118" t="s">
-        <v>472</v>
+      <c r="C22" s="121" t="s">
+        <v>493</v>
+      </c>
+      <c r="D22" s="114" t="s">
+        <v>459</v>
+      </c>
+      <c r="E22" s="116" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="C23" s="120"/>
-      <c r="D23" s="116" t="s">
-        <v>458</v>
-      </c>
-      <c r="E23" s="118" t="s">
-        <v>466</v>
+      <c r="C23" s="118"/>
+      <c r="D23" s="114" t="s">
+        <v>449</v>
+      </c>
+      <c r="E23" s="116" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="C24" s="120"/>
-      <c r="D24" s="116" t="s">
-        <v>452</v>
-      </c>
-      <c r="E24" s="118" t="s">
-        <v>459</v>
+      <c r="C24" s="118"/>
+      <c r="D24" s="114" t="s">
+        <v>443</v>
+      </c>
+      <c r="E24" s="116" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="C25" s="121"/>
-      <c r="D25" s="116" t="s">
-        <v>448</v>
-      </c>
-      <c r="E25" s="115" t="s">
-        <v>456</v>
+      <c r="C25" s="119"/>
+      <c r="D25" s="114" t="s">
+        <v>439</v>
+      </c>
+      <c r="E25" s="113" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.4">
@@ -5546,11 +5582,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="101" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>500</v>
+        <v>491</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
@@ -5559,11 +5595,11 @@
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="104" t="s">
-        <v>499</v>
-      </c>
-      <c r="D3" s="105"/>
-      <c r="E3" s="106"/>
+      <c r="C3" s="102" t="s">
+        <v>490</v>
+      </c>
+      <c r="D3" s="103"/>
+      <c r="E3" s="104"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B5" s="5" t="s">
@@ -5573,13 +5609,13 @@
     <row r="6" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B6" s="6"/>
       <c r="C6" s="6" t="s">
-        <v>498</v>
+        <v>489</v>
       </c>
       <c r="F6" s="29"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B7" s="6"/>
-      <c r="C7" s="126"/>
+      <c r="C7" s="124"/>
       <c r="D7" s="27"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.4">
@@ -5596,30 +5632,30 @@
         <v>10</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>498</v>
+        <v>489</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="103" t="s">
-        <v>497</v>
-      </c>
-      <c r="E11" s="103" t="s">
-        <v>496</v>
-      </c>
-      <c r="F11" s="103" t="s">
-        <v>495</v>
-      </c>
-      <c r="G11" s="103" t="s">
-        <v>494</v>
-      </c>
-      <c r="H11" s="103" t="s">
-        <v>493</v>
+      <c r="D11" s="101" t="s">
+        <v>488</v>
+      </c>
+      <c r="E11" s="101" t="s">
+        <v>487</v>
+      </c>
+      <c r="F11" s="101" t="s">
+        <v>486</v>
+      </c>
+      <c r="G11" s="101" t="s">
+        <v>485</v>
+      </c>
+      <c r="H11" s="101" t="s">
+        <v>484</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.4">
@@ -5627,56 +5663,56 @@
         <f>"(D"&amp;ROW()&amp;"に関数入力)"</f>
         <v>(D12に関数入力)</v>
       </c>
-      <c r="D12" s="108" t="s">
+      <c r="D12" s="106" t="s">
         <v>295</v>
       </c>
-      <c r="E12" s="108" t="s">
+      <c r="E12" s="106" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="108" t="s">
+      <c r="F12" s="106" t="s">
         <v>295</v>
       </c>
-      <c r="G12" s="108" t="s">
+      <c r="G12" s="106" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="108" t="s">
+      <c r="H12" s="106" t="s">
         <v>295</v>
       </c>
-      <c r="I12" s="108" t="s">
+      <c r="I12" s="106" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D13" s="26"/>
-      <c r="E13" s="108"/>
+      <c r="E13" s="106"/>
       <c r="F13" s="26"/>
-      <c r="G13" s="108"/>
+      <c r="G13" s="106"/>
       <c r="H13" s="26"/>
-      <c r="I13" s="108"/>
+      <c r="I13" s="106"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D14" s="26"/>
-      <c r="E14" s="108"/>
+      <c r="E14" s="106"/>
       <c r="F14" s="26"/>
-      <c r="G14" s="108"/>
+      <c r="G14" s="106"/>
       <c r="H14" s="26"/>
-      <c r="I14" s="108"/>
+      <c r="I14" s="106"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D15" s="26"/>
-      <c r="E15" s="108"/>
+      <c r="E15" s="106"/>
       <c r="F15" s="26"/>
-      <c r="G15" s="108"/>
+      <c r="G15" s="106"/>
       <c r="H15" s="26"/>
-      <c r="I15" s="108"/>
+      <c r="I15" s="106"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.4">
       <c r="D16" s="26"/>
-      <c r="E16" s="108"/>
+      <c r="E16" s="106"/>
       <c r="F16" s="26"/>
-      <c r="G16" s="108"/>
+      <c r="G16" s="106"/>
       <c r="H16" s="26"/>
-      <c r="I16" s="108"/>
+      <c r="I16" s="106"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.4">
       <c r="D17" s="46"/>
@@ -5712,7 +5748,7 @@
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B21" s="112"/>
+      <c r="B21" s="110"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
@@ -5729,39 +5765,39 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="9" style="136"/>
-    <col min="3" max="3" width="19.125" style="136" customWidth="1"/>
-    <col min="4" max="4" width="18" style="136" customWidth="1"/>
-    <col min="5" max="14" width="21" style="136" customWidth="1"/>
-    <col min="15" max="16" width="22.25" style="136" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9" style="136"/>
+    <col min="1" max="2" width="9" style="134"/>
+    <col min="3" max="3" width="19.125" style="134" customWidth="1"/>
+    <col min="4" max="4" width="18" style="134" customWidth="1"/>
+    <col min="5" max="14" width="21" style="134" customWidth="1"/>
+    <col min="15" max="16" width="22.25" style="134" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9" style="134"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B2" s="132" t="s">
+      <c r="B2" s="130" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="132" t="s">
-        <v>533</v>
-      </c>
-      <c r="D2" s="133"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="135"/>
-      <c r="H2" s="135"/>
+      <c r="C2" s="130" t="s">
+        <v>524</v>
+      </c>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="132"/>
+      <c r="G2" s="133"/>
+      <c r="H2" s="133"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B3" s="137" t="s">
+      <c r="B3" s="135" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="132" t="s">
-        <v>523</v>
-      </c>
-      <c r="D3" s="133"/>
-      <c r="E3" s="133"/>
-      <c r="F3" s="134"/>
-      <c r="G3" s="135"/>
-      <c r="H3" s="135"/>
+      <c r="C3" s="130" t="s">
+        <v>514</v>
+      </c>
+      <c r="D3" s="131"/>
+      <c r="E3" s="131"/>
+      <c r="F3" s="132"/>
+      <c r="G3" s="133"/>
+      <c r="H3" s="133"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B5" s="5" t="s">
@@ -5769,17 +5805,17 @@
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="C6" s="138" t="s">
-        <v>524</v>
+      <c r="C6" s="136" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="C7" s="139" t="s">
+      <c r="C7" s="137" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="C8" s="140" t="s">
+      <c r="C8" s="138" t="s">
         <v>295</v>
       </c>
     </row>
@@ -5787,273 +5823,273 @@
       <c r="B10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="141"/>
-      <c r="D10" s="141"/>
+      <c r="C10" s="139"/>
+      <c r="D10" s="139"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="C12" s="142" t="s">
+      <c r="C12" s="140" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="143" t="s">
-        <v>535</v>
+      <c r="D12" s="141" t="s">
+        <v>526</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="C13" s="135"/>
-      <c r="D13" s="144"/>
-      <c r="E13" s="145"/>
-      <c r="F13" s="146"/>
-      <c r="G13" s="147" t="s">
-        <v>536</v>
-      </c>
-      <c r="H13" s="146"/>
-      <c r="I13" s="148"/>
-      <c r="J13" s="146"/>
-      <c r="K13" s="146"/>
-      <c r="L13" s="146"/>
-      <c r="M13" s="147" t="s">
-        <v>537</v>
-      </c>
-      <c r="N13" s="148"/>
-      <c r="O13" s="160"/>
-      <c r="P13" s="160"/>
+      <c r="C13" s="133"/>
+      <c r="D13" s="142"/>
+      <c r="E13" s="143"/>
+      <c r="F13" s="144"/>
+      <c r="G13" s="145" t="s">
+        <v>527</v>
+      </c>
+      <c r="H13" s="144"/>
+      <c r="I13" s="146"/>
+      <c r="J13" s="144"/>
+      <c r="K13" s="144"/>
+      <c r="L13" s="144"/>
+      <c r="M13" s="145" t="s">
+        <v>528</v>
+      </c>
+      <c r="N13" s="146"/>
+      <c r="O13" s="158"/>
+      <c r="P13" s="158"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="C14" s="149" t="s">
+      <c r="C14" s="147" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="150" t="s">
+      <c r="D14" s="148" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="159" t="s">
-        <v>525</v>
-      </c>
-      <c r="F14" s="159" t="s">
-        <v>529</v>
-      </c>
-      <c r="G14" s="159" t="s">
-        <v>531</v>
-      </c>
-      <c r="H14" s="159" t="s">
-        <v>532</v>
-      </c>
-      <c r="I14" s="159" t="s">
-        <v>543</v>
-      </c>
-      <c r="J14" s="159" t="s">
-        <v>525</v>
-      </c>
-      <c r="K14" s="159" t="s">
-        <v>529</v>
-      </c>
-      <c r="L14" s="159" t="s">
-        <v>531</v>
-      </c>
-      <c r="M14" s="159" t="s">
-        <v>532</v>
-      </c>
-      <c r="N14" s="159" t="s">
-        <v>543</v>
+      <c r="E14" s="157" t="s">
+        <v>516</v>
+      </c>
+      <c r="F14" s="157" t="s">
+        <v>520</v>
+      </c>
+      <c r="G14" s="157" t="s">
+        <v>522</v>
+      </c>
+      <c r="H14" s="157" t="s">
+        <v>523</v>
+      </c>
+      <c r="I14" s="157" t="s">
+        <v>534</v>
+      </c>
+      <c r="J14" s="157" t="s">
+        <v>516</v>
+      </c>
+      <c r="K14" s="157" t="s">
+        <v>520</v>
+      </c>
+      <c r="L14" s="157" t="s">
+        <v>522</v>
+      </c>
+      <c r="M14" s="157" t="s">
+        <v>523</v>
+      </c>
+      <c r="N14" s="157" t="s">
+        <v>534</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="C15" s="135" t="str">
+      <c r="C15" s="133" t="str">
         <f>"(D"&amp;ROW()&amp;"に関数入力)"</f>
         <v>(D15に関数入力)</v>
       </c>
-      <c r="D15" s="151" t="s">
-        <v>534</v>
-      </c>
-      <c r="E15" s="151" t="s">
+      <c r="D15" s="149" t="s">
+        <v>525</v>
+      </c>
+      <c r="E15" s="149" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="151" t="s">
+      <c r="F15" s="149" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="151" t="s">
+      <c r="G15" s="149" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="151" t="s">
+      <c r="H15" s="149" t="s">
         <v>14</v>
       </c>
-      <c r="I15" s="151" t="s">
+      <c r="I15" s="149" t="s">
         <v>14</v>
       </c>
-      <c r="J15" s="151" t="s">
+      <c r="J15" s="149" t="s">
         <v>14</v>
       </c>
-      <c r="K15" s="151" t="s">
+      <c r="K15" s="149" t="s">
         <v>14</v>
       </c>
-      <c r="L15" s="151" t="s">
+      <c r="L15" s="149" t="s">
         <v>14</v>
       </c>
-      <c r="M15" s="151" t="s">
+      <c r="M15" s="149" t="s">
         <v>14</v>
       </c>
-      <c r="N15" s="151" t="s">
+      <c r="N15" s="149" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="D16" s="151"/>
-      <c r="E16" s="151"/>
-      <c r="F16" s="151"/>
-      <c r="G16" s="151"/>
-      <c r="H16" s="151"/>
-      <c r="I16" s="151"/>
-      <c r="J16" s="151"/>
-      <c r="K16" s="151"/>
-      <c r="L16" s="151"/>
-      <c r="M16" s="151"/>
-      <c r="N16" s="151"/>
+      <c r="D16" s="149"/>
+      <c r="E16" s="149"/>
+      <c r="F16" s="149"/>
+      <c r="G16" s="149"/>
+      <c r="H16" s="149"/>
+      <c r="I16" s="149"/>
+      <c r="J16" s="149"/>
+      <c r="K16" s="149"/>
+      <c r="L16" s="149"/>
+      <c r="M16" s="149"/>
+      <c r="N16" s="149"/>
     </row>
     <row r="17" spans="3:14" x14ac:dyDescent="0.4">
-      <c r="D17" s="151"/>
-      <c r="E17" s="151"/>
-      <c r="F17" s="151"/>
-      <c r="G17" s="151"/>
-      <c r="H17" s="151"/>
-      <c r="I17" s="151"/>
-      <c r="J17" s="151"/>
-      <c r="K17" s="151"/>
-      <c r="L17" s="151"/>
-      <c r="M17" s="151"/>
-      <c r="N17" s="151"/>
+      <c r="D17" s="149"/>
+      <c r="E17" s="149"/>
+      <c r="F17" s="149"/>
+      <c r="G17" s="149"/>
+      <c r="H17" s="149"/>
+      <c r="I17" s="149"/>
+      <c r="J17" s="149"/>
+      <c r="K17" s="149"/>
+      <c r="L17" s="149"/>
+      <c r="M17" s="149"/>
+      <c r="N17" s="149"/>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.4">
-      <c r="D18" s="151"/>
-      <c r="E18" s="151"/>
-      <c r="F18" s="151"/>
-      <c r="G18" s="151"/>
-      <c r="H18" s="151"/>
-      <c r="I18" s="151"/>
-      <c r="J18" s="151"/>
-      <c r="K18" s="151"/>
-      <c r="L18" s="151"/>
-      <c r="M18" s="151"/>
-      <c r="N18" s="151"/>
+      <c r="D18" s="149"/>
+      <c r="E18" s="149"/>
+      <c r="F18" s="149"/>
+      <c r="G18" s="149"/>
+      <c r="H18" s="149"/>
+      <c r="I18" s="149"/>
+      <c r="J18" s="149"/>
+      <c r="K18" s="149"/>
+      <c r="L18" s="149"/>
+      <c r="M18" s="149"/>
+      <c r="N18" s="149"/>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.4">
-      <c r="D19" s="151"/>
-      <c r="E19" s="151"/>
-      <c r="F19" s="151"/>
-      <c r="G19" s="151"/>
-      <c r="H19" s="151"/>
-      <c r="I19" s="151"/>
-      <c r="J19" s="151"/>
-      <c r="K19" s="151"/>
-      <c r="L19" s="151"/>
-      <c r="M19" s="151"/>
-      <c r="N19" s="151"/>
+      <c r="D19" s="149"/>
+      <c r="E19" s="149"/>
+      <c r="F19" s="149"/>
+      <c r="G19" s="149"/>
+      <c r="H19" s="149"/>
+      <c r="I19" s="149"/>
+      <c r="J19" s="149"/>
+      <c r="K19" s="149"/>
+      <c r="L19" s="149"/>
+      <c r="M19" s="149"/>
+      <c r="N19" s="149"/>
     </row>
     <row r="20" spans="3:14" x14ac:dyDescent="0.4">
-      <c r="D20" s="151"/>
-      <c r="E20" s="151"/>
-      <c r="F20" s="151"/>
-      <c r="G20" s="151"/>
-      <c r="H20" s="151"/>
-      <c r="I20" s="151"/>
-      <c r="J20" s="151"/>
-      <c r="K20" s="151"/>
-      <c r="L20" s="151"/>
-      <c r="M20" s="151"/>
-      <c r="N20" s="151"/>
+      <c r="D20" s="149"/>
+      <c r="E20" s="149"/>
+      <c r="F20" s="149"/>
+      <c r="G20" s="149"/>
+      <c r="H20" s="149"/>
+      <c r="I20" s="149"/>
+      <c r="J20" s="149"/>
+      <c r="K20" s="149"/>
+      <c r="L20" s="149"/>
+      <c r="M20" s="149"/>
+      <c r="N20" s="149"/>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.4">
-      <c r="C23" s="152" t="s">
-        <v>525</v>
-      </c>
-      <c r="D23" s="153" t="s">
-        <v>526</v>
-      </c>
-      <c r="E23" s="192" t="s">
-        <v>527</v>
-      </c>
-      <c r="F23" s="193"/>
+      <c r="C23" s="150" t="s">
+        <v>516</v>
+      </c>
+      <c r="D23" s="151" t="s">
+        <v>517</v>
+      </c>
+      <c r="E23" s="203" t="s">
+        <v>518</v>
+      </c>
+      <c r="F23" s="204"/>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.4">
-      <c r="C24" s="163"/>
-      <c r="D24" s="155" t="s">
-        <v>548</v>
-      </c>
-      <c r="E24" s="194" t="s">
-        <v>549</v>
-      </c>
-      <c r="F24" s="194"/>
+      <c r="C24" s="161"/>
+      <c r="D24" s="153" t="s">
+        <v>539</v>
+      </c>
+      <c r="E24" s="205" t="s">
+        <v>540</v>
+      </c>
+      <c r="F24" s="205"/>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.4">
-      <c r="C25" s="154"/>
-      <c r="D25" s="155">
+      <c r="C25" s="152"/>
+      <c r="D25" s="153">
         <v>0</v>
       </c>
-      <c r="E25" s="195" t="s">
-        <v>550</v>
-      </c>
-      <c r="F25" s="195"/>
+      <c r="E25" s="206" t="s">
+        <v>541</v>
+      </c>
+      <c r="F25" s="206"/>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.4">
-      <c r="C26" s="154"/>
-      <c r="D26" s="156">
+      <c r="C26" s="152"/>
+      <c r="D26" s="154">
         <v>1</v>
       </c>
-      <c r="E26" s="196" t="s">
-        <v>551</v>
-      </c>
-      <c r="F26" s="196"/>
+      <c r="E26" s="207" t="s">
+        <v>542</v>
+      </c>
+      <c r="F26" s="207"/>
     </row>
     <row r="27" spans="3:14" x14ac:dyDescent="0.4">
-      <c r="C27" s="157"/>
-      <c r="D27" s="155">
+      <c r="C27" s="155"/>
+      <c r="D27" s="153">
         <v>2</v>
       </c>
-      <c r="E27" s="195" t="s">
-        <v>552</v>
-      </c>
-      <c r="F27" s="195"/>
+      <c r="E27" s="206" t="s">
+        <v>543</v>
+      </c>
+      <c r="F27" s="206"/>
     </row>
     <row r="29" spans="3:14" x14ac:dyDescent="0.4">
-      <c r="D29" s="161" t="s">
-        <v>542</v>
-      </c>
-      <c r="E29" s="136" t="s">
+      <c r="D29" s="159" t="s">
+        <v>533</v>
+      </c>
+      <c r="E29" s="134" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="30" spans="3:14" x14ac:dyDescent="0.4">
+      <c r="D30" s="160"/>
+      <c r="E30" s="134" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="31" spans="3:14" x14ac:dyDescent="0.4">
+      <c r="E31" s="134" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="32" spans="3:14" x14ac:dyDescent="0.4">
+      <c r="E32" s="134" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.4">
+      <c r="D33" s="160" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="30" spans="3:14" x14ac:dyDescent="0.4">
-      <c r="D30" s="162"/>
-      <c r="E30" s="136" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="31" spans="3:14" x14ac:dyDescent="0.4">
-      <c r="E31" s="136" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="32" spans="3:14" x14ac:dyDescent="0.4">
-      <c r="E32" s="136" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.4">
-      <c r="D33" s="162" t="s">
-        <v>547</v>
-      </c>
-      <c r="E33" s="136" t="s">
-        <v>544</v>
+      <c r="E33" s="134" t="s">
+        <v>535</v>
       </c>
     </row>
     <row r="34" spans="4:5" x14ac:dyDescent="0.4">
-      <c r="D34" s="162" t="s">
-        <v>545</v>
-      </c>
-      <c r="E34" s="136" t="s">
-        <v>546</v>
+      <c r="D34" s="160" t="s">
+        <v>536</v>
+      </c>
+      <c r="E34" s="134" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="40" spans="4:5" x14ac:dyDescent="0.4">
-      <c r="D40" s="158"/>
+      <c r="D40" s="156"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -6759,12 +6795,12 @@
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B39" t="s">
-        <v>504</v>
+        <v>495</v>
       </c>
       <c r="C39" s="16" t="s">
         <v>40</v>
@@ -6774,10 +6810,10 @@
       </c>
     </row>
     <row r="40" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C40" s="128" t="s">
-        <v>407</v>
-      </c>
-      <c r="D40" s="129">
+      <c r="C40" s="126" t="s">
+        <v>398</v>
+      </c>
+      <c r="D40" s="127">
         <v>300</v>
       </c>
     </row>
@@ -9214,13 +9250,13 @@
     </row>
     <row r="35" spans="1:89" x14ac:dyDescent="0.4">
       <c r="C35" s="35" t="s">
-        <v>505</v>
-      </c>
-      <c r="D35" s="130">
+        <v>496</v>
+      </c>
+      <c r="D35" s="128">
         <v>0</v>
       </c>
       <c r="E35" s="35" t="s">
-        <v>506</v>
+        <v>497</v>
       </c>
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
@@ -9309,7 +9345,7 @@
     </row>
     <row r="36" spans="1:89" x14ac:dyDescent="0.4">
       <c r="C36" s="35"/>
-      <c r="D36" s="130">
+      <c r="D36" s="128">
         <v>1</v>
       </c>
       <c r="E36" s="35" t="s">
@@ -9318,101 +9354,101 @@
     </row>
     <row r="37" spans="1:89" x14ac:dyDescent="0.4">
       <c r="C37" s="35"/>
-      <c r="D37" s="130">
+      <c r="D37" s="128">
         <v>101</v>
       </c>
       <c r="E37" s="35" t="s">
-        <v>507</v>
+        <v>498</v>
       </c>
     </row>
     <row r="38" spans="1:89" x14ac:dyDescent="0.4">
       <c r="C38" s="35"/>
-      <c r="D38" s="130">
+      <c r="D38" s="128">
         <v>103</v>
       </c>
       <c r="E38" s="35" t="s">
-        <v>508</v>
+        <v>499</v>
       </c>
     </row>
     <row r="39" spans="1:89" x14ac:dyDescent="0.4">
       <c r="C39" s="35"/>
-      <c r="D39" s="130">
+      <c r="D39" s="128">
         <v>107</v>
       </c>
       <c r="E39" s="35" t="s">
-        <v>509</v>
+        <v>500</v>
       </c>
     </row>
     <row r="40" spans="1:89" x14ac:dyDescent="0.4">
       <c r="C40" s="35"/>
-      <c r="D40" s="130">
+      <c r="D40" s="128">
         <v>121</v>
       </c>
       <c r="E40" s="35" t="s">
-        <v>510</v>
+        <v>501</v>
       </c>
     </row>
     <row r="41" spans="1:89" x14ac:dyDescent="0.4">
       <c r="C41" s="35"/>
-      <c r="D41" s="130">
+      <c r="D41" s="128">
         <v>144</v>
       </c>
       <c r="E41" s="35" t="s">
-        <v>511</v>
+        <v>502</v>
       </c>
     </row>
     <row r="42" spans="1:89" x14ac:dyDescent="0.4">
       <c r="C42" s="35"/>
-      <c r="D42" s="130">
+      <c r="D42" s="128">
         <v>145</v>
       </c>
       <c r="E42" s="35" t="s">
-        <v>512</v>
+        <v>503</v>
       </c>
     </row>
     <row r="43" spans="1:89" x14ac:dyDescent="0.4">
       <c r="C43" s="35"/>
-      <c r="D43" s="130">
+      <c r="D43" s="128">
         <v>154</v>
       </c>
       <c r="E43" s="35" t="s">
-        <v>513</v>
+        <v>504</v>
       </c>
     </row>
     <row r="44" spans="1:89" x14ac:dyDescent="0.4">
       <c r="C44" s="35"/>
-      <c r="D44" s="130">
+      <c r="D44" s="128">
         <v>155</v>
       </c>
       <c r="E44" s="35" t="s">
-        <v>514</v>
+        <v>505</v>
       </c>
     </row>
     <row r="45" spans="1:89" x14ac:dyDescent="0.4">
       <c r="C45" s="35"/>
-      <c r="D45" s="130">
+      <c r="D45" s="128">
         <v>171</v>
       </c>
       <c r="E45" s="35" t="s">
-        <v>515</v>
+        <v>506</v>
       </c>
     </row>
     <row r="46" spans="1:89" x14ac:dyDescent="0.4">
       <c r="C46" s="35"/>
-      <c r="D46" s="130">
+      <c r="D46" s="128">
         <v>901</v>
       </c>
       <c r="E46" s="35" t="s">
-        <v>516</v>
+        <v>507</v>
       </c>
     </row>
     <row r="47" spans="1:89" x14ac:dyDescent="0.4">
       <c r="C47" s="7"/>
-      <c r="D47" s="131">
+      <c r="D47" s="129">
         <v>907</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>517</v>
+        <v>508</v>
       </c>
     </row>
   </sheetData>
@@ -9492,8 +9528,8 @@
       <c r="D7" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="E7" s="100" t="s">
-        <v>389</v>
+      <c r="E7" s="98" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.4">
@@ -9519,10 +9555,10 @@
         <v>268</v>
       </c>
       <c r="G10" s="34" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
       <c r="H10" s="34" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.4">
@@ -9539,7 +9575,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="26" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.4">
@@ -9556,7 +9592,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="26" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.4">
@@ -9568,7 +9604,7 @@
         <v>196</v>
       </c>
       <c r="H13" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.4">
@@ -9625,7 +9661,7 @@
         <v>198</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.4">
@@ -9827,7 +9863,7 @@
       </c>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="B28" s="101" t="s">
+      <c r="B28" s="99" t="s">
         <v>311</v>
       </c>
     </row>
@@ -10000,89 +10036,89 @@
       <c r="C11" s="72" t="s">
         <v>305</v>
       </c>
-      <c r="D11" s="172" t="s">
+      <c r="D11" s="174" t="s">
         <v>299</v>
       </c>
-      <c r="E11" s="173"/>
-      <c r="F11" s="172" t="s">
+      <c r="E11" s="175"/>
+      <c r="F11" s="174" t="s">
         <v>300</v>
       </c>
-      <c r="G11" s="173"/>
+      <c r="G11" s="175"/>
       <c r="L11" t="s">
-        <v>519</v>
+        <v>510</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B12" s="188" t="s">
+      <c r="B12" s="190" t="s">
         <v>279</v>
       </c>
       <c r="C12" s="48">
         <v>0</v>
       </c>
-      <c r="D12" s="184" t="s">
+      <c r="D12" s="186" t="s">
         <v>203</v>
       </c>
-      <c r="E12" s="185"/>
-      <c r="F12" s="174" t="s">
+      <c r="E12" s="187"/>
+      <c r="F12" s="176" t="s">
         <v>301</v>
       </c>
-      <c r="G12" s="175"/>
+      <c r="G12" s="177"/>
       <c r="L12" t="s">
-        <v>520</v>
+        <v>511</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B13" s="188"/>
+      <c r="B13" s="190"/>
       <c r="C13" s="48">
         <v>1</v>
       </c>
-      <c r="D13" s="184" t="s">
+      <c r="D13" s="186" t="s">
         <v>202</v>
       </c>
-      <c r="E13" s="185"/>
-      <c r="F13" s="176" t="s">
+      <c r="E13" s="187"/>
+      <c r="F13" s="178" t="s">
         <v>308</v>
       </c>
-      <c r="G13" s="177"/>
+      <c r="G13" s="179"/>
       <c r="L13" t="s">
-        <v>521</v>
+        <v>512</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B14" s="188"/>
+      <c r="B14" s="190"/>
       <c r="C14" s="48">
         <v>2</v>
       </c>
-      <c r="D14" s="184" t="s">
+      <c r="D14" s="186" t="s">
         <v>201</v>
       </c>
-      <c r="E14" s="185"/>
-      <c r="F14" s="176"/>
-      <c r="G14" s="177"/>
+      <c r="E14" s="187"/>
+      <c r="F14" s="178"/>
+      <c r="G14" s="179"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B15" s="188"/>
+      <c r="B15" s="190"/>
       <c r="C15" s="49">
         <v>3</v>
       </c>
-      <c r="D15" s="184" t="s">
+      <c r="D15" s="186" t="s">
         <v>266</v>
       </c>
-      <c r="E15" s="185"/>
-      <c r="F15" s="176"/>
-      <c r="G15" s="177"/>
+      <c r="E15" s="187"/>
+      <c r="F15" s="178"/>
+      <c r="G15" s="179"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B16" s="188"/>
+      <c r="B16" s="190"/>
       <c r="C16" s="49">
         <v>4</v>
       </c>
-      <c r="D16" s="184" t="s">
+      <c r="D16" s="186" t="s">
         <v>267</v>
       </c>
-      <c r="E16" s="185"/>
-      <c r="F16" s="178"/>
-      <c r="G16" s="179"/>
+      <c r="E16" s="187"/>
+      <c r="F16" s="180"/>
+      <c r="G16" s="181"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B17" s="65" t="s">
@@ -10137,30 +10173,30 @@
       <c r="G20" s="69"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B21" s="186" t="s">
+      <c r="B21" s="188" t="s">
         <v>288</v>
       </c>
       <c r="C21" s="48" t="b">
         <v>1</v>
       </c>
-      <c r="D21" s="184" t="s">
+      <c r="D21" s="186" t="s">
         <v>306</v>
       </c>
-      <c r="E21" s="185"/>
+      <c r="E21" s="187"/>
       <c r="F21" s="73" t="s">
         <v>301</v>
       </c>
       <c r="G21" s="74"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B22" s="186"/>
+      <c r="B22" s="188"/>
       <c r="C22" s="48" t="b">
         <v>0</v>
       </c>
-      <c r="D22" s="184" t="s">
+      <c r="D22" s="186" t="s">
         <v>307</v>
       </c>
-      <c r="E22" s="185"/>
+      <c r="E22" s="187"/>
       <c r="F22" s="75" t="s">
         <v>309</v>
       </c>
@@ -10183,130 +10219,130 @@
       <c r="G23" s="71"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B24" s="186" t="s">
+      <c r="B24" s="188" t="s">
         <v>291</v>
       </c>
       <c r="C24" s="47">
         <v>1</v>
       </c>
-      <c r="D24" s="182" t="s">
+      <c r="D24" s="184" t="s">
         <v>289</v>
       </c>
-      <c r="E24" s="183"/>
-      <c r="F24" s="180" t="s">
+      <c r="E24" s="185"/>
+      <c r="F24" s="182" t="s">
         <v>301</v>
       </c>
-      <c r="G24" s="181"/>
+      <c r="G24" s="183"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B25" s="186"/>
+      <c r="B25" s="188"/>
       <c r="C25" s="47">
         <v>2</v>
       </c>
-      <c r="D25" s="170" t="s">
+      <c r="D25" s="172" t="s">
         <v>280</v>
       </c>
-      <c r="E25" s="171"/>
-      <c r="F25" s="164" t="s">
+      <c r="E25" s="173"/>
+      <c r="F25" s="166" t="s">
         <v>308</v>
       </c>
-      <c r="G25" s="165"/>
+      <c r="G25" s="167"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B26" s="186"/>
+      <c r="B26" s="188"/>
       <c r="C26" s="47">
         <v>3</v>
       </c>
-      <c r="D26" s="170" t="s">
+      <c r="D26" s="172" t="s">
         <v>281</v>
       </c>
-      <c r="E26" s="171"/>
-      <c r="F26" s="164"/>
-      <c r="G26" s="165"/>
+      <c r="E26" s="173"/>
+      <c r="F26" s="166"/>
+      <c r="G26" s="167"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B27" s="186"/>
+      <c r="B27" s="188"/>
       <c r="C27" s="47">
         <v>4</v>
       </c>
-      <c r="D27" s="170" t="s">
+      <c r="D27" s="172" t="s">
         <v>282</v>
       </c>
-      <c r="E27" s="171"/>
-      <c r="F27" s="164"/>
-      <c r="G27" s="165"/>
+      <c r="E27" s="173"/>
+      <c r="F27" s="166"/>
+      <c r="G27" s="167"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B28" s="186"/>
+      <c r="B28" s="188"/>
       <c r="C28" s="47">
         <v>5</v>
       </c>
-      <c r="D28" s="170" t="s">
+      <c r="D28" s="172" t="s">
         <v>283</v>
       </c>
-      <c r="E28" s="171"/>
-      <c r="F28" s="168"/>
-      <c r="G28" s="169"/>
+      <c r="E28" s="173"/>
+      <c r="F28" s="170"/>
+      <c r="G28" s="171"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B29" s="186" t="s">
+      <c r="B29" s="188" t="s">
         <v>292</v>
       </c>
       <c r="C29" s="47">
         <v>1</v>
       </c>
-      <c r="D29" s="182" t="s">
+      <c r="D29" s="184" t="s">
         <v>290</v>
       </c>
-      <c r="E29" s="183"/>
-      <c r="F29" s="180" t="s">
+      <c r="E29" s="185"/>
+      <c r="F29" s="182" t="s">
         <v>301</v>
       </c>
-      <c r="G29" s="181"/>
+      <c r="G29" s="183"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B30" s="186"/>
+      <c r="B30" s="188"/>
       <c r="C30" s="47">
         <v>2</v>
       </c>
-      <c r="D30" s="170" t="s">
+      <c r="D30" s="172" t="s">
         <v>284</v>
       </c>
-      <c r="E30" s="171"/>
-      <c r="F30" s="164" t="s">
+      <c r="E30" s="173"/>
+      <c r="F30" s="166" t="s">
         <v>308</v>
       </c>
-      <c r="G30" s="165"/>
+      <c r="G30" s="167"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B31" s="187" t="s">
+      <c r="B31" s="189" t="s">
         <v>293</v>
       </c>
       <c r="C31" s="47">
         <v>2</v>
       </c>
-      <c r="D31" s="170" t="s">
+      <c r="D31" s="172" t="s">
         <v>285</v>
       </c>
-      <c r="E31" s="171"/>
-      <c r="F31" s="166" t="s">
+      <c r="E31" s="173"/>
+      <c r="F31" s="168" t="s">
         <v>301</v>
       </c>
-      <c r="G31" s="167"/>
+      <c r="G31" s="169"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B32" s="187"/>
+      <c r="B32" s="189"/>
       <c r="C32" s="47">
         <v>3</v>
       </c>
-      <c r="D32" s="170" t="s">
+      <c r="D32" s="172" t="s">
         <v>286</v>
       </c>
-      <c r="E32" s="171"/>
-      <c r="F32" s="168" t="s">
+      <c r="E32" s="173"/>
+      <c r="F32" s="170" t="s">
         <v>308</v>
       </c>
-      <c r="G32" s="169"/>
+      <c r="G32" s="171"/>
     </row>
     <row r="33" spans="1:37" x14ac:dyDescent="0.4">
       <c r="B33" s="6"/>
@@ -10411,7 +10447,7 @@
         <v>129</v>
       </c>
       <c r="W39" s="8" t="s">
-        <v>518</v>
+        <v>509</v>
       </c>
       <c r="X39" s="8" t="s">
         <v>130</v>
@@ -10520,7 +10556,7 @@
         <v>85</v>
       </c>
       <c r="W40" s="7" t="s">
-        <v>522</v>
+        <v>513</v>
       </c>
       <c r="X40" s="7" t="s">
         <v>85</v>
@@ -10820,7 +10856,7 @@
         <v>85</v>
       </c>
       <c r="W44" s="7" t="s">
-        <v>522</v>
+        <v>513</v>
       </c>
       <c r="X44" s="7" t="s">
         <v>85</v>
@@ -21308,11 +21344,11 @@
       <c r="D7" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="102" t="s">
+      <c r="E7" s="100" t="s">
         <v>292</v>
       </c>
-      <c r="F7" s="102" t="s">
-        <v>389</v>
+      <c r="F7" s="100" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.4">
@@ -21341,13 +21377,13 @@
         <v>292</v>
       </c>
       <c r="G10" s="34" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="I10" s="34" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
       <c r="J10" s="34" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.4">
@@ -21361,13 +21397,13 @@
         <v>1</v>
       </c>
       <c r="G11" s="26" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
       <c r="I11" s="26" t="b">
         <v>1</v>
       </c>
       <c r="J11" s="26" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.4">
@@ -21387,7 +21423,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="26" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.4">
@@ -21398,7 +21434,7 @@
         <v>201</v>
       </c>
       <c r="J13" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.4">
@@ -21431,7 +21467,7 @@
         <v>10</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.4">
@@ -21745,7 +21781,7 @@
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="B28" s="101" t="s">
+      <c r="B28" s="99" t="s">
         <v>311</v>
       </c>
     </row>
@@ -22134,7 +22170,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T64"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -22160,40 +22196,40 @@
     <col min="25" max="16384" width="9" style="82"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="79" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="D2" s="80"/>
       <c r="E2" s="80"/>
       <c r="F2" s="81"/>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="79" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="D3" s="80"/>
       <c r="E3" s="80"/>
       <c r="F3" s="81"/>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B5" s="83" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B6" s="84"/>
       <c r="C6" s="84" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.4">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B7" s="84"/>
       <c r="C7" s="42" t="s">
         <v>312</v>
@@ -22202,37 +22238,37 @@
         <v>313</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B8" s="84"/>
-      <c r="C8" s="98">
+      <c r="C8" s="97">
         <v>1</v>
       </c>
-      <c r="D8" s="98" t="s">
+      <c r="D8" s="97" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.4">
       <c r="C10" s="72" t="s">
         <v>352</v>
       </c>
-      <c r="D10" s="189" t="s">
+      <c r="D10" s="191" t="s">
         <v>268</v>
       </c>
-      <c r="E10" s="190"/>
+      <c r="E10" s="192"/>
       <c r="H10" s="72" t="s">
         <v>352</v>
       </c>
-      <c r="I10" s="189" t="s">
+      <c r="I10" s="191" t="s">
         <v>268</v>
       </c>
-      <c r="J10" s="190"/>
-      <c r="K10" s="191" t="s">
+      <c r="J10" s="192"/>
+      <c r="K10" s="193" t="s">
         <v>300</v>
       </c>
-      <c r="L10" s="191"/>
-      <c r="M10" s="191"/>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="L10" s="193"/>
+      <c r="M10" s="193"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B11" s="90" t="s">
         <v>315</v>
       </c>
@@ -22246,18 +22282,20 @@
       <c r="G11" s="96" t="s">
         <v>316</v>
       </c>
-      <c r="H11" s="97" t="s">
+      <c r="H11" s="163" t="s">
         <v>314</v>
       </c>
       <c r="I11" s="92" t="s">
         <v>368</v>
       </c>
       <c r="J11" s="81"/>
-      <c r="K11" s="92"/>
-      <c r="L11" s="80"/>
-      <c r="M11" s="81"/>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="K11" s="194" t="s">
+        <v>550</v>
+      </c>
+      <c r="L11" s="195"/>
+      <c r="M11" s="196"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B12" s="93"/>
       <c r="C12" s="91">
         <v>2</v>
@@ -22267,18 +22305,18 @@
       </c>
       <c r="E12" s="81"/>
       <c r="G12" s="94"/>
-      <c r="H12" s="97" t="s">
+      <c r="H12" s="163" t="s">
         <v>369</v>
       </c>
       <c r="I12" s="92" t="s">
         <v>370</v>
       </c>
       <c r="J12" s="81"/>
-      <c r="K12" s="92"/>
-      <c r="L12" s="80"/>
-      <c r="M12" s="81"/>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="K12" s="197"/>
+      <c r="L12" s="198"/>
+      <c r="M12" s="199"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B13" s="93"/>
       <c r="C13" s="91">
         <v>3</v>
@@ -22288,20 +22326,19 @@
       </c>
       <c r="E13" s="81"/>
       <c r="G13" s="94"/>
-      <c r="H13" s="97" t="s">
-        <v>371</v>
-      </c>
-      <c r="I13" s="92" t="s">
-        <v>372</v>
+      <c r="H13" s="164" t="s">
+        <v>544</v>
+      </c>
+      <c r="I13" s="165" t="s">
+        <v>547</v>
       </c>
       <c r="J13" s="81"/>
-      <c r="K13" s="99" t="s">
-        <v>388</v>
-      </c>
-      <c r="L13" s="80"/>
-      <c r="M13" s="81"/>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="K13" s="197"/>
+      <c r="L13" s="198"/>
+      <c r="M13" s="199"/>
+      <c r="N13" s="162"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B14" s="93"/>
       <c r="C14" s="91">
         <v>4</v>
@@ -22311,20 +22348,19 @@
       </c>
       <c r="E14" s="81"/>
       <c r="G14" s="94"/>
-      <c r="H14" s="97" t="s">
-        <v>373</v>
-      </c>
-      <c r="I14" s="92" t="s">
-        <v>374</v>
+      <c r="H14" s="164" t="s">
+        <v>545</v>
+      </c>
+      <c r="I14" s="165" t="s">
+        <v>548</v>
       </c>
       <c r="J14" s="81"/>
-      <c r="K14" s="99" t="s">
-        <v>388</v>
-      </c>
-      <c r="L14" s="80"/>
-      <c r="M14" s="81"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="K14" s="197"/>
+      <c r="L14" s="198"/>
+      <c r="M14" s="199"/>
+      <c r="N14" s="162"/>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B15" s="93"/>
       <c r="C15" s="91">
         <v>5</v>
@@ -22334,18 +22370,19 @@
       </c>
       <c r="E15" s="81"/>
       <c r="G15" s="94"/>
-      <c r="H15" s="97" t="s">
-        <v>375</v>
-      </c>
-      <c r="I15" s="92" t="s">
-        <v>376</v>
+      <c r="H15" s="164" t="s">
+        <v>546</v>
+      </c>
+      <c r="I15" s="165" t="s">
+        <v>549</v>
       </c>
       <c r="J15" s="81"/>
-      <c r="K15" s="92"/>
-      <c r="L15" s="80"/>
-      <c r="M15" s="81"/>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="K15" s="197"/>
+      <c r="L15" s="198"/>
+      <c r="M15" s="199"/>
+      <c r="N15" s="162"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B16" s="93"/>
       <c r="C16" s="91">
         <v>6</v>
@@ -22355,16 +22392,16 @@
       </c>
       <c r="E16" s="81"/>
       <c r="G16" s="94"/>
-      <c r="H16" s="97" t="s">
-        <v>377</v>
+      <c r="H16" s="163" t="s">
+        <v>371</v>
       </c>
       <c r="I16" s="92" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="J16" s="81"/>
-      <c r="K16" s="92"/>
-      <c r="L16" s="80"/>
-      <c r="M16" s="81"/>
+      <c r="K16" s="197"/>
+      <c r="L16" s="198"/>
+      <c r="M16" s="199"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B17" s="93"/>
@@ -22376,16 +22413,16 @@
       </c>
       <c r="E17" s="81"/>
       <c r="G17" s="94"/>
-      <c r="H17" s="97" t="s">
-        <v>379</v>
+      <c r="H17" s="163" t="s">
+        <v>373</v>
       </c>
       <c r="I17" s="92" t="s">
-        <v>380</v>
+        <v>196</v>
       </c>
       <c r="J17" s="81"/>
-      <c r="K17" s="92"/>
-      <c r="L17" s="80"/>
-      <c r="M17" s="81"/>
+      <c r="K17" s="197"/>
+      <c r="L17" s="198"/>
+      <c r="M17" s="199"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B18" s="93"/>
@@ -22396,17 +22433,17 @@
         <v>360</v>
       </c>
       <c r="E18" s="81"/>
-      <c r="G18" s="94"/>
-      <c r="H18" s="97" t="s">
-        <v>381</v>
+      <c r="G18" s="95"/>
+      <c r="H18" s="163" t="s">
+        <v>374</v>
       </c>
       <c r="I18" s="92" t="s">
-        <v>196</v>
+        <v>375</v>
       </c>
       <c r="J18" s="81"/>
-      <c r="K18" s="92"/>
-      <c r="L18" s="80"/>
-      <c r="M18" s="81"/>
+      <c r="K18" s="200"/>
+      <c r="L18" s="201"/>
+      <c r="M18" s="202"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B19" s="94"/>
@@ -22417,17 +22454,7 @@
         <v>361</v>
       </c>
       <c r="E19" s="81"/>
-      <c r="G19" s="95"/>
-      <c r="H19" s="97" t="s">
-        <v>382</v>
-      </c>
-      <c r="I19" s="92" t="s">
-        <v>383</v>
-      </c>
-      <c r="J19" s="81"/>
-      <c r="K19" s="92"/>
-      <c r="L19" s="80"/>
-      <c r="M19" s="81"/>
+      <c r="G19" s="88"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.4">
       <c r="B20" s="94"/>
@@ -22502,7 +22529,7 @@
         <v>198</v>
       </c>
       <c r="D30" s="89" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.4">
@@ -23619,20 +23646,22 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="I10:J10"/>
     <mergeCell ref="K10:M10"/>
+    <mergeCell ref="K11:M18"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8">
       <formula1>$C$11:$C$25</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8">
-      <formula1>$H$11:$H$19</formula1>
+      <formula1>$H$11:$H$18</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated files for ver5.22.0
</commit_message>
<xml_diff>
--- a/sample/ExcelMacro/kabuSTATION_API_function_sample.xlsx
+++ b/sample/ExcelMacro/kabuSTATION_API_function_sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tw.hosokawa\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\06.VaR対応、東証マザーズ指数名変更\kabusapi\sample\ExcelMacro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718A666F-301F-468A-93D6-4C6AD99187E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7293E6D5-4306-4476-90FF-1EDA877D403B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="787" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="787" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="注文取消" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1666" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1666" uniqueCount="577">
   <si>
     <t>概要</t>
     <rPh sb="0" eb="2">
@@ -1369,12 +1369,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>MOTHERS</t>
-  </si>
-  <si>
-    <t>東証マザーズ先物</t>
-  </si>
-  <si>
     <t>JPX400</t>
   </si>
   <si>
@@ -2749,9 +2743,6 @@
     <t>日経平均VI</t>
   </si>
   <si>
-    <t>東証マザーズ指数先物</t>
-  </si>
-  <si>
     <t>TOPIX_REIT</t>
   </si>
   <si>
@@ -3206,6 +3197,14 @@
   </si>
   <si>
     <t>=SYMBOLNAME.OPTION(C8,D8,E8,F8)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>GROWTH</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>グロース250先物</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -4399,7 +4398,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B2:I19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -4567,7 +4566,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B2:T64"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -4598,7 +4599,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="72" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D2" s="73"/>
       <c r="E2" s="73"/>
@@ -4609,7 +4610,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="72" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D3" s="73"/>
       <c r="E3" s="73"/>
@@ -4623,16 +4624,16 @@
     <row r="6" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B6" s="44"/>
       <c r="C6" s="44" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B7" s="44"/>
       <c r="C7" s="37" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.4">
@@ -4641,53 +4642,53 @@
         <v>1</v>
       </c>
       <c r="D8" s="87" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.4">
       <c r="C10" s="65" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D10" s="172" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E10" s="173"/>
       <c r="H10" s="65" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="I10" s="172" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="J10" s="173"/>
       <c r="K10" s="174" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="L10" s="174"/>
       <c r="M10" s="174"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B11" s="80" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C11" s="81">
         <v>1</v>
       </c>
       <c r="D11" s="82" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E11" s="74"/>
       <c r="G11" s="86" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H11" s="142" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="I11" s="82" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="J11" s="74"/>
       <c r="K11" s="175" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="L11" s="176"/>
       <c r="M11" s="177"/>
@@ -4698,15 +4699,15 @@
         <v>2</v>
       </c>
       <c r="D12" s="82" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E12" s="74"/>
       <c r="G12" s="84"/>
       <c r="H12" s="142" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="I12" s="82" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="J12" s="74"/>
       <c r="K12" s="178"/>
@@ -4719,15 +4720,15 @@
         <v>3</v>
       </c>
       <c r="D13" s="82" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E13" s="74"/>
       <c r="G13" s="84"/>
       <c r="H13" s="143" t="s">
+        <v>540</v>
+      </c>
+      <c r="I13" s="144" t="s">
         <v>543</v>
-      </c>
-      <c r="I13" s="144" t="s">
-        <v>546</v>
       </c>
       <c r="J13" s="74"/>
       <c r="K13" s="178"/>
@@ -4741,15 +4742,15 @@
         <v>4</v>
       </c>
       <c r="D14" s="82" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E14" s="74"/>
       <c r="G14" s="84"/>
       <c r="H14" s="143" t="s">
+        <v>541</v>
+      </c>
+      <c r="I14" s="144" t="s">
         <v>544</v>
-      </c>
-      <c r="I14" s="144" t="s">
-        <v>547</v>
       </c>
       <c r="J14" s="74"/>
       <c r="K14" s="178"/>
@@ -4763,15 +4764,15 @@
         <v>5</v>
       </c>
       <c r="D15" s="82" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E15" s="74"/>
       <c r="G15" s="84"/>
       <c r="H15" s="143" t="s">
+        <v>542</v>
+      </c>
+      <c r="I15" s="144" t="s">
         <v>545</v>
-      </c>
-      <c r="I15" s="144" t="s">
-        <v>548</v>
       </c>
       <c r="J15" s="74"/>
       <c r="K15" s="178"/>
@@ -4785,15 +4786,15 @@
         <v>6</v>
       </c>
       <c r="D16" s="82" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E16" s="74"/>
       <c r="G16" s="84"/>
       <c r="H16" s="142" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="I16" s="82" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J16" s="74"/>
       <c r="K16" s="178"/>
@@ -4806,12 +4807,12 @@
         <v>7</v>
       </c>
       <c r="D17" s="82" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E17" s="74"/>
       <c r="G17" s="84"/>
       <c r="H17" s="142" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="I17" s="82" t="s">
         <v>196</v>
@@ -4827,15 +4828,15 @@
         <v>8</v>
       </c>
       <c r="D18" s="82" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E18" s="74"/>
       <c r="G18" s="85"/>
       <c r="H18" s="142" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="I18" s="82" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="J18" s="74"/>
       <c r="K18" s="181"/>
@@ -4848,7 +4849,7 @@
         <v>9</v>
       </c>
       <c r="D19" s="82" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E19" s="74"/>
       <c r="G19" s="78"/>
@@ -4859,7 +4860,7 @@
         <v>10</v>
       </c>
       <c r="D20" s="82" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E20" s="74"/>
     </row>
@@ -4869,7 +4870,7 @@
         <v>11</v>
       </c>
       <c r="D21" s="82" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E21" s="74"/>
     </row>
@@ -4879,7 +4880,7 @@
         <v>12</v>
       </c>
       <c r="D22" s="82" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E22" s="74"/>
     </row>
@@ -4889,7 +4890,7 @@
         <v>13</v>
       </c>
       <c r="D23" s="82" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E23" s="74"/>
     </row>
@@ -4899,7 +4900,7 @@
         <v>14</v>
       </c>
       <c r="D24" s="82" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E24" s="74"/>
     </row>
@@ -4909,7 +4910,7 @@
         <v>15</v>
       </c>
       <c r="D25" s="82" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E25" s="74"/>
     </row>
@@ -4926,7 +4927,7 @@
         <v>198</v>
       </c>
       <c r="D30" s="79" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.4">
@@ -4934,49 +4935,49 @@
         <v>12</v>
       </c>
       <c r="D31" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="F31" s="8" t="s">
         <v>315</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="G31" s="8" t="s">
         <v>316</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="H31" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="G31" s="8" t="s">
+      <c r="I31" s="8" t="s">
         <v>318</v>
       </c>
-      <c r="H31" s="8" t="s">
+      <c r="J31" s="8" t="s">
         <v>319</v>
       </c>
-      <c r="I31" s="8" t="s">
+      <c r="K31" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="J31" s="8" t="s">
+      <c r="L31" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="K31" s="8" t="s">
+      <c r="M31" s="8" t="s">
         <v>322</v>
       </c>
-      <c r="L31" s="8" t="s">
+      <c r="N31" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="M31" s="8" t="s">
+      <c r="O31" s="8" t="s">
         <v>324</v>
       </c>
-      <c r="N31" s="8" t="s">
+      <c r="P31" s="8" t="s">
         <v>325</v>
       </c>
-      <c r="O31" s="8" t="s">
+      <c r="Q31" s="8" t="s">
         <v>326</v>
       </c>
-      <c r="P31" s="8" t="s">
+      <c r="R31" s="8" t="s">
         <v>327</v>
-      </c>
-      <c r="Q31" s="8" t="s">
-        <v>328</v>
-      </c>
-      <c r="R31" s="8" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.4">
@@ -4985,46 +4986,46 @@
         <v>(D32に関数入力)</v>
       </c>
       <c r="D32" s="76" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E32" s="77" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F32" s="71">
         <v>1</v>
       </c>
       <c r="G32" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H32" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="I32" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J32" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="K32" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L32" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="M32" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="N32" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="O32" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="P32" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="Q32" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="R32" s="71" t="s">
         <v>14</v>
@@ -5035,37 +5036,37 @@
         <v>2</v>
       </c>
       <c r="G33" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H33" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="I33" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J33" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="K33" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L33" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="M33" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="N33" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="O33" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="P33" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="Q33" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="R33" s="71" t="s">
         <v>14</v>
@@ -5076,37 +5077,37 @@
         <v>3</v>
       </c>
       <c r="G34" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H34" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="I34" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J34" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="K34" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L34" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="M34" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="N34" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="O34" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="P34" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="Q34" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="R34" s="71" t="s">
         <v>14</v>
@@ -5120,7 +5121,7 @@
         <v>198</v>
       </c>
       <c r="D36" s="79" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="G36" s="78"/>
     </row>
@@ -5129,43 +5130,43 @@
         <v>12</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E37" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="J37" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="K37" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="L37" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="M37" s="8" t="s">
         <v>332</v>
       </c>
-      <c r="F37" s="8" t="s">
+      <c r="N37" s="8" t="s">
         <v>333</v>
       </c>
-      <c r="G37" s="8" t="s">
-        <v>318</v>
-      </c>
-      <c r="H37" s="8" t="s">
-        <v>319</v>
-      </c>
-      <c r="I37" s="8" t="s">
-        <v>320</v>
-      </c>
-      <c r="J37" s="8" t="s">
-        <v>321</v>
-      </c>
-      <c r="K37" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="L37" s="8" t="s">
-        <v>323</v>
-      </c>
-      <c r="M37" s="8" t="s">
+      <c r="O37" s="8" t="s">
         <v>334</v>
       </c>
-      <c r="N37" s="8" t="s">
+      <c r="P37" s="8" t="s">
         <v>335</v>
-      </c>
-      <c r="O37" s="8" t="s">
-        <v>336</v>
-      </c>
-      <c r="P37" s="8" t="s">
-        <v>337</v>
       </c>
       <c r="Q37" s="8" t="s">
         <v>58</v>
@@ -5177,7 +5178,7 @@
         <v>148</v>
       </c>
       <c r="T37" s="8" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="38" spans="3:20" x14ac:dyDescent="0.4">
@@ -5186,46 +5187,46 @@
         <v>(D38に関数入力)</v>
       </c>
       <c r="D38" s="76" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E38" s="77" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F38" s="71">
         <v>1</v>
       </c>
       <c r="G38" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H38" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="I38" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J38" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="K38" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L38" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="M38" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="N38" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="O38" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="P38" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="Q38" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="R38" s="71" t="s">
         <v>14</v>
@@ -5242,37 +5243,37 @@
         <v>2</v>
       </c>
       <c r="G39" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H39" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="I39" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J39" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="K39" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L39" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="M39" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="N39" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="O39" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="P39" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="Q39" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="R39" s="71" t="s">
         <v>14</v>
@@ -5289,37 +5290,37 @@
         <v>3</v>
       </c>
       <c r="G40" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H40" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="I40" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J40" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="K40" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L40" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="M40" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="N40" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="O40" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="P40" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="Q40" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="R40" s="71" t="s">
         <v>14</v>
@@ -5336,7 +5337,7 @@
         <v>198</v>
       </c>
       <c r="D42" s="79" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="G42" s="78"/>
     </row>
@@ -5345,49 +5346,49 @@
         <v>12</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G43" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="H43" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="I43" s="8" t="s">
         <v>318</v>
       </c>
-      <c r="H43" s="8" t="s">
+      <c r="J43" s="8" t="s">
         <v>319</v>
       </c>
-      <c r="I43" s="8" t="s">
+      <c r="K43" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="J43" s="8" t="s">
+      <c r="L43" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="K43" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="L43" s="8" t="s">
-        <v>323</v>
-      </c>
       <c r="M43" s="8" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="N43" s="8" t="s">
         <v>58</v>
       </c>
       <c r="O43" s="8" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="P43" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="Q43" s="8" t="s">
         <v>148</v>
       </c>
       <c r="R43" s="8" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="44" spans="3:20" x14ac:dyDescent="0.4">
@@ -5396,46 +5397,46 @@
         <v>(D44に関数入力)</v>
       </c>
       <c r="D44" s="76" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E44" s="77" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F44" s="71">
         <v>1</v>
       </c>
       <c r="G44" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H44" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="I44" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J44" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="K44" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L44" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="M44" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="N44" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="O44" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="P44" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="Q44" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="R44" s="71" t="s">
         <v>14</v>
@@ -5446,37 +5447,37 @@
         <v>2</v>
       </c>
       <c r="G45" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H45" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="I45" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J45" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="K45" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L45" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="M45" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="N45" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="O45" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="P45" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="Q45" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="R45" s="71" t="s">
         <v>14</v>
@@ -5487,37 +5488,37 @@
         <v>3</v>
       </c>
       <c r="G46" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H46" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="I46" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J46" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="K46" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L46" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="M46" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="N46" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="O46" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="P46" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="Q46" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="R46" s="71" t="s">
         <v>14</v>
@@ -5528,7 +5529,7 @@
         <v>198</v>
       </c>
       <c r="D48" s="79" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="G48" s="78"/>
     </row>
@@ -5537,49 +5538,49 @@
         <v>12</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G49" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="H49" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="I49" s="8" t="s">
         <v>318</v>
       </c>
-      <c r="H49" s="8" t="s">
+      <c r="J49" s="8" t="s">
         <v>319</v>
       </c>
-      <c r="I49" s="8" t="s">
+      <c r="K49" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="J49" s="8" t="s">
+      <c r="L49" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="K49" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="L49" s="8" t="s">
-        <v>323</v>
-      </c>
       <c r="M49" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="N49" s="8" t="s">
         <v>61</v>
       </c>
       <c r="O49" s="8" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="P49" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="Q49" s="8" t="s">
         <v>148</v>
       </c>
       <c r="R49" s="8" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="50" spans="3:18" x14ac:dyDescent="0.4">
@@ -5588,46 +5589,46 @@
         <v>(D50に関数入力)</v>
       </c>
       <c r="D50" s="76" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E50" s="77" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F50" s="71">
         <v>1</v>
       </c>
       <c r="G50" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H50" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="I50" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J50" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="K50" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L50" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="M50" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="N50" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="O50" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="P50" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="Q50" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="R50" s="71" t="s">
         <v>14</v>
@@ -5638,37 +5639,37 @@
         <v>2</v>
       </c>
       <c r="G51" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H51" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="I51" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J51" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="K51" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L51" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="M51" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="N51" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="O51" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="P51" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="Q51" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="R51" s="71" t="s">
         <v>14</v>
@@ -5679,37 +5680,37 @@
         <v>3</v>
       </c>
       <c r="G52" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H52" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="I52" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J52" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="K52" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L52" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="M52" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="N52" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="O52" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="P52" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="Q52" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="R52" s="71" t="s">
         <v>14</v>
@@ -5720,7 +5721,7 @@
         <v>198</v>
       </c>
       <c r="D54" s="79" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E54" s="78"/>
       <c r="G54" s="78"/>
@@ -5730,40 +5731,40 @@
         <v>12</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="H55" s="8" t="s">
         <v>89</v>
       </c>
       <c r="I55" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="J55" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="K55" s="8" t="s">
         <v>344</v>
       </c>
-      <c r="J55" s="8" t="s">
+      <c r="L55" s="8" t="s">
         <v>345</v>
       </c>
-      <c r="K55" s="8" t="s">
+      <c r="M55" s="8" t="s">
         <v>346</v>
-      </c>
-      <c r="L55" s="8" t="s">
-        <v>347</v>
-      </c>
-      <c r="M55" s="8" t="s">
-        <v>348</v>
       </c>
       <c r="N55" s="8" t="s">
         <v>148</v>
       </c>
       <c r="O55" s="8" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="56" spans="3:18" x14ac:dyDescent="0.4">
@@ -5772,40 +5773,40 @@
         <v>(D56に関数入力)</v>
       </c>
       <c r="D56" s="76" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E56" s="77" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F56" s="71">
         <v>1</v>
       </c>
       <c r="G56" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H56" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="I56" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J56" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="K56" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L56" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="M56" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="N56" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="O56" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="57" spans="3:18" x14ac:dyDescent="0.4">
@@ -5813,31 +5814,31 @@
         <v>2</v>
       </c>
       <c r="G57" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H57" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="I57" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J57" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="K57" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L57" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="M57" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="N57" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="O57" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="58" spans="3:18" x14ac:dyDescent="0.4">
@@ -5845,31 +5846,31 @@
         <v>3</v>
       </c>
       <c r="G58" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H58" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="I58" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J58" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="K58" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L58" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="M58" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="N58" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="O58" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="60" spans="3:18" x14ac:dyDescent="0.4">
@@ -5877,7 +5878,7 @@
         <v>198</v>
       </c>
       <c r="D60" s="79" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E60" s="78"/>
     </row>
@@ -5886,25 +5887,25 @@
         <v>12</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="H61" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="I61" s="8" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="J61" s="8" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="K61" s="8" t="s">
         <v>160</v>
@@ -5913,10 +5914,10 @@
         <v>50</v>
       </c>
       <c r="M61" s="8" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="N61" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="62" spans="3:18" x14ac:dyDescent="0.4">
@@ -5925,37 +5926,37 @@
         <v>(D62に関数入力)</v>
       </c>
       <c r="D62" s="76" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E62" s="77" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F62" s="71">
         <v>1</v>
       </c>
       <c r="G62" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H62" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="I62" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J62" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="K62" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L62" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="M62" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="N62" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="63" spans="3:18" x14ac:dyDescent="0.4">
@@ -5963,28 +5964,28 @@
         <v>2</v>
       </c>
       <c r="G63" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H63" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="I63" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J63" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="K63" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L63" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="M63" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="N63" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="64" spans="3:18" x14ac:dyDescent="0.4">
@@ -5992,28 +5993,28 @@
         <v>3</v>
       </c>
       <c r="G64" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H64" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="I64" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J64" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="K64" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L64" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="M64" s="71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="N64" s="71" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -6067,7 +6068,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -6078,7 +6079,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="92" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D3" s="93"/>
       <c r="E3" s="93"/>
@@ -6092,21 +6093,21 @@
     <row r="6" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B6" s="6"/>
       <c r="C6" s="6" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F6" s="26"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B7" s="6"/>
       <c r="C7" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E7" s="24"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B8" s="6"/>
       <c r="C8" s="7" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E8" s="25"/>
     </row>
@@ -6127,7 +6128,7 @@
         <v>198</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.4">
@@ -6135,22 +6136,22 @@
         <v>12</v>
       </c>
       <c r="D13" s="8" t="s">
+        <v>391</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>393</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="F13" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="G13" s="8" t="s">
         <v>395</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>396</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>397</v>
-      </c>
       <c r="H13" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="I13" s="8" t="s">
         <v>323</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.4">
@@ -6159,22 +6160,22 @@
         <v>(D14に関数入力)</v>
       </c>
       <c r="D14" s="95" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G14" s="23" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H14" s="23" t="s">
         <v>14</v>
       </c>
       <c r="I14" s="23" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.4">
@@ -6204,98 +6205,98 @@
     <row r="20" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B20" s="96"/>
       <c r="C20" s="97" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C21" s="98" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D21" s="98" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C22" s="98" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D22" s="98" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C23" s="98" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D23" s="98" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C24" s="98" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D24" s="98" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C25" s="98" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D25" s="98" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C26" s="98" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D26" s="98" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C27" s="98" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D27" s="98" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C28" s="98" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D28" s="98" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C29" s="98" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D29" s="98" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C30" s="98" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D30" s="98" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C31" s="98" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D31" s="98" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.4">
@@ -6358,7 +6359,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -6369,7 +6370,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="92" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D3" s="93"/>
       <c r="E3" s="93"/>
@@ -6383,17 +6384,17 @@
     <row r="6" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B6" s="6"/>
       <c r="C6" s="6" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="F6" s="26"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B7" s="6"/>
       <c r="C7" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="E7" s="24"/>
     </row>
@@ -6410,159 +6411,159 @@
     <row r="10" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C10" s="100"/>
       <c r="D10" s="111" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="E10" s="111" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="G10" s="100"/>
       <c r="H10" s="111" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="I10" s="111" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C11" s="109" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D11" s="103" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E11" s="103" t="s">
+        <v>461</v>
+      </c>
+      <c r="G11" s="109" t="s">
+        <v>466</v>
+      </c>
+      <c r="H11" s="103" t="s">
         <v>463</v>
       </c>
-      <c r="G11" s="109" t="s">
-        <v>468</v>
-      </c>
-      <c r="H11" s="103" t="s">
+      <c r="I11" s="103" t="s">
         <v>465</v>
-      </c>
-      <c r="I11" s="103" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C12" s="106"/>
       <c r="D12" s="103" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="E12" s="103" t="s">
+        <v>455</v>
+      </c>
+      <c r="G12" s="106" t="s">
+        <v>459</v>
+      </c>
+      <c r="H12" s="103" t="s">
         <v>457</v>
       </c>
-      <c r="G12" s="106" t="s">
-        <v>461</v>
-      </c>
-      <c r="H12" s="103" t="s">
-        <v>459</v>
-      </c>
       <c r="I12" s="103" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C13" s="106"/>
       <c r="D13" s="103" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E13" s="103" t="s">
+        <v>448</v>
+      </c>
+      <c r="G13" s="104" t="s">
+        <v>452</v>
+      </c>
+      <c r="H13" s="103" t="s">
         <v>450</v>
       </c>
-      <c r="G13" s="104" t="s">
-        <v>454</v>
-      </c>
-      <c r="H13" s="103" t="s">
-        <v>452</v>
-      </c>
       <c r="I13" s="103" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C14" s="107"/>
       <c r="D14" s="103" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E14" s="102" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="17" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C17" s="100"/>
       <c r="D17" s="111" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="E17" s="111" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="G17" s="100"/>
       <c r="H17" s="111" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="I17" s="111" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C18" s="109" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D18" s="103" t="s">
+        <v>463</v>
+      </c>
+      <c r="E18" s="103" t="s">
         <v>465</v>
       </c>
-      <c r="E18" s="103" t="s">
-        <v>467</v>
-      </c>
       <c r="G18" s="109" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="H18" s="103" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I18" s="103" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C19" s="106"/>
       <c r="D19" s="103" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E19" s="103" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="G19" s="106"/>
       <c r="H19" s="103" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="I19" s="103" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="20" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C20" s="106"/>
       <c r="D20" s="103" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="E20" s="103" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="G20" s="104"/>
       <c r="H20" s="103" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="I20" s="103" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C21" s="106"/>
       <c r="D21" s="103" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E21" s="103" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="L21" s="100"/>
       <c r="M21" s="101"/>
@@ -6571,10 +6572,10 @@
     <row r="22" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C22" s="106"/>
       <c r="D22" s="103" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E22" s="102" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="L22" s="100"/>
       <c r="M22" s="101"/>
@@ -6583,10 +6584,10 @@
     <row r="23" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C23" s="106"/>
       <c r="D23" s="103" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E23" s="103" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="L23" s="100"/>
       <c r="M23" s="101"/>
@@ -6595,10 +6596,10 @@
     <row r="24" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C24" s="106"/>
       <c r="D24" s="103" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E24" s="103" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="L24" s="100"/>
       <c r="M24" s="101"/>
@@ -6607,10 +6608,10 @@
     <row r="25" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C25" s="104"/>
       <c r="D25" s="103" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="E25" s="103" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="L25" s="100"/>
       <c r="M25" s="101"/>
@@ -6629,10 +6630,10 @@
     <row r="28" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C28" s="100"/>
       <c r="D28" s="111" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="E28" s="111" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="L28" s="100"/>
       <c r="M28" s="101"/>
@@ -6640,13 +6641,13 @@
     </row>
     <row r="29" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C29" s="109" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D29" s="103" t="s">
+        <v>463</v>
+      </c>
+      <c r="E29" s="103" t="s">
         <v>465</v>
-      </c>
-      <c r="E29" s="103" t="s">
-        <v>467</v>
       </c>
       <c r="L29" s="100"/>
       <c r="M29" s="101"/>
@@ -6654,13 +6655,13 @@
     </row>
     <row r="30" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C30" s="108" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D30" s="103" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E30" s="103" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="L30" s="100"/>
       <c r="M30" s="101"/>
@@ -6668,13 +6669,13 @@
     </row>
     <row r="31" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C31" s="106" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D31" s="103" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="E31" s="103" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="L31" s="100"/>
       <c r="M31" s="101"/>
@@ -6683,10 +6684,10 @@
     <row r="32" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C32" s="106"/>
       <c r="D32" s="103" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="E32" s="103" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="L32" s="100"/>
       <c r="M32" s="101"/>
@@ -6695,10 +6696,10 @@
     <row r="33" spans="2:14" x14ac:dyDescent="0.4">
       <c r="C33" s="106"/>
       <c r="D33" s="103" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E33" s="103" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="L33" s="100"/>
       <c r="M33" s="101"/>
@@ -6707,10 +6708,10 @@
     <row r="34" spans="2:14" x14ac:dyDescent="0.4">
       <c r="C34" s="106"/>
       <c r="D34" s="103" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E34" s="102" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="L34" s="100"/>
       <c r="M34" s="101"/>
@@ -6719,10 +6720,10 @@
     <row r="35" spans="2:14" x14ac:dyDescent="0.4">
       <c r="C35" s="106"/>
       <c r="D35" s="103" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E35" s="103" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="L35" s="100"/>
       <c r="M35" s="101"/>
@@ -6731,10 +6732,10 @@
     <row r="36" spans="2:14" x14ac:dyDescent="0.4">
       <c r="C36" s="106"/>
       <c r="D36" s="103" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="E36" s="103" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="L36" s="100"/>
       <c r="M36" s="101"/>
@@ -6743,10 +6744,10 @@
     <row r="37" spans="2:14" x14ac:dyDescent="0.4">
       <c r="C37" s="105"/>
       <c r="D37" s="103" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E37" s="103" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="L37" s="100"/>
       <c r="M37" s="101"/>
@@ -6755,10 +6756,10 @@
     <row r="38" spans="2:14" x14ac:dyDescent="0.4">
       <c r="C38" s="104"/>
       <c r="D38" s="103" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E38" s="102" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="L38" s="100"/>
       <c r="M38" s="101"/>
@@ -6788,7 +6789,7 @@
         <v>10</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.4">
@@ -6796,28 +6797,28 @@
         <v>12</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="J45" s="8" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="K45" s="8" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.4">
@@ -6826,25 +6827,25 @@
         <v>(D46に関数入力)</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E46" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F46" s="23" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G46" s="23" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H46" s="23" t="s">
         <v>14</v>
       </c>
       <c r="I46" s="23" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="J46" s="23" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="K46" s="23" t="s">
         <v>14</v>
@@ -6852,25 +6853,25 @@
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.4">
       <c r="D47" s="7" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E47" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F47" s="23" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G47" s="23" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H47" s="23" t="s">
         <v>14</v>
       </c>
       <c r="I47" s="23" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="J47" s="23" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="K47" s="23" t="s">
         <v>14</v>
@@ -6878,25 +6879,25 @@
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.4">
       <c r="D48" s="7" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E48" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F48" s="23" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G48" s="23" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H48" s="23" t="s">
         <v>14</v>
       </c>
       <c r="I48" s="23" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="J48" s="23" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="K48" s="23" t="s">
         <v>14</v>
@@ -6945,17 +6946,17 @@
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B56" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B57" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B58" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
   </sheetData>
@@ -7001,7 +7002,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D2" s="4"/>
     </row>
@@ -7010,7 +7011,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="92" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D3" s="94"/>
     </row>
@@ -7022,14 +7023,14 @@
     <row r="6" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B6" s="6"/>
       <c r="C6" s="6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="F6" s="26"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B7" s="6"/>
       <c r="C7" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E7" s="24"/>
     </row>
@@ -7055,7 +7056,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.4">
@@ -7063,10 +7064,10 @@
         <v>12</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.4">
@@ -7075,7 +7076,7 @@
         <v>(D14に関数入力)</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>14</v>
@@ -7099,7 +7100,7 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D19" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.4">
@@ -7108,48 +7109,48 @@
     <row r="21" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C21" s="100"/>
       <c r="D21" s="111" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="E21" s="111" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C22" s="109" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="D22" s="103" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E22" s="103" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C23" s="106"/>
       <c r="D23" s="103" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="E23" s="103" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C24" s="106"/>
       <c r="D24" s="103" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E24" s="103" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C25" s="107"/>
       <c r="D25" s="103" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E25" s="102" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.4">
@@ -7210,7 +7211,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
@@ -7220,7 +7221,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="92" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D3" s="93"/>
       <c r="E3" s="94"/>
@@ -7233,7 +7234,7 @@
     <row r="6" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B6" s="6"/>
       <c r="C6" s="6" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F6" s="26"/>
     </row>
@@ -7255,7 +7256,7 @@
         <v>10</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.4">
@@ -7263,28 +7264,28 @@
         <v>12</v>
       </c>
       <c r="D11" s="91" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="E11" s="91" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="F11" s="91" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="G11" s="91" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="H11" s="91" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="I11" s="91" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="J11" s="91" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.4">
@@ -7293,13 +7294,13 @@
         <v>(D12に関数入力)</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>14</v>
@@ -7308,10 +7309,10 @@
         <v>14</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="K12" s="7" t="s">
         <v>14</v>
@@ -7407,7 +7408,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="114" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="D2" s="115"/>
       <c r="E2" s="115"/>
@@ -7418,7 +7419,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="114" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="D3" s="115"/>
       <c r="E3" s="115"/>
@@ -7431,17 +7432,17 @@
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.4">
       <c r="C6" s="119" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.4">
       <c r="C7" s="120" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.4">
       <c r="C8" s="121" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.4">
@@ -7456,7 +7457,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="122" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.4">
@@ -7464,7 +7465,7 @@
       <c r="E13" s="124"/>
       <c r="F13" s="125"/>
       <c r="G13" s="126" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="H13" s="125"/>
       <c r="I13" s="127"/>
@@ -7472,7 +7473,7 @@
       <c r="K13" s="125"/>
       <c r="L13" s="125"/>
       <c r="M13" s="126" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="N13" s="127"/>
       <c r="O13" s="123"/>
@@ -7486,34 +7487,34 @@
         <v>39</v>
       </c>
       <c r="E14" s="137" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="F14" s="137" t="s">
+        <v>516</v>
+      </c>
+      <c r="G14" s="137" t="s">
+        <v>518</v>
+      </c>
+      <c r="H14" s="137" t="s">
         <v>519</v>
       </c>
-      <c r="G14" s="137" t="s">
-        <v>521</v>
-      </c>
-      <c r="H14" s="137" t="s">
-        <v>522</v>
-      </c>
       <c r="I14" s="137" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="J14" s="137" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="K14" s="137" t="s">
+        <v>516</v>
+      </c>
+      <c r="L14" s="137" t="s">
+        <v>518</v>
+      </c>
+      <c r="M14" s="137" t="s">
         <v>519</v>
       </c>
-      <c r="L14" s="137" t="s">
-        <v>521</v>
-      </c>
-      <c r="M14" s="137" t="s">
-        <v>522</v>
-      </c>
       <c r="N14" s="137" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.4">
@@ -7522,7 +7523,7 @@
         <v>(D15に関数入力)</v>
       </c>
       <c r="D15" s="129" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="E15" s="129" t="s">
         <v>14</v>
@@ -7622,23 +7623,23 @@
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C23" s="130" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D23" s="131" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="E23" s="184" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="F23" s="185"/>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.4">
       <c r="C24" s="140"/>
       <c r="D24" s="133" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="E24" s="186" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="F24" s="186"/>
     </row>
@@ -7648,7 +7649,7 @@
         <v>0</v>
       </c>
       <c r="E25" s="187" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="F25" s="187"/>
     </row>
@@ -7658,7 +7659,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="188" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="F26" s="188"/>
     </row>
@@ -7668,48 +7669,48 @@
         <v>2</v>
       </c>
       <c r="E27" s="187" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="F27" s="187"/>
     </row>
     <row r="29" spans="3:14" x14ac:dyDescent="0.4">
       <c r="D29" s="138" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="E29" s="117" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="30" spans="3:14" x14ac:dyDescent="0.4">
       <c r="D30" s="139"/>
       <c r="E30" s="117" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="31" spans="3:14" x14ac:dyDescent="0.4">
       <c r="E31" s="117" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="32" spans="3:14" x14ac:dyDescent="0.4">
       <c r="E32" s="117" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="33" spans="4:5" x14ac:dyDescent="0.4">
       <c r="D33" s="139" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="E33" s="117" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
     <row r="34" spans="4:5" x14ac:dyDescent="0.4">
       <c r="D34" s="139" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="E34" s="117" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="40" spans="4:5" x14ac:dyDescent="0.4">
@@ -8020,12 +8021,12 @@
         <v>193</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B34" s="32" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C34" s="23">
         <v>1</v>
@@ -8036,7 +8037,7 @@
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B35" s="33" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C35" s="23">
         <v>3</v>
@@ -8065,24 +8066,24 @@
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B38" s="35" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C38" s="23">
         <v>2</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B39" s="33" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C39" s="23">
         <v>23</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.4">
@@ -8091,7 +8092,7 @@
         <v>24</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -8303,12 +8304,12 @@
         <v>193</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B23" s="32" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C23" s="23">
         <v>1</v>
@@ -8319,7 +8320,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B24" s="33" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C24" s="23">
         <v>3</v>
@@ -8348,24 +8349,24 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B27" s="35" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C27" s="23">
         <v>2</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B28" s="33" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C28" s="23">
         <v>23</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.4">
@@ -8374,7 +8375,7 @@
         <v>24</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.4">
@@ -8404,12 +8405,12 @@
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B39" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C39" s="15" t="s">
         <v>40</v>
@@ -8420,7 +8421,7 @@
     </row>
     <row r="40" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C40" s="112" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D40" s="113">
         <v>300</v>
@@ -8585,7 +8586,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A2:H32"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -8638,7 +8639,7 @@
     <row r="5" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B5" s="29"/>
       <c r="C5" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -8647,7 +8648,7 @@
     <row r="6" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B6" s="30"/>
       <c r="C6" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -8661,7 +8662,7 @@
     <row r="9" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B9" s="6"/>
       <c r="C9" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.4">
@@ -8710,7 +8711,7 @@
         <v>198</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.4">
@@ -8721,13 +8722,13 @@
         <v>183</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="H18" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.4">
@@ -8746,22 +8747,22 @@
         <v>7</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.4">
       <c r="H20" s="145" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.4">
       <c r="H21" s="145" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.4">
       <c r="H22" s="6" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.4">
@@ -8772,15 +8773,15 @@
         <v>193</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H23" s="146" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B24" s="32" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C24" s="23">
         <v>1</v>
@@ -8818,7 +8819,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B28" s="32" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C28" s="23">
         <v>1</v>
@@ -8838,24 +8839,24 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B30" s="35" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C30" s="23">
         <v>2</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B31" s="33" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C31" s="23">
         <v>23</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.4">
@@ -8864,7 +8865,7 @@
         <v>24</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -8881,16 +8882,14 @@
   </sheetPr>
   <dimension ref="A2:CL49"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="16.125" customWidth="1"/>
     <col min="3" max="3" width="15.875" customWidth="1"/>
     <col min="4" max="4" width="14.75" customWidth="1"/>
-    <col min="5" max="5" width="24.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.875" customWidth="1"/>
     <col min="6" max="6" width="10.375" customWidth="1"/>
     <col min="7" max="7" width="8.375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.625" bestFit="1" customWidth="1"/>
@@ -9010,13 +9009,13 @@
         <v>193</v>
       </c>
       <c r="E11" s="31" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B12" s="6"/>
       <c r="C12" s="32" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D12" s="23">
         <v>1</v>
@@ -9028,7 +9027,7 @@
     <row r="13" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B13" s="6"/>
       <c r="C13" s="33" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D13" s="23">
         <v>3</v>
@@ -9060,25 +9059,25 @@
     <row r="16" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B16" s="6"/>
       <c r="C16" s="35" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D16" s="23">
         <v>2</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="17" spans="1:90" x14ac:dyDescent="0.4">
       <c r="B17" s="6"/>
       <c r="C17" s="33" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D17" s="23">
         <v>23</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="18" spans="1:90" x14ac:dyDescent="0.4">
@@ -9088,7 +9087,7 @@
         <v>24</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="19" spans="1:90" x14ac:dyDescent="0.4">
@@ -10363,10 +10362,10 @@
     </row>
     <row r="34" spans="1:89" x14ac:dyDescent="0.4">
       <c r="D34" s="31" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="E34" s="31" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
@@ -10458,7 +10457,7 @@
         <v>0</v>
       </c>
       <c r="E35" s="32" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
@@ -10550,7 +10549,7 @@
         <v>1</v>
       </c>
       <c r="E36" s="32" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="37" spans="1:89" x14ac:dyDescent="0.4">
@@ -10558,7 +10557,7 @@
         <v>101</v>
       </c>
       <c r="E37" s="32" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="38" spans="1:89" x14ac:dyDescent="0.4">
@@ -10566,7 +10565,7 @@
         <v>103</v>
       </c>
       <c r="E38" s="32" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="39" spans="1:89" x14ac:dyDescent="0.4">
@@ -10574,7 +10573,7 @@
         <v>107</v>
       </c>
       <c r="E39" s="32" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="40" spans="1:89" x14ac:dyDescent="0.4">
@@ -10582,7 +10581,7 @@
         <v>121</v>
       </c>
       <c r="E40" s="32" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="41" spans="1:89" x14ac:dyDescent="0.4">
@@ -10590,7 +10589,7 @@
         <v>144</v>
       </c>
       <c r="E41" s="32" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="42" spans="1:89" x14ac:dyDescent="0.4">
@@ -10598,7 +10597,7 @@
         <v>145</v>
       </c>
       <c r="E42" s="32" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="43" spans="1:89" x14ac:dyDescent="0.4">
@@ -10606,7 +10605,7 @@
         <v>154</v>
       </c>
       <c r="E43" s="32" t="s">
-        <v>503</v>
+        <v>576</v>
       </c>
     </row>
     <row r="44" spans="1:89" x14ac:dyDescent="0.4">
@@ -10614,7 +10613,7 @@
         <v>155</v>
       </c>
       <c r="E44" s="32" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="45" spans="1:89" x14ac:dyDescent="0.4">
@@ -10622,7 +10621,7 @@
         <v>171</v>
       </c>
       <c r="E45" s="32" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="46" spans="1:89" x14ac:dyDescent="0.4">
@@ -10630,7 +10629,7 @@
         <v>901</v>
       </c>
       <c r="E46" s="32" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="47" spans="1:89" x14ac:dyDescent="0.4">
@@ -10638,7 +10637,7 @@
         <v>907</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="48" spans="1:89" x14ac:dyDescent="0.4">
@@ -10646,7 +10645,7 @@
         <v>903</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="49" spans="4:5" x14ac:dyDescent="0.4">
@@ -10654,7 +10653,7 @@
         <v>1001</v>
       </c>
       <c r="E49" s="23" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
   </sheetData>
@@ -10737,7 +10736,7 @@
         <v>166</v>
       </c>
       <c r="E7" s="88" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.4">
@@ -10760,18 +10759,18 @@
         <v>193</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G10" s="31" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H10" s="31" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.4">
       <c r="C11" s="32" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D11" s="23">
         <v>1</v>
@@ -10783,12 +10782,12 @@
         <v>1</v>
       </c>
       <c r="H11" s="23" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.4">
       <c r="C12" s="33" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D12" s="23">
         <v>3</v>
@@ -10800,7 +10799,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="23" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.4">
@@ -10812,7 +10811,7 @@
         <v>196</v>
       </c>
       <c r="H13" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.4">
@@ -10826,24 +10825,24 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.4">
       <c r="C15" s="35" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D15" s="23">
         <v>2</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.4">
       <c r="C16" s="33" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D16" s="23">
         <v>23</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.4">
@@ -10852,7 +10851,7 @@
         <v>24</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.4">
@@ -10869,7 +10868,7 @@
         <v>198</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.4">
@@ -11072,7 +11071,7 @@
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.4">
       <c r="B28" s="89" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -11094,7 +11093,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A2:AL319"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -11163,7 +11162,7 @@
     <row r="6" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B6" s="6"/>
       <c r="C6" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.4">
@@ -11172,25 +11171,25 @@
         <v>199</v>
       </c>
       <c r="D7" s="37" t="s">
+        <v>270</v>
+      </c>
+      <c r="E7" s="37" t="s">
+        <v>271</v>
+      </c>
+      <c r="F7" s="37" t="s">
         <v>272</v>
       </c>
-      <c r="E7" s="37" t="s">
+      <c r="G7" s="37" t="s">
         <v>273</v>
       </c>
-      <c r="F7" s="37" t="s">
+      <c r="H7" s="37" t="s">
         <v>274</v>
       </c>
-      <c r="G7" s="37" t="s">
+      <c r="I7" s="37" t="s">
         <v>275</v>
       </c>
-      <c r="H7" s="37" t="s">
+      <c r="J7" s="37" t="s">
         <v>276</v>
-      </c>
-      <c r="I7" s="37" t="s">
-        <v>277</v>
-      </c>
-      <c r="J7" s="37" t="s">
-        <v>278</v>
       </c>
       <c r="L7" t="s">
         <v>186</v>
@@ -11202,16 +11201,16 @@
         <v>0</v>
       </c>
       <c r="D8" s="39" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E8" s="48" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F8" s="39" t="b">
         <v>1</v>
       </c>
       <c r="G8" s="39" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H8" s="39">
         <v>2</v>
@@ -11236,31 +11235,31 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="L10" s="70" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B11" s="31" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C11" s="65" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D11" s="155" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E11" s="156"/>
       <c r="F11" s="155" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G11" s="156"/>
       <c r="L11" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B12" s="171" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C12" s="42">
         <v>0</v>
@@ -11270,11 +11269,11 @@
       </c>
       <c r="E12" s="168"/>
       <c r="F12" s="157" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G12" s="158"/>
       <c r="L12" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.4">
@@ -11287,11 +11286,11 @@
       </c>
       <c r="E13" s="168"/>
       <c r="F13" s="159" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G13" s="160"/>
       <c r="L13" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.4">
@@ -11312,7 +11311,7 @@
         <v>3</v>
       </c>
       <c r="D15" s="167" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E15" s="168"/>
       <c r="F15" s="159"/>
@@ -11324,7 +11323,7 @@
         <v>4</v>
       </c>
       <c r="D16" s="167" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E16" s="168"/>
       <c r="F16" s="161"/>
@@ -11332,17 +11331,17 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B17" s="58" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C17" s="60" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D17" s="54" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E17" s="55"/>
       <c r="F17" s="54" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G17" s="55"/>
     </row>
@@ -11352,23 +11351,23 @@
       <c r="D18" s="52"/>
       <c r="E18" s="53"/>
       <c r="F18" s="52" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="G18" s="53"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B19" s="58" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C19" s="57" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D19" s="54" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E19" s="55"/>
       <c r="F19" s="61" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G19" s="62"/>
     </row>
@@ -11378,23 +11377,23 @@
       <c r="D20" s="52"/>
       <c r="E20" s="53"/>
       <c r="F20" s="61" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G20" s="62"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B21" s="169" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C21" s="42" t="b">
         <v>1</v>
       </c>
       <c r="D21" s="167" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E21" s="168"/>
       <c r="F21" s="66" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G21" s="67"/>
     </row>
@@ -11404,11 +11403,11 @@
         <v>0</v>
       </c>
       <c r="D22" s="167" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E22" s="168"/>
       <c r="F22" s="68" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G22" s="69"/>
     </row>
@@ -11424,23 +11423,23 @@
       </c>
       <c r="E23" s="51"/>
       <c r="F23" s="63" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G23" s="64"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B24" s="169" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C24" s="41">
         <v>1</v>
       </c>
       <c r="D24" s="165" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E24" s="166"/>
       <c r="F24" s="163" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G24" s="164"/>
     </row>
@@ -11450,11 +11449,11 @@
         <v>2</v>
       </c>
       <c r="D25" s="153" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E25" s="154"/>
       <c r="F25" s="147" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G25" s="148"/>
     </row>
@@ -11464,7 +11463,7 @@
         <v>3</v>
       </c>
       <c r="D26" s="153" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E26" s="154"/>
       <c r="F26" s="147"/>
@@ -11476,7 +11475,7 @@
         <v>4</v>
       </c>
       <c r="D27" s="153" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E27" s="154"/>
       <c r="F27" s="147"/>
@@ -11488,7 +11487,7 @@
         <v>5</v>
       </c>
       <c r="D28" s="153" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E28" s="154"/>
       <c r="F28" s="151"/>
@@ -11496,17 +11495,17 @@
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B29" s="169" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C29" s="41">
         <v>1</v>
       </c>
       <c r="D29" s="165" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E29" s="166"/>
       <c r="F29" s="163" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G29" s="164"/>
     </row>
@@ -11516,27 +11515,27 @@
         <v>2</v>
       </c>
       <c r="D30" s="153" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E30" s="154"/>
       <c r="F30" s="147" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G30" s="148"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B31" s="170" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C31" s="41">
         <v>2</v>
       </c>
       <c r="D31" s="153" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E31" s="154"/>
       <c r="F31" s="149" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G31" s="150"/>
     </row>
@@ -11546,11 +11545,11 @@
         <v>3</v>
       </c>
       <c r="D32" s="153" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E32" s="154"/>
       <c r="F32" s="151" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G32" s="152"/>
     </row>
@@ -11576,7 +11575,7 @@
         <v>198</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="X38" s="12" t="s">
         <v>110</v>
@@ -11657,7 +11656,7 @@
         <v>129</v>
       </c>
       <c r="W39" s="8" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="X39" s="8" t="s">
         <v>130</v>
@@ -11766,7 +11765,7 @@
         <v>85</v>
       </c>
       <c r="W40" s="7" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="X40" s="7" t="s">
         <v>85</v>
@@ -12066,7 +12065,7 @@
         <v>85</v>
       </c>
       <c r="W44" s="7" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="X44" s="7" t="s">
         <v>85</v>
@@ -22540,7 +22539,7 @@
     <row r="6" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B6" s="6"/>
       <c r="C6" s="6" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.4">
@@ -22552,10 +22551,10 @@
         <v>39</v>
       </c>
       <c r="E7" s="90" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F7" s="90" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.4">
@@ -22564,7 +22563,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E8" s="23">
         <v>1</v>
@@ -22578,19 +22577,19 @@
         <v>200</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F10" s="31" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="G10" s="31" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="I10" s="31" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="J10" s="31" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.4">
@@ -22604,13 +22603,13 @@
         <v>1</v>
       </c>
       <c r="G11" s="23" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="I11" s="23" t="b">
         <v>1</v>
       </c>
       <c r="J11" s="23" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.4">
@@ -22624,13 +22623,13 @@
         <v>2</v>
       </c>
       <c r="G12" s="23" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="I12" s="23" t="b">
         <v>0</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.4">
@@ -22641,7 +22640,7 @@
         <v>201</v>
       </c>
       <c r="J13" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.4">
@@ -22649,7 +22648,7 @@
         <v>3</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.4">
@@ -22657,7 +22656,7 @@
         <v>4</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.4">
@@ -22674,7 +22673,7 @@
         <v>10</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.4">
@@ -22989,7 +22988,7 @@
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.4">
       <c r="B28" s="89" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -23016,14 +23015,12 @@
   </sheetPr>
   <dimension ref="A2:F28"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="17.625" customWidth="1"/>
-    <col min="3" max="3" width="22.75" customWidth="1"/>
+    <col min="3" max="3" width="26.625" customWidth="1"/>
     <col min="4" max="4" width="28.875" customWidth="1"/>
     <col min="5" max="5" width="23.75" customWidth="1"/>
     <col min="6" max="6" width="33.25" customWidth="1"/>
@@ -23136,7 +23133,7 @@
         <v>227</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.4">
@@ -23173,58 +23170,58 @@
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B22" s="23" t="s">
-        <v>236</v>
+        <v>575</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>237</v>
+        <v>576</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B23" s="23" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B24" s="23" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B25" s="23" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B26" s="23" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B27" s="23" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B28" s="23" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
   </sheetData>
@@ -23256,7 +23253,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D2" s="4"/>
     </row>
@@ -23265,7 +23262,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D3" s="4"/>
     </row>
@@ -23277,7 +23274,7 @@
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B6" s="6"/>
       <c r="C6" s="6" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="H6" t="s">
         <v>186</v>
@@ -23286,16 +23283,16 @@
     <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B7" s="6"/>
       <c r="C7" s="8" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>223</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="H7" t="s">
         <v>188</v>
@@ -23304,7 +23301,7 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B8" s="6"/>
       <c r="C8" s="7" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>225</v>
@@ -23313,7 +23310,7 @@
         <v>190</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H8" t="s">
         <v>187</v>
@@ -23333,7 +23330,7 @@
         <v>198</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.4">
@@ -23357,7 +23354,7 @@
         <v>145123218</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
@@ -23367,50 +23364,50 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B17" s="31" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B18" s="23" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B19" s="23" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B21" s="31" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B22" s="23" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B23" s="23" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -23444,7 +23441,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="D2" s="4"/>
     </row>
@@ -23453,7 +23450,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="D3" s="4"/>
     </row>
@@ -23465,7 +23462,7 @@
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="B6" s="6"/>
       <c r="C6" s="6" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="H6" t="s">
         <v>186</v>
@@ -23477,13 +23474,13 @@
         <v>223</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="H7" t="s">
         <v>188</v>
@@ -23501,7 +23498,7 @@
         <v>190</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H8" t="s">
         <v>187</v>
@@ -23521,7 +23518,7 @@
         <v>198</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.4">
@@ -23542,10 +23539,10 @@
         <v>(D14に関数入力)</v>
       </c>
       <c r="D14" s="36" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
@@ -23555,26 +23552,26 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B17" s="31" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B18" s="23" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B19" s="23" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
uploaded preview for SOR-ph2
</commit_message>
<xml_diff>
--- a/sample/ExcelMacro/kabuSTATION_API_function_sample.xlsx
+++ b/sample/ExcelMacro/kabuSTATION_API_function_sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\14.不正アクセス防止対応API\kabusapi\sample\ExcelMacro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\15.MSSOR_Ph2\kabusapi\sample\ExcelMacro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66B771F-9AC5-489F-91CD-709D957F1E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816D03C6-A3BF-4FB5-A4EF-E1853DFF697C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="787" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="787" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="注文取消" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1664" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1668" uniqueCount="578">
   <si>
     <t>概要</t>
     <rPh sb="0" eb="2">
@@ -3198,6 +3198,17 @@
   </si>
   <si>
     <t>=CANCELORDER(C8)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>SOR</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>東証+</t>
+    <rPh sb="0" eb="2">
+      <t>トウショウ</t>
+    </rPh>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -3982,31 +3993,22 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4015,29 +4017,11 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4051,11 +4035,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4391,7 +4402,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B2:I19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
@@ -4554,7 +4567,7 @@
   <dimension ref="B2:T64"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75"/>
@@ -6962,7 +6975,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="B2:F29"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
@@ -7722,7 +7737,9 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A2:H40"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
@@ -8571,9 +8588,9 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A2:H32"/>
+  <dimension ref="A2:H36"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
@@ -8805,53 +8822,89 @@
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="B28" s="32" t="s">
-        <v>266</v>
-      </c>
+      <c r="B28" s="33"/>
       <c r="C28" s="23">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>192</v>
+        <v>576</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="B29" s="33"/>
       <c r="C29" s="23">
+        <v>27</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="B30" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="C30" s="23">
+        <v>1</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="B31" s="33"/>
+      <c r="C31" s="23">
         <v>3</v>
       </c>
-      <c r="D29" s="23" t="s">
+      <c r="D31" s="23" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
-      <c r="B30" s="35" t="s">
+    <row r="32" spans="1:8">
+      <c r="B32" s="33"/>
+      <c r="C32" s="23">
+        <v>9</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" s="33"/>
+      <c r="C33" s="23">
+        <v>27</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4">
+      <c r="B34" s="35" t="s">
         <v>262</v>
       </c>
-      <c r="C30" s="23">
+      <c r="C34" s="23">
         <v>2</v>
       </c>
-      <c r="D30" s="23" t="s">
+      <c r="D34" s="23" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
-      <c r="B31" s="33" t="s">
+    <row r="35" spans="2:4">
+      <c r="B35" s="33" t="s">
         <v>263</v>
       </c>
-      <c r="C31" s="23">
+      <c r="C35" s="23">
         <v>23</v>
       </c>
-      <c r="D31" s="23" t="s">
+      <c r="D35" s="23" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
-      <c r="B32" s="34"/>
-      <c r="C32" s="23">
+    <row r="36" spans="2:4">
+      <c r="B36" s="34"/>
+      <c r="C36" s="23">
         <v>24</v>
       </c>
-      <c r="D32" s="23" t="s">
+      <c r="D36" s="23" t="s">
         <v>259</v>
       </c>
     </row>
@@ -8869,7 +8922,9 @@
   </sheetPr>
   <dimension ref="A2:CL49"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
@@ -10654,7 +10709,7 @@
   <dimension ref="A2:AA28"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -11080,8 +11135,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A2:AL319"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -11232,89 +11287,89 @@
       <c r="C11" s="65" t="s">
         <v>301</v>
       </c>
-      <c r="D11" s="150" t="s">
+      <c r="D11" s="155" t="s">
         <v>295</v>
       </c>
-      <c r="E11" s="151"/>
-      <c r="F11" s="150" t="s">
+      <c r="E11" s="156"/>
+      <c r="F11" s="155" t="s">
         <v>296</v>
       </c>
-      <c r="G11" s="151"/>
+      <c r="G11" s="156"/>
       <c r="L11" t="s">
         <v>504</v>
       </c>
     </row>
     <row r="12" spans="2:12">
-      <c r="B12" s="149" t="s">
+      <c r="B12" s="171" t="s">
         <v>275</v>
       </c>
       <c r="C12" s="42">
         <v>0</v>
       </c>
-      <c r="D12" s="152" t="s">
+      <c r="D12" s="167" t="s">
         <v>201</v>
       </c>
-      <c r="E12" s="153"/>
-      <c r="F12" s="166" t="s">
+      <c r="E12" s="168"/>
+      <c r="F12" s="157" t="s">
         <v>297</v>
       </c>
-      <c r="G12" s="167"/>
+      <c r="G12" s="158"/>
       <c r="L12" t="s">
         <v>505</v>
       </c>
     </row>
     <row r="13" spans="2:12">
-      <c r="B13" s="149"/>
+      <c r="B13" s="171"/>
       <c r="C13" s="42">
         <v>1</v>
       </c>
-      <c r="D13" s="152" t="s">
+      <c r="D13" s="167" t="s">
         <v>200</v>
       </c>
-      <c r="E13" s="153"/>
-      <c r="F13" s="168" t="s">
+      <c r="E13" s="168"/>
+      <c r="F13" s="159" t="s">
         <v>304</v>
       </c>
-      <c r="G13" s="169"/>
+      <c r="G13" s="160"/>
       <c r="L13" t="s">
         <v>506</v>
       </c>
     </row>
     <row r="14" spans="2:12">
-      <c r="B14" s="149"/>
+      <c r="B14" s="171"/>
       <c r="C14" s="42">
         <v>2</v>
       </c>
-      <c r="D14" s="152" t="s">
+      <c r="D14" s="167" t="s">
         <v>199</v>
       </c>
-      <c r="E14" s="153"/>
-      <c r="F14" s="168"/>
-      <c r="G14" s="169"/>
+      <c r="E14" s="168"/>
+      <c r="F14" s="159"/>
+      <c r="G14" s="160"/>
     </row>
     <row r="15" spans="2:12">
-      <c r="B15" s="149"/>
+      <c r="B15" s="171"/>
       <c r="C15" s="42">
         <v>3</v>
       </c>
-      <c r="D15" s="152" t="s">
+      <c r="D15" s="167" t="s">
         <v>262</v>
       </c>
-      <c r="E15" s="153"/>
-      <c r="F15" s="168"/>
-      <c r="G15" s="169"/>
+      <c r="E15" s="168"/>
+      <c r="F15" s="159"/>
+      <c r="G15" s="160"/>
     </row>
     <row r="16" spans="2:12">
-      <c r="B16" s="149"/>
+      <c r="B16" s="171"/>
       <c r="C16" s="42">
         <v>4</v>
       </c>
-      <c r="D16" s="152" t="s">
+      <c r="D16" s="167" t="s">
         <v>263</v>
       </c>
-      <c r="E16" s="153"/>
-      <c r="F16" s="162"/>
-      <c r="G16" s="163"/>
+      <c r="E16" s="168"/>
+      <c r="F16" s="161"/>
+      <c r="G16" s="162"/>
     </row>
     <row r="17" spans="2:7">
       <c r="B17" s="58" t="s">
@@ -11369,30 +11424,30 @@
       <c r="G20" s="62"/>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="147" t="s">
+      <c r="B21" s="169" t="s">
         <v>284</v>
       </c>
       <c r="C21" s="42" t="b">
         <v>1</v>
       </c>
-      <c r="D21" s="152" t="s">
+      <c r="D21" s="167" t="s">
         <v>302</v>
       </c>
-      <c r="E21" s="153"/>
+      <c r="E21" s="168"/>
       <c r="F21" s="66" t="s">
         <v>297</v>
       </c>
       <c r="G21" s="67"/>
     </row>
     <row r="22" spans="2:7">
-      <c r="B22" s="147"/>
+      <c r="B22" s="169"/>
       <c r="C22" s="42" t="b">
         <v>0</v>
       </c>
-      <c r="D22" s="152" t="s">
+      <c r="D22" s="167" t="s">
         <v>303</v>
       </c>
-      <c r="E22" s="153"/>
+      <c r="E22" s="168"/>
       <c r="F22" s="68" t="s">
         <v>305</v>
       </c>
@@ -11415,130 +11470,130 @@
       <c r="G23" s="64"/>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="147" t="s">
+      <c r="B24" s="169" t="s">
         <v>287</v>
       </c>
       <c r="C24" s="41">
         <v>1</v>
       </c>
-      <c r="D24" s="154" t="s">
+      <c r="D24" s="165" t="s">
         <v>285</v>
       </c>
-      <c r="E24" s="155"/>
-      <c r="F24" s="160" t="s">
+      <c r="E24" s="166"/>
+      <c r="F24" s="163" t="s">
         <v>297</v>
       </c>
-      <c r="G24" s="161"/>
+      <c r="G24" s="164"/>
     </row>
     <row r="25" spans="2:7">
-      <c r="B25" s="147"/>
+      <c r="B25" s="169"/>
       <c r="C25" s="41">
         <v>2</v>
       </c>
-      <c r="D25" s="156" t="s">
+      <c r="D25" s="153" t="s">
         <v>276</v>
       </c>
-      <c r="E25" s="157"/>
-      <c r="F25" s="164" t="s">
+      <c r="E25" s="154"/>
+      <c r="F25" s="147" t="s">
         <v>304</v>
       </c>
-      <c r="G25" s="165"/>
+      <c r="G25" s="148"/>
     </row>
     <row r="26" spans="2:7">
-      <c r="B26" s="147"/>
+      <c r="B26" s="169"/>
       <c r="C26" s="41">
         <v>3</v>
       </c>
-      <c r="D26" s="156" t="s">
+      <c r="D26" s="153" t="s">
         <v>277</v>
       </c>
-      <c r="E26" s="157"/>
-      <c r="F26" s="164"/>
-      <c r="G26" s="165"/>
+      <c r="E26" s="154"/>
+      <c r="F26" s="147"/>
+      <c r="G26" s="148"/>
     </row>
     <row r="27" spans="2:7">
-      <c r="B27" s="147"/>
+      <c r="B27" s="169"/>
       <c r="C27" s="41">
         <v>4</v>
       </c>
-      <c r="D27" s="156" t="s">
+      <c r="D27" s="153" t="s">
         <v>278</v>
       </c>
-      <c r="E27" s="157"/>
-      <c r="F27" s="164"/>
-      <c r="G27" s="165"/>
+      <c r="E27" s="154"/>
+      <c r="F27" s="147"/>
+      <c r="G27" s="148"/>
     </row>
     <row r="28" spans="2:7">
-      <c r="B28" s="147"/>
+      <c r="B28" s="169"/>
       <c r="C28" s="41">
         <v>5</v>
       </c>
-      <c r="D28" s="156" t="s">
+      <c r="D28" s="153" t="s">
         <v>279</v>
       </c>
-      <c r="E28" s="157"/>
-      <c r="F28" s="158"/>
-      <c r="G28" s="159"/>
+      <c r="E28" s="154"/>
+      <c r="F28" s="151"/>
+      <c r="G28" s="152"/>
     </row>
     <row r="29" spans="2:7">
-      <c r="B29" s="147" t="s">
+      <c r="B29" s="169" t="s">
         <v>288</v>
       </c>
       <c r="C29" s="41">
         <v>1</v>
       </c>
-      <c r="D29" s="154" t="s">
+      <c r="D29" s="165" t="s">
         <v>286</v>
       </c>
-      <c r="E29" s="155"/>
-      <c r="F29" s="160" t="s">
+      <c r="E29" s="166"/>
+      <c r="F29" s="163" t="s">
         <v>297</v>
       </c>
-      <c r="G29" s="161"/>
+      <c r="G29" s="164"/>
     </row>
     <row r="30" spans="2:7">
-      <c r="B30" s="147"/>
+      <c r="B30" s="169"/>
       <c r="C30" s="41">
         <v>2</v>
       </c>
-      <c r="D30" s="156" t="s">
+      <c r="D30" s="153" t="s">
         <v>280</v>
       </c>
-      <c r="E30" s="157"/>
-      <c r="F30" s="164" t="s">
+      <c r="E30" s="154"/>
+      <c r="F30" s="147" t="s">
         <v>304</v>
       </c>
-      <c r="G30" s="165"/>
+      <c r="G30" s="148"/>
     </row>
     <row r="31" spans="2:7">
-      <c r="B31" s="148" t="s">
+      <c r="B31" s="170" t="s">
         <v>289</v>
       </c>
       <c r="C31" s="41">
         <v>2</v>
       </c>
-      <c r="D31" s="156" t="s">
+      <c r="D31" s="153" t="s">
         <v>281</v>
       </c>
-      <c r="E31" s="157"/>
-      <c r="F31" s="170" t="s">
+      <c r="E31" s="154"/>
+      <c r="F31" s="149" t="s">
         <v>297</v>
       </c>
-      <c r="G31" s="171"/>
+      <c r="G31" s="150"/>
     </row>
     <row r="32" spans="2:7">
-      <c r="B32" s="148"/>
+      <c r="B32" s="170"/>
       <c r="C32" s="41">
         <v>3</v>
       </c>
-      <c r="D32" s="156" t="s">
+      <c r="D32" s="153" t="s">
         <v>282</v>
       </c>
-      <c r="E32" s="157"/>
-      <c r="F32" s="158" t="s">
+      <c r="E32" s="154"/>
+      <c r="F32" s="151" t="s">
         <v>304</v>
       </c>
-      <c r="G32" s="159"/>
+      <c r="G32" s="152"/>
     </row>
     <row r="33" spans="1:37">
       <c r="B33" s="6"/>
@@ -22401,43 +22456,43 @@
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
     <mergeCell ref="F30:G30"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="F32:G32"/>
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B24:B28"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="B21:B22"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <dataValidations count="5">
@@ -22466,9 +22521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A2:Y28"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
@@ -23003,7 +23056,7 @@
   <dimension ref="A2:F28"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>

</xml_diff>